<commit_message>
[Update] Affichage de la precision terminée - A optimiser un poil Next step : Score
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -210,12 +210,6 @@
     <t>Background scene</t>
   </si>
   <si>
-    <t>affichage GUI + Différencier les touchs</t>
-  </si>
-  <si>
-    <t>Necropole X selectionnée + police supplémentaire ? Text ? Title ?</t>
-  </si>
-  <si>
     <t>Bump arrow model (flash)</t>
   </si>
   <si>
@@ -238,13 +232,19 @@
   </si>
   <si>
     <t>Alpha Test gameplay</t>
+  </si>
+  <si>
+    <t>Fini</t>
+  </si>
+  <si>
+    <t>Necropole X selectionnée + police supplémentaire ? Text ? Title ? Score ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +265,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +330,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -322,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -336,6 +369,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,78 +713,71 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
+      <c r="A2" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
@@ -753,190 +785,190 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+      <c r="E29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+      <c r="E30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="5" t="s">
+      <c r="E31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>31</v>
-      </c>
-      <c r="E30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>34</v>
       </c>
       <c r="E33" s="6">
         <v>0</v>
@@ -944,7 +976,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E34" s="6">
         <v>0</v>
@@ -952,7 +984,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E35" s="6">
         <v>0</v>
@@ -960,146 +992,146 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
+      <c r="E41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="E42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="E44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="10" t="s">
+      <c r="E46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+      <c r="E47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E48" s="7">
         <v>0.5</v>
       </c>
-      <c r="F45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-      <c r="C47" t="s">
+      <c r="E49" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+      <c r="C50" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="10"/>
-      <c r="C48" t="s">
+      <c r="E50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="C51" t="s">
         <v>62</v>
       </c>
-      <c r="E48" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="E51" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="E50" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E51" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" s="6">
-        <v>0</v>
-      </c>
+      <c r="B52" s="9"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E53" s="6">
         <v>0</v>
@@ -1107,52 +1139,63 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
         <v>58</v>
       </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>73</v>
-      </c>
-      <c r="E60" s="6">
+      <c r="E61" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>70</v>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,11 +1206,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" s="6">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update/Add] WIP score + life - Création DataManager.cs EnumManager.cs - Affichage de score en texture (Graphics.dt) - Optimisation, clean code - Update planning
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>prio</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Progression</t>
   </si>
   <si>
-    <t>En cours de réa</t>
-  </si>
-  <si>
     <t>Reste :</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
     <t>A faire rapidement</t>
   </si>
   <si>
-    <t>GUI ? 3D ? + life gestion</t>
-  </si>
-  <si>
-    <t>GUI ? 3DText ? + scoring</t>
-  </si>
-  <si>
     <t>Rush/Cross detection</t>
   </si>
   <si>
@@ -237,7 +228,19 @@
     <t>Fini</t>
   </si>
   <si>
-    <t>Necropole X selectionnée + police supplémentaire ? Text ? Title ? Score ?</t>
+    <t>Textures</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Necropole X selectionnée + Zekton ?</t>
+  </si>
+  <si>
+    <t>work in progress !</t>
+  </si>
+  <si>
+    <t>Display "slow/fast"</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -375,6 +378,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,12 +713,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -737,7 +741,7 @@
         <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -754,122 +758,123 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
+      <c r="E10" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="E17" s="6">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>63</v>
+      <c r="B18" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="E18" s="6">
         <v>0</v>
       </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="6">
-        <v>0</v>
-      </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="6">
         <v>0</v>
@@ -877,23 +882,23 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>19</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>20</v>
       </c>
       <c r="E24" s="6">
         <v>0</v>
@@ -901,7 +906,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="6">
         <v>0</v>
@@ -909,18 +914,15 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
         <v>23</v>
-      </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" t="s">
-        <v>25</v>
       </c>
       <c r="E27" s="6">
         <v>0</v>
@@ -928,15 +930,18 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>26</v>
-      </c>
-      <c r="E28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>27</v>
       </c>
       <c r="E29" s="6">
         <v>0</v>
@@ -944,7 +949,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="6">
         <v>0</v>
@@ -952,278 +957,286 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+      <c r="E35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+      <c r="E41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="3" t="s">
+      <c r="E42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="E44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="E45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="10" t="s">
+      <c r="E47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="7">
+      <c r="E48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" s="7">
         <v>0.5</v>
       </c>
-      <c r="F48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
-      <c r="C50" t="s">
-        <v>61</v>
+      <c r="F49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="E50" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="10"/>
       <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="10"/>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="E51" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>53</v>
-      </c>
-      <c r="E56" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E57" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>67</v>
-      </c>
-      <c r="E61" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>66</v>
-      </c>
-      <c r="E62" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>71</v>
-      </c>
-      <c r="E63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="E66" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>67</v>
+      </c>
+      <c r="E68" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] [Buggé] Score affiché + Jumps gérés Jumps à finir : Pas de suppression dans la arrowList si miss => gros bug
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -228,9 +228,6 @@
     <t>Fini</t>
   </si>
   <si>
-    <t>Textures</t>
-  </si>
-  <si>
     <t>3D</t>
   </si>
   <si>
@@ -241,13 +238,16 @@
   </si>
   <si>
     <t>Display "slow/fast"</t>
+  </si>
+  <si>
+    <t>Caler selon la résolution - Prendre en compte le quad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +285,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -358,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -379,6 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +721,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,21 +768,21 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="F9" t="s">
         <v>74</v>
-      </c>
-      <c r="E8" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,7 +793,7 @@
         <v>0.3</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1106,7 +1114,7 @@
         <v>0.5</v>
       </c>
       <c r="F49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] LifeBar fait ! Next step : Offset et audio
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -228,9 +228,6 @@
     <t>Fini</t>
   </si>
   <si>
-    <t>3D</t>
-  </si>
-  <si>
     <t>Necropole X selectionnée + Zekton ?</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Caler selon la résolution - Prendre en compte le quad</t>
+  </si>
+  <si>
+    <t>Fini - Caler selon la résolution</t>
   </si>
 </sst>
 </file>
@@ -297,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +352,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -365,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -387,6 +393,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,7 +775,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="19">
         <v>0</v>
@@ -779,21 +786,21 @@
         <v>6</v>
       </c>
       <c r="E9" s="20">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="20">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -837,7 +844,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="21" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="6">
@@ -1114,7 +1121,7 @@
         <v>0.5</v>
       </c>
       <c r="F49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Audio ok Next step : Synchronisation ! (Offset + pos 3D + globalOffset ??)
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>prio</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Fini - Caler selon la résolution</t>
+  </si>
+  <si>
+    <t>Audio ok; Synchroniser la chart avec la musique</t>
   </si>
 </sst>
 </file>
@@ -698,7 +701,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,11 +831,14 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="6">
-        <v>0</v>
+      <c r="E14" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,14 +850,11 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
+      <c r="E16" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Audio et chart synchronized ! Next step : Bump model + combo !
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>prio</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>Fini - Caler selon la résolution</t>
-  </si>
-  <si>
-    <t>Audio ok; Synchroniser la chart avec la musique</t>
   </si>
 </sst>
 </file>
@@ -374,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -386,7 +383,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -396,7 +392,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,7 +697,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,26 +731,26 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
       <c r="E5" t="s">
         <v>46</v>
       </c>
@@ -768,27 +764,27 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <v>1</v>
       </c>
       <c r="F9" t="s">
@@ -796,10 +792,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <v>1</v>
       </c>
       <c r="F10" t="s">
@@ -831,14 +827,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="F14" t="s">
-        <v>75</v>
+      <c r="E14" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,10 +843,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>1</v>
       </c>
     </row>
@@ -866,7 +859,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="20" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="6">
@@ -1117,7 +1110,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E49" s="7">

</xml_diff>

<commit_message>
[Update] Bump arrow ok !
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -180,9 +180,6 @@
     <t>LoadChartManager</t>
   </si>
   <si>
-    <t>A faire rapidement</t>
-  </si>
-  <si>
     <t>Rush/Cross detection</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Fini - Caler selon la résolution</t>
+  </si>
+  <si>
+    <t>Façon plus opti ?</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,12 +727,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="18">
         <v>0</v>
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="20" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="6">
@@ -859,19 +859,19 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
+      <c r="B18" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
@@ -1111,18 +1111,18 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" s="7">
         <v>0.5</v>
       </c>
       <c r="F49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E50" s="6">
         <v>0</v>
@@ -1131,7 +1131,7 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="10"/>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" s="6">
         <v>0</v>
@@ -1140,7 +1140,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="10"/>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E52" s="6">
         <v>0</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E59" s="6">
         <v>0</v>
@@ -1203,12 +1203,12 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E62" s="6">
         <v>0</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E63" s="6">
         <v>0</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E64" s="6">
         <v>0</v>
@@ -1232,12 +1232,12 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="6">
         <v>0</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E68" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
[Update] Progress Bar en cours
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>prio</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Façon plus opti ?</t>
+  </si>
+  <si>
+    <t>Afficher la barre suivant la première et dernière flèche</t>
   </si>
 </sst>
 </file>
@@ -697,7 +700,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,8 +841,11 @@
       <c r="B15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="6">
-        <v>0</v>
+      <c r="E15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] progress bar + code combo done Next step : GUI combo !
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>prio</t>
   </si>
@@ -243,7 +243,10 @@
     <t>Façon plus opti ?</t>
   </si>
   <si>
-    <t>Afficher la barre suivant la première et dernière flèche</t>
+    <t>Rajouter une petite particule ?</t>
+  </si>
+  <si>
+    <t>Code fait + Afficher le GUI</t>
   </si>
 </sst>
 </file>
@@ -699,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,11 +817,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="6">
-        <v>0</v>
+      <c r="E12" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -838,11 +844,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="7">
-        <v>0.3</v>
+      <c r="E15" s="19">
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
[Update] [Bug version] Combo codé pas compilé ni débuggé
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -246,10 +246,10 @@
     <t>Rajouter une petite particule ?</t>
   </si>
   <si>
-    <t>Code fait + Afficher le GUI</t>
-  </si>
-  <si>
-    <t>Améliorable !</t>
+    <t>Améliorable ! Déplacement moins rapides</t>
+  </si>
+  <si>
+    <t>Debbugger, optimiser</t>
   </si>
 </sst>
 </file>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,10 +824,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="7">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Combo finis Next step : Display slow/fast ou les mines
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>prio</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>Améliorable ! Déplacement moins rapides</t>
-  </si>
-  <si>
-    <t>Debbugger, optimiser</t>
   </si>
 </sst>
 </file>
@@ -306,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,12 +358,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -380,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -401,7 +392,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,14 +810,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>77</v>
+      <c r="E12" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Mine ok Next step : Display slow/fast et Optimisation !
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>prio</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>Améliorable ! Déplacement moins rapides</t>
+  </si>
+  <si>
+    <t>Optimisation</t>
+  </si>
+  <si>
+    <t>En cours</t>
+  </si>
+  <si>
+    <t>Objectif 200 FPS+ en debug</t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +367,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -371,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -392,6 +413,8 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +781,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -802,11 +825,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6">
-        <v>0</v>
+      <c r="E11" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -883,22 +906,25 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="6">
         <v>0</v>
@@ -906,23 +932,23 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>19</v>
-      </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>20</v>
       </c>
       <c r="E25" s="6">
         <v>0</v>
@@ -930,7 +956,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="6">
         <v>0</v>
@@ -938,18 +964,15 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>23</v>
-      </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" t="s">
-        <v>25</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
@@ -957,15 +980,18 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>26</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>27</v>
       </c>
       <c r="E30" s="6">
         <v>0</v>
@@ -973,7 +999,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31" s="6">
         <v>0</v>
@@ -981,31 +1007,31 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>31</v>
-      </c>
-      <c r="E34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>32</v>
       </c>
       <c r="E35" s="6">
         <v>0</v>
@@ -1013,7 +1039,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" s="6">
         <v>0</v>
@@ -1021,7 +1047,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" s="6">
         <v>0</v>
@@ -1029,7 +1055,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" s="6">
         <v>0</v>
@@ -1037,7 +1063,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E39" s="6">
         <v>0</v>
@@ -1045,15 +1071,15 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
         <v>37</v>
-      </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="E41" s="6">
         <v>0</v>
@@ -1061,82 +1087,81 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="3" t="s">
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="E44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+      <c r="E45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="E46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="s">
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E47" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="10" t="s">
+      <c r="E48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
+      <c r="E49" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E50" s="7">
         <v>0.5</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="E50" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="10"/>
-      <c r="C51" t="s">
-        <v>57</v>
       </c>
       <c r="E51" s="6">
         <v>0</v>
@@ -1145,38 +1170,39 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="10"/>
       <c r="C52" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="10"/>
+      <c r="C53" t="s">
         <v>58</v>
       </c>
-      <c r="E52" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="B54" s="9"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="3" t="s">
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>51</v>
       </c>
       <c r="E56" s="6">
         <v>0</v>
@@ -1184,44 +1210,44 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>54</v>
       </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="E60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>63</v>
-      </c>
-      <c r="E62" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E63" s="6">
         <v>0</v>
@@ -1229,30 +1255,38 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>65</v>
-      </c>
-      <c r="E67" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="E68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>66</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E69" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] Améliorations faits (display slowfast) Final Stop : Optimisation. 50 à 100 FPS à gagner.
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>prio</t>
   </si>
@@ -255,7 +255,10 @@
     <t>En cours</t>
   </si>
   <si>
-    <t>Objectif 200 FPS+ en debug</t>
+    <t>Mettre combo derrière et centré</t>
+  </si>
+  <si>
+    <t>I5 + GT 560 Ti = 200/250 FPS en 1920 x 1080. Objectif 300.</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -411,7 +414,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -716,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +783,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -795,18 +797,18 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="18">
-        <v>0</v>
+      <c r="E8" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>1</v>
       </c>
       <c r="F9" t="s">
@@ -817,7 +819,7 @@
       <c r="B10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>1</v>
       </c>
       <c r="F10" t="s">
@@ -841,98 +843,99 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="12">
-        <v>1</v>
+      <c r="E14" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="19">
+        <v>11</v>
+      </c>
+      <c r="E15" s="12">
         <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="18">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E17" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
+      <c r="E18" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E20" s="18">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="6">
         <v>0</v>
@@ -940,23 +943,23 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>19</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>20</v>
       </c>
       <c r="E26" s="6">
         <v>0</v>
@@ -964,7 +967,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" s="6">
         <v>0</v>
@@ -972,18 +975,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>23</v>
-      </c>
-      <c r="E28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" t="s">
-        <v>25</v>
       </c>
       <c r="E29" s="6">
         <v>0</v>
@@ -991,15 +991,18 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>26</v>
-      </c>
-      <c r="E30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>27</v>
       </c>
       <c r="E31" s="6">
         <v>0</v>
@@ -1007,7 +1010,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E32" s="6">
         <v>0</v>
@@ -1015,31 +1018,31 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="E35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>31</v>
-      </c>
-      <c r="E35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>32</v>
       </c>
       <c r="E36" s="6">
         <v>0</v>
@@ -1047,7 +1050,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="6">
         <v>0</v>
@@ -1055,7 +1058,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="6">
         <v>0</v>
@@ -1063,7 +1066,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E39" s="6">
         <v>0</v>
@@ -1071,7 +1074,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E40" s="6">
         <v>0</v>
@@ -1079,15 +1082,15 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>37</v>
-      </c>
-      <c r="E41" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="E42" s="6">
         <v>0</v>
@@ -1095,82 +1098,81 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="3" t="s">
+      <c r="E44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="E45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+      <c r="E46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="E47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="9" t="s">
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="10" t="s">
+      <c r="E49" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="11" t="s">
+      <c r="E50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E51" s="7">
         <v>0.5</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="E51" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="10"/>
-      <c r="C52" t="s">
-        <v>57</v>
       </c>
       <c r="E52" s="6">
         <v>0</v>
@@ -1179,38 +1181,39 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="10"/>
       <c r="C53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="10"/>
+      <c r="C54" t="s">
         <v>58</v>
       </c>
-      <c r="E53" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="E54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="B55" s="9"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>49</v>
       </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E56" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>51</v>
       </c>
       <c r="E57" s="6">
         <v>0</v>
@@ -1218,44 +1221,44 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>52</v>
       </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+      <c r="E60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>54</v>
       </c>
-      <c r="E60" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="E61" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="E63" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E64" s="6">
         <v>0</v>
@@ -1263,30 +1266,38 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>67</v>
       </c>
-      <c r="E65" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="E66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>65</v>
-      </c>
-      <c r="E68" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>65</v>
+      </c>
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>66</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E70" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] MainMenu v3 Next step : Ajouter une fake stepchart en fond Ajouter le son Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -255,9 +255,6 @@
     <t>Mettre combo derrière et centré</t>
   </si>
   <si>
-    <t>I5 + GT 560 Ti = 200/250 FPS en 1920 x 1080. Objectif 300.</t>
-  </si>
-  <si>
     <t>Display medal</t>
   </si>
   <si>
@@ -276,7 +273,10 @@
     <t>en cours</t>
   </si>
   <si>
-    <t>Fond et placement boutons menu fait</t>
+    <t>Boutons faits : faire une fake stepchart à gauche + activer les boutons</t>
+  </si>
+  <si>
+    <t>Idée : SetActive les gameObject + setDisable les particules</t>
   </si>
 </sst>
 </file>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,10 +941,10 @@
         <v>59</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,12 +955,12 @@
         <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22" s="20">
         <v>0</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" s="20">
         <v>0</v>
@@ -983,7 +983,7 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="6"/>
     </row>
@@ -1000,10 +1000,10 @@
         <v>17</v>
       </c>
       <c r="E27" s="7">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>0.5</v>
       </c>
       <c r="F63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] MainMenu finalisé. Next step : GUI + text
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>prio</t>
   </si>
@@ -270,20 +270,20 @@
     <t>Splash screen</t>
   </si>
   <si>
-    <t>en cours</t>
-  </si>
-  <si>
-    <t>Boutons faits : faire une fake stepchart à gauche + activer les boutons</t>
-  </si>
-  <si>
     <t>Idée : SetActive les gameObject + setDisable les particules</t>
+  </si>
+  <si>
+    <t>Quasi fini : paufinage + retours</t>
+  </si>
+  <si>
+    <t>D'autres trucs à rajouter par la suite ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,7 +537,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -572,7 +571,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -748,14 +746,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
@@ -765,7 +763,7 @@
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,15 +783,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -801,7 +799,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -813,12 +811,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" s="17" t="s">
         <v>5</v>
       </c>
@@ -826,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" s="13"/>
       <c r="C8" s="17" t="s">
         <v>71</v>
@@ -835,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" s="17" t="s">
         <v>6</v>
       </c>
@@ -846,7 +844,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" s="17" t="s">
         <v>7</v>
       </c>
@@ -857,7 +855,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" s="17" t="s">
         <v>8</v>
       </c>
@@ -865,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
@@ -873,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="B13" s="13"/>
       <c r="C13" s="17" t="s">
         <v>78</v>
@@ -882,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
@@ -890,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" s="17" t="s">
         <v>11</v>
       </c>
@@ -898,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" s="17" t="s">
         <v>12</v>
       </c>
@@ -909,7 +907,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="B17" s="17" t="s">
         <v>13</v>
       </c>
@@ -917,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -925,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="B19" s="17" t="s">
         <v>60</v>
       </c>
@@ -936,7 +934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="B20" s="17" t="s">
         <v>59</v>
       </c>
@@ -947,7 +945,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="B21" s="22" t="s">
         <v>76</v>
       </c>
@@ -955,10 +953,10 @@
         <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="B22" s="24" t="s">
         <v>79</v>
       </c>
@@ -966,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="B23" s="24" t="s">
         <v>80</v>
       </c>
@@ -974,20 +972,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="25"/>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
@@ -995,26 +995,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="B27" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+    <row r="28" spans="1:6">
+      <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="C29" t="s">
         <v>19</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="D30" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="D31" t="s">
         <v>21</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="D32" t="s">
         <v>23</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5">
       <c r="C33" t="s">
         <v>24</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5">
       <c r="C34" t="s">
         <v>26</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5">
       <c r="D35" t="s">
         <v>27</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5">
       <c r="D36" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5">
       <c r="D37" t="s">
         <v>29</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5">
       <c r="D38" s="5" t="s">
         <v>30</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5">
       <c r="D40" t="s">
         <v>32</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5">
       <c r="D41" t="s">
         <v>33</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5">
       <c r="D42" t="s">
         <v>34</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5">
       <c r="D43" t="s">
         <v>35</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5">
       <c r="D44" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5">
       <c r="B46" s="3" t="s">
         <v>38</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5">
       <c r="B47" s="3" t="s">
         <v>39</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5">
       <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="B49" t="s">
         <v>41</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="C50" t="s">
         <v>44</v>
       </c>
@@ -1193,13 +1196,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>42</v>
       </c>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="B52" s="9" t="s">
         <v>43</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="9"/>
       <c r="B53" s="10" t="s">
         <v>45</v>
@@ -1216,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="B54" s="11" t="s">
         <v>55</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="B55" s="10" t="s">
         <v>56</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="B56" s="10"/>
       <c r="C56" t="s">
         <v>57</v>
@@ -1244,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="B57" s="10"/>
       <c r="C57" t="s">
         <v>58</v>
@@ -1253,14 +1256,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>48</v>
       </c>
       <c r="B58" s="9"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="B59" t="s">
         <v>49</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="B60" s="3" t="s">
         <v>50</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="B62" t="s">
         <v>52</v>
       </c>
@@ -1292,18 +1295,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="B63" s="21" t="s">
         <v>53</v>
       </c>
       <c r="E63" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="C64" t="s">
         <v>54</v>
       </c>
@@ -1311,12 +1314,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="B67" t="s">
         <v>63</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="B68" t="s">
         <v>62</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="B69" t="s">
         <v>67</v>
       </c>
@@ -1340,12 +1343,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="B72" t="s">
         <v>65</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="B73" t="s">
         <v>66</v>
       </c>
@@ -1368,24 +1371,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Update] Menu utilisable Next Step : Transition vers la wheel song
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>prio</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Fini</t>
   </si>
   <si>
-    <t>Necropole X selectionnée + Zekton ?</t>
-  </si>
-  <si>
     <t>work in progress !</t>
   </si>
   <si>
@@ -277,13 +274,19 @@
   </si>
   <si>
     <t>D'autres trucs à rajouter par la suite ?</t>
+  </si>
+  <si>
+    <t>FadeManager</t>
+  </si>
+  <si>
+    <t>Necropole X selectionnée + Zekton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +406,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -431,7 +452,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -448,6 +468,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,6 +562,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -571,6 +597,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -746,14 +773,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
@@ -763,7 +790,7 @@
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -780,30 +807,30 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="13"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" t="s">
         <v>46</v>
       </c>
@@ -811,76 +838,76 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="13"/>
-      <c r="C8" s="17" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="12">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="18">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="B11" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="B12" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="13"/>
-      <c r="C13" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
@@ -888,34 +915,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="17" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="17" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="B17" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -923,90 +950,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="B19" s="17" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="B20" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="23" t="s">
-        <v>82</v>
+      <c r="E20" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>77</v>
-      </c>
       <c r="F21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="B22" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="B23" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="E23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="25"/>
-      <c r="B25" s="8" t="s">
-        <v>83</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="E25" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="B27" s="21" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="7">
         <v>0.9</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
@@ -1014,10 +1041,10 @@
         <v>0.9</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>19</v>
       </c>
@@ -1025,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>20</v>
       </c>
@@ -1033,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>24</v>
       </c>
@@ -1060,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>29</v>
       </c>
@@ -1092,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>30</v>
       </c>
@@ -1100,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -1108,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>32</v>
       </c>
@@ -1116,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>33</v>
       </c>
@@ -1124,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>34</v>
       </c>
@@ -1132,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>35</v>
       </c>
@@ -1140,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>36</v>
       </c>
@@ -1148,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1156,23 +1183,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="3" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E46" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="3" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="26" t="s">
         <v>39</v>
       </c>
       <c r="E47" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
@@ -1180,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>41</v>
       </c>
@@ -1188,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>44</v>
       </c>
@@ -1196,13 +1223,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>43</v>
       </c>
@@ -1210,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="10" t="s">
         <v>45</v>
@@ -1219,18 +1246,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="B54" s="11" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="7">
-        <v>0.5</v>
+      <c r="E54" s="11">
+        <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
         <v>56</v>
       </c>
@@ -1238,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="10"/>
       <c r="C56" t="s">
         <v>57</v>
@@ -1247,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="10"/>
       <c r="C57" t="s">
         <v>58</v>
@@ -1256,14 +1283,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
       <c r="B58" s="9"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>49</v>
       </c>
@@ -1271,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>50</v>
       </c>
@@ -1279,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -1287,80 +1314,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
-      <c r="B62" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E62" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="B63" s="21" t="s">
+      <c r="E62" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E64" s="7">
         <v>0.9</v>
       </c>
-      <c r="F63" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="C64" t="s">
+      <c r="F64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>54</v>
       </c>
-      <c r="E64" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
-      <c r="B67" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>63</v>
       </c>
-      <c r="E67" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="B68" t="s">
+      <c r="E68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>62</v>
       </c>
-      <c r="E68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="B69" t="s">
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>67</v>
       </c>
-      <c r="E69" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
+      <c r="E70" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
-      <c r="B72" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="B73" t="s">
+      <c r="E73" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>66</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E74" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1371,24 +1406,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Update] SongWheel en cours de réa. Buggé
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>prio</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Idée : SetActive les gameObject + setDisable les particules</t>
   </si>
   <si>
-    <t>Quasi fini : paufinage + retours</t>
-  </si>
-  <si>
     <t>D'autres trucs à rajouter par la suite ?</t>
   </si>
   <si>
@@ -280,6 +277,15 @@
   </si>
   <si>
     <t>Necropole X selectionnée + Zekton</t>
+  </si>
+  <si>
+    <t>Choix des packs à débugger</t>
+  </si>
+  <si>
+    <t>paufinage + retours</t>
+  </si>
+  <si>
+    <t>A tester + ajouter d'autres trucs ?</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,25 +1029,25 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="7">
-        <v>0.9</v>
+      <c r="E27" s="17">
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="7">
-        <v>0.9</v>
+      <c r="E28" s="17">
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1076,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>24</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>26</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>28</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>29</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>30</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>32</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>33</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>34</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>35</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>36</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1183,15 +1189,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="26" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
         <v>39</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
@@ -1254,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1324,10 +1333,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E63" s="19">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,7 +1350,7 @@
         <v>0.9</v>
       </c>
       <c r="F64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Progression de la wheelSong
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>prio</t>
   </si>
@@ -270,6 +270,9 @@
     <t>Idée : SetActive les gameObject + setDisable les particules</t>
   </si>
   <si>
+    <t>Quasi fini : paufinage + retours</t>
+  </si>
+  <si>
     <t>D'autres trucs à rajouter par la suite ?</t>
   </si>
   <si>
@@ -277,15 +280,6 @@
   </si>
   <si>
     <t>Necropole X selectionnée + Zekton</t>
-  </si>
-  <si>
-    <t>Choix des packs à débugger</t>
-  </si>
-  <si>
-    <t>paufinage + retours</t>
-  </si>
-  <si>
-    <t>A tester + ajouter d'autres trucs ?</t>
   </si>
 </sst>
 </file>
@@ -478,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,25 +1023,25 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="17">
-        <v>1</v>
+      <c r="E27" s="7">
+        <v>0.9</v>
       </c>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="17">
-        <v>1</v>
+      <c r="E28" s="7">
+        <v>0.9</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>24</v>
       </c>
@@ -1093,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>26</v>
       </c>
@@ -1101,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>27</v>
       </c>
@@ -1109,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>28</v>
       </c>
@@ -1117,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>29</v>
       </c>
@@ -1125,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>30</v>
       </c>
@@ -1133,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>32</v>
       </c>
@@ -1149,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>33</v>
       </c>
@@ -1157,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>34</v>
       </c>
@@ -1165,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>35</v>
       </c>
@@ -1173,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>36</v>
       </c>
@@ -1181,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1189,18 +1183,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="20" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
         <v>39</v>
       </c>
@@ -1208,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
@@ -1263,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1333,13 +1324,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E63" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F63" t="s">
-        <v>89</v>
+        <v>86</v>
+      </c>
+      <c r="E63" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1350,7 +1338,7 @@
         <v>0.9</v>
       </c>
       <c r="F64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Selection de chanson en cours de réa next Step : Slide de la liste Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
   <si>
     <t>prio</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Necropole X selectionnée + Zekton</t>
+  </si>
+  <si>
+    <t>Pack ok, song en cours</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,22 +1026,22 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="7">
-        <v>0.9</v>
+      <c r="E27" s="17">
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="7">
-        <v>0.9</v>
+      <c r="E28" s="17">
+        <v>1</v>
       </c>
       <c r="F28" t="s">
         <v>84</v>
@@ -1076,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>24</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>26</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>28</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>29</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>30</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>32</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>33</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>34</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>35</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>36</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1183,15 +1186,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="26" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
         <v>39</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
@@ -1326,8 +1332,11 @@
       <c r="B63" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E63" s="19">
-        <v>0</v>
+      <c r="E63" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Wheel et supress. Toujours bug
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>prio</t>
   </si>
@@ -283,6 +283,24 @@
   </si>
   <si>
     <t>Pack ok, song en cours</t>
+  </si>
+  <si>
+    <t>Packs</t>
+  </si>
+  <si>
+    <t>Songs</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Lancement song</t>
+  </si>
+  <si>
+    <t>Choix difficulté</t>
+  </si>
+  <si>
+    <t>En cours, buggé</t>
   </si>
 </sst>
 </file>
@@ -777,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,220 +1209,268 @@
         <v>38</v>
       </c>
       <c r="E46" s="7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F46" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="24"/>
+      <c r="C47" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="24"/>
+      <c r="C48" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="24"/>
+      <c r="C49" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="24"/>
+      <c r="C50" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="24"/>
+      <c r="C51" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="3" t="s">
+      <c r="E52" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>41</v>
       </c>
-      <c r="E49" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+      <c r="E54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="9" t="s">
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
-      <c r="B53" s="10" t="s">
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+      <c r="B58" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="28" t="s">
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="11">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="E59" s="11">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="10" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="10"/>
-      <c r="C56" t="s">
+      <c r="E60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="10"/>
+      <c r="C61" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="10"/>
-      <c r="C57" t="s">
+      <c r="E61" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="10"/>
+      <c r="C62" t="s">
         <v>58</v>
       </c>
-      <c r="E57" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="E62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>48</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="B63" s="9"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>49</v>
       </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+      <c r="E64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E60" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>51</v>
       </c>
-      <c r="E61" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="16" t="s">
+      <c r="E66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E62" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="29" t="s">
+      <c r="E67" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E68" s="7">
         <v>0.9</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F68" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="20" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E69" s="7">
         <v>0.9</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F69" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>54</v>
       </c>
-      <c r="E65" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="E70" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>63</v>
       </c>
-      <c r="E68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+      <c r="E73" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>62</v>
       </c>
-      <c r="E69" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="E74" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="E75" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>65</v>
       </c>
-      <c r="E73" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="E78" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>66</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E79" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] Graph ok ! Description ok ! FadeIn fadeOut vers Option ok ! Next step : Panneau d'option / lien vers la scene de song / lien vers le mainmenu
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>prio</t>
   </si>
@@ -171,9 +171,6 @@
     <t>DataManager</t>
   </si>
   <si>
-    <t>SaveManager</t>
-  </si>
-  <si>
     <t>TextManager</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>Necropole X selectionnée + Zekton</t>
   </si>
   <si>
-    <t>Pack ok, song en cours</t>
-  </si>
-  <si>
     <t>Packs</t>
   </si>
   <si>
@@ -300,7 +294,31 @@
     <t>Choix difficulté</t>
   </si>
   <si>
-    <t>En cours, buggé</t>
+    <t>Si possible de modifier ?</t>
+  </si>
+  <si>
+    <t>Display medals</t>
+  </si>
+  <si>
+    <t>Display best score</t>
+  </si>
+  <si>
+    <t>En attente de l'implémentation des profils</t>
+  </si>
+  <si>
+    <t>idem</t>
+  </si>
+  <si>
+    <t>FadeIn / FadeOut effectué : next step : afficher les options</t>
+  </si>
+  <si>
+    <t>En stand by de l'implémentation des profils</t>
+  </si>
+  <si>
+    <t>ProfileManager</t>
+  </si>
+  <si>
+    <t>Améliorer les cross detection (suite 1-2-3-1)</t>
   </si>
 </sst>
 </file>
@@ -357,7 +375,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,12 +456,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -491,9 +503,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,12 +840,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,7 +887,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="11">
         <v>1</v>
@@ -889,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -900,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,7 +934,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" s="11">
         <v>1</v>
@@ -952,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -973,40 +985,40 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="11">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22" s="19">
         <v>0</v>
@@ -1014,7 +1026,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="19">
         <v>0</v>
@@ -1028,8 +1040,8 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="27" t="s">
-        <v>82</v>
+      <c r="B25" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="E25" s="6">
         <v>0</v>
@@ -1051,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1062,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1209,16 +1221,16 @@
         <v>38</v>
       </c>
       <c r="E46" s="7">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="F46" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
       <c r="C47" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E47" s="11">
         <v>1</v>
@@ -1226,251 +1238,281 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="24"/>
-      <c r="C48" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F48" t="s">
-        <v>94</v>
+      <c r="C48" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="24"/>
-      <c r="C49" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E49" s="7">
-        <v>0</v>
+      <c r="C49" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="17">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="24"/>
-      <c r="C50" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" s="7">
-        <v>0</v>
+      <c r="C50" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="24"/>
-      <c r="C51" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" s="7">
-        <v>0</v>
+      <c r="C51" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" s="19">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="24"/>
+      <c r="C52" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="19">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="24"/>
+      <c r="C53" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="25" t="s">
+      <c r="E54" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E53" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>41</v>
       </c>
-      <c r="E54" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E57" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10" t="s">
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="28" t="s">
+      <c r="E60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="11">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E59" s="11">
-        <v>1</v>
-      </c>
-      <c r="F59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
+      <c r="E62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="10"/>
+      <c r="C63" t="s">
         <v>56</v>
       </c>
-      <c r="E60" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="10"/>
-      <c r="C61" t="s">
+      <c r="E63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="10"/>
+      <c r="C64" t="s">
         <v>57</v>
       </c>
-      <c r="E61" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="10"/>
-      <c r="C62" t="s">
-        <v>58</v>
-      </c>
-      <c r="E62" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="E64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>48</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>49</v>
-      </c>
-      <c r="E64" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E65" s="6">
-        <v>0</v>
-      </c>
+      <c r="B65" s="9"/>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>99</v>
+      </c>
+      <c r="E68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E66" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="16" t="s">
+      <c r="E69" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E67" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="7">
+      <c r="E71" s="17">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C72" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E72" s="7">
         <v>0.9</v>
       </c>
-      <c r="F68" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E69" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F69" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>54</v>
-      </c>
-      <c r="E70" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>63</v>
-      </c>
-      <c r="E73" s="6">
-        <v>0</v>
+      <c r="F72" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>62</v>
-      </c>
-      <c r="E74" s="6">
-        <v>0</v>
+      <c r="A74" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E75" s="6">
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76" s="6">
+        <v>0</v>
+      </c>
+    </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="B77" t="s">
+        <v>66</v>
+      </c>
+      <c r="E77" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="E80" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>65</v>
       </c>
-      <c r="E78" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>66</v>
-      </c>
-      <c r="E79" s="6">
+      <c r="E81" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] Preview song ok ! Option judge ok ! Next step : Faire les options / tri / lancer la song / application des options
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
   <si>
     <t>prio</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Fun</t>
   </si>
   <si>
-    <t>1j, 2j, mode 8t</t>
-  </si>
-  <si>
     <t>Modes</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Medaille</t>
   </si>
   <si>
-    <t>Notes ? Autres ?</t>
-  </si>
-  <si>
     <t>Background scene</t>
   </si>
   <si>
@@ -237,9 +231,6 @@
     <t>Façon plus opti ?</t>
   </si>
   <si>
-    <t>Rajouter une petite particule ?</t>
-  </si>
-  <si>
     <t>Optimisation</t>
   </si>
   <si>
@@ -267,9 +258,6 @@
     <t>Idée : SetActive les gameObject + setDisable les particules</t>
   </si>
   <si>
-    <t>Quasi fini : paufinage + retours</t>
-  </si>
-  <si>
     <t>D'autres trucs à rajouter par la suite ?</t>
   </si>
   <si>
@@ -319,6 +307,45 @@
   </si>
   <si>
     <t>Améliorer les cross detection (suite 1-2-3-1)</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Pas compliqué</t>
+  </si>
+  <si>
+    <t>Option affection</t>
+  </si>
+  <si>
+    <t>Skin "flèche"</t>
+  </si>
+  <si>
+    <t>avec le temps</t>
+  </si>
+  <si>
+    <t>Skin "rond"</t>
+  </si>
+  <si>
+    <t>Skin "&lt;"</t>
+  </si>
+  <si>
+    <t>Tester le refresh !!!!</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Update Profiles</t>
+  </si>
+  <si>
+    <t>1j, 2jLAN, mode 8t</t>
+  </si>
+  <si>
+    <t>Tri</t>
+  </si>
+  <si>
+    <t>Ajouter le son</t>
   </si>
 </sst>
 </file>
@@ -375,7 +402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +487,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -473,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -499,13 +538,18 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,12 +884,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,10 +909,10 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
         <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -887,7 +931,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" s="11">
         <v>1</v>
@@ -901,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -912,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,6 +966,9 @@
       <c r="E11" s="11">
         <v>1</v>
       </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
@@ -934,19 +981,17 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
@@ -960,11 +1005,8 @@
       <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="17">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>73</v>
+      <c r="E16" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,118 +1026,108 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="11">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="B19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="F23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="F21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="25" t="s">
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="17">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+      <c r="E29" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="17">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>19</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>21</v>
       </c>
       <c r="E31" s="6">
         <v>0</v>
@@ -1103,42 +1135,42 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>24</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>25</v>
-      </c>
-      <c r="E33" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>28</v>
       </c>
       <c r="E36" s="6">
         <v>0</v>
@@ -1146,39 +1178,39 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D38" s="5" t="s">
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>30</v>
-      </c>
-      <c r="E38" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>33</v>
       </c>
       <c r="E41" s="6">
         <v>0</v>
@@ -1186,7 +1218,7 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E42" s="6">
         <v>0</v>
@@ -1194,7 +1226,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E43" s="6">
         <v>0</v>
@@ -1202,7 +1234,7 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E44" s="6">
         <v>0</v>
@@ -1210,309 +1242,375 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
+      <c r="E48" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="23"/>
+      <c r="C49" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="23"/>
+      <c r="C50" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="23"/>
+      <c r="C51" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="17">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="23"/>
+      <c r="C52" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="23"/>
+      <c r="C53" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="19">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="23"/>
+      <c r="C54" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="19">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="23"/>
+      <c r="C55" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="23"/>
+      <c r="C56" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="19">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="24"/>
-      <c r="C47" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="24"/>
-      <c r="C48" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E48" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="24"/>
-      <c r="C49" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="17">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="24"/>
-      <c r="C50" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="24"/>
-      <c r="C51" s="29" t="s">
+      <c r="E57" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F57" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="19">
-        <v>0</v>
-      </c>
-      <c r="F51" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="24"/>
-      <c r="C52" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" s="19">
-        <v>0</v>
-      </c>
-      <c r="F52" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="24"/>
-      <c r="C53" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="8" t="s">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E54" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F54" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="8" t="s">
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>41</v>
       </c>
-      <c r="E56" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
+      <c r="B66" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
-      <c r="B60" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="27" t="s">
+      <c r="E66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="11">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="11">
-        <v>1</v>
-      </c>
-      <c r="F61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="10" t="s">
+      <c r="E68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="10"/>
+      <c r="C69" t="s">
         <v>55</v>
       </c>
-      <c r="E62" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="10"/>
-      <c r="C63" t="s">
-        <v>56</v>
-      </c>
-      <c r="E63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="10"/>
-      <c r="C64" t="s">
-        <v>57</v>
-      </c>
-      <c r="E64" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="10"/>
+      <c r="C70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="10"/>
+      <c r="C71" t="s">
+        <v>102</v>
+      </c>
+      <c r="E71" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="10"/>
+      <c r="C72" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" s="6">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="9"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>48</v>
       </c>
-      <c r="B65" s="9"/>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="E74" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E66" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E67" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E69" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E70" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F70" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E71" s="17">
-        <v>1</v>
-      </c>
-      <c r="F71" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C72" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E72" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F72" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>62</v>
-      </c>
-      <c r="E75" s="6">
-        <v>0</v>
+      <c r="E75" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>95</v>
+      </c>
+      <c r="E76" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" s="17">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" s="17">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C80" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F80" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>60</v>
+      </c>
+      <c r="E83" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>59</v>
+      </c>
+      <c r="E84" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>61</v>
       </c>
-      <c r="E76" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>66</v>
-      </c>
-      <c r="E77" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E88" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>64</v>
-      </c>
-      <c r="E80" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>65</v>
-      </c>
-      <c r="E81" s="6">
+      <c r="E89" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] Ecran d'option clean. Début des options dans le InGameScript
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>prio</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Splash screen</t>
   </si>
   <si>
-    <t>Idée : SetActive les gameObject + setDisable les particules</t>
-  </si>
-  <si>
     <t>D'autres trucs à rajouter par la suite ?</t>
   </si>
   <si>
@@ -346,6 +343,21 @@
   </si>
   <si>
     <t>Ajouter le son</t>
+  </si>
+  <si>
+    <t>Idée : Particle : Mettre un script pour les disable si !isPlaying, gameObject : Mettre un script qui a la liste de tous les GO et active ceux &lt; à 10 sec du timer</t>
+  </si>
+  <si>
+    <t>Tuto</t>
+  </si>
+  <si>
+    <t>tuto classique</t>
+  </si>
+  <si>
+    <t>Mode "repeat" val</t>
+  </si>
+  <si>
+    <t>Changer le streaming en loading complet</t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -550,6 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1000,6 +1013,9 @@
       <c r="E15" s="11">
         <v>1</v>
       </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
@@ -1027,7 +1043,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
@@ -1035,7 +1051,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" s="6">
         <v>0</v>
@@ -1071,7 +1087,7 @@
         <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1094,7 +1110,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>78</v>
       </c>
       <c r="E27" s="6">
@@ -1141,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>23</v>
       </c>
@@ -1157,18 +1173,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>26</v>
       </c>
@@ -1184,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>27</v>
       </c>
@@ -1192,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>28</v>
       </c>
@@ -1200,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
         <v>29</v>
       </c>
@@ -1208,107 +1224,101 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>30</v>
       </c>
-      <c r="E41" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+      <c r="E44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+      <c r="E45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
+      <c r="E46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
+      <c r="E47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+      <c r="E48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+      <c r="E49" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="20" t="s">
+      <c r="E50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E51" s="7">
         <v>0.9</v>
       </c>
-      <c r="F48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="23"/>
-      <c r="C49" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="23"/>
-      <c r="C50" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E50" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="23"/>
-      <c r="C51" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E51" s="17">
-        <v>1</v>
-      </c>
       <c r="F51" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="23"/>
       <c r="C52" s="16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E52" s="11">
         <v>1</v>
@@ -1316,93 +1326,101 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="23"/>
-      <c r="C53" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E53" s="19">
-        <v>0</v>
-      </c>
-      <c r="F53" t="s">
-        <v>91</v>
+      <c r="C53" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="23"/>
-      <c r="C54" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" s="19">
-        <v>0</v>
+      <c r="C54" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="17">
+        <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="23"/>
-      <c r="C55" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="E55" s="19">
-        <v>0</v>
+      <c r="C55" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="23"/>
-      <c r="C56" s="32" t="s">
-        <v>86</v>
+      <c r="C56" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="E56" s="19">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="23"/>
+      <c r="C57" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E57" s="19">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="23"/>
+      <c r="C58" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="E58" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="23"/>
+      <c r="C59" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="19">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E60" s="7">
         <v>0.5</v>
       </c>
-      <c r="F57" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="8" t="s">
+      <c r="F60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>43</v>
-      </c>
-      <c r="E60" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>41</v>
-      </c>
-      <c r="E61" s="6"/>
+      <c r="E61" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="E62" s="6">
         <v>0</v>
@@ -1410,71 +1428,66 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>106</v>
-      </c>
-      <c r="E63" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="E63" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
       <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="9" t="s">
+      <c r="B65" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E65" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="10" t="s">
+      <c r="E68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="9"/>
+      <c r="B69" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E66" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="26" t="s">
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E67" s="11">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
+      <c r="E70" s="11">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="E68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="10"/>
-      <c r="C69" t="s">
-        <v>55</v>
-      </c>
-      <c r="E69" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="10"/>
-      <c r="C70" t="s">
-        <v>103</v>
-      </c>
-      <c r="E70" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="10"/>
-      <c r="C71" t="s">
-        <v>102</v>
       </c>
       <c r="E71" s="6">
         <v>0</v>
@@ -1483,134 +1496,161 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="10"/>
       <c r="C72" t="s">
+        <v>55</v>
+      </c>
+      <c r="E72" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="10"/>
+      <c r="C73" t="s">
+        <v>102</v>
+      </c>
+      <c r="E73" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="10"/>
+      <c r="C74" t="s">
+        <v>101</v>
+      </c>
+      <c r="E74" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="10"/>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" s="6">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>48</v>
+      </c>
+      <c r="E77" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E72" s="6">
-        <v>0</v>
-      </c>
-      <c r="F72" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="E73" s="6"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>48</v>
-      </c>
-      <c r="E74" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" s="17">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82" s="17">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F83" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E77" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E78" s="17">
-        <v>1</v>
-      </c>
-      <c r="F78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E79" s="17">
-        <v>1</v>
-      </c>
-      <c r="F79" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E80" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F80" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>60</v>
       </c>
-      <c r="E83" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+      <c r="E86" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>59</v>
       </c>
-      <c r="E84" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+      <c r="E87" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>64</v>
       </c>
-      <c r="E85" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="E88" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>62</v>
       </c>
-      <c r="E88" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+      <c r="E91" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>63</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E92" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Update] AnimOption ok, SearchBar en cours
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t>prio</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Changer le streaming en loading complet</t>
+  </si>
+  <si>
+    <t>Prévoir le support only keyboard/tapis</t>
   </si>
 </sst>
 </file>
@@ -866,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1407,7 @@
         <v>38</v>
       </c>
       <c r="E60" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F60" t="s">
         <v>92</v>
@@ -1414,8 +1417,11 @@
       <c r="C61" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E61" s="6">
-        <v>0</v>
+      <c r="E61" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F61" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] Clear ok, Fail ok, Full Combo ok. Next Step : Splach Screen launch song + Score Screen.
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -527,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -554,18 +554,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1003,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="6"/>
@@ -1024,7 +1023,7 @@
       <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1037,7 +1036,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="6">
@@ -1045,7 +1044,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="34" t="s">
         <v>98</v>
       </c>
       <c r="E19" s="6">
@@ -1053,7 +1052,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="16" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="6">
@@ -1094,13 +1093,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="28" t="s">
         <v>74</v>
       </c>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>75</v>
       </c>
       <c r="E25" s="19"/>
@@ -1121,7 +1120,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="30" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="6">
@@ -1228,7 +1227,7 @@
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="24" t="s">
         <v>110</v>
       </c>
       <c r="E41" s="6">
@@ -1236,7 +1235,7 @@
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="33" t="s">
         <v>111</v>
       </c>
       <c r="E42" s="6">
@@ -1244,7 +1243,7 @@
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="27" t="s">
         <v>112</v>
       </c>
       <c r="E43" s="6">
@@ -1308,11 +1307,11 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="7">
-        <v>0.9</v>
+      <c r="E51" s="17">
+        <v>1</v>
       </c>
       <c r="F51" t="s">
         <v>93</v>
@@ -1359,7 +1358,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="23"/>
-      <c r="C56" s="28" t="s">
+      <c r="C56" s="27" t="s">
         <v>88</v>
       </c>
       <c r="E56" s="19">
@@ -1371,7 +1370,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="23"/>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="27" t="s">
         <v>89</v>
       </c>
       <c r="E57" s="19">
@@ -1383,7 +1382,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" s="23"/>
-      <c r="C58" s="33" t="s">
+      <c r="C58" s="31" t="s">
         <v>107</v>
       </c>
       <c r="E58" s="19">
@@ -1392,7 +1391,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" s="23"/>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="16" t="s">
         <v>85</v>
       </c>
       <c r="E59" s="19">
@@ -1403,22 +1402,22 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="7">
-        <v>0.9</v>
+      <c r="E60" s="17">
+        <v>1</v>
       </c>
       <c r="F60" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E61" s="7">
-        <v>0.9</v>
+      <c r="E61" s="17">
+        <v>1</v>
       </c>
       <c r="F61" t="s">
         <v>114</v>
@@ -1481,7 +1480,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="26" t="s">
+      <c r="B70" s="25" t="s">
         <v>53</v>
       </c>
       <c r="E70" s="11">
@@ -1600,7 +1599,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C83" s="27" t="s">
+      <c r="C83" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E83" s="7">

</xml_diff>

<commit_message>
[Build 100] Score screen quasi fini. Reste à animer et à corriger certains points
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Stepchart</t>
   </si>
@@ -222,18 +222,12 @@
     <t>???</t>
   </si>
   <si>
-    <t>Correction de la detection de cross, son dans la wheelsong</t>
-  </si>
-  <si>
     <t>dll</t>
   </si>
   <si>
     <t>dll previewSong</t>
   </si>
   <si>
-    <t>Encardrement des chiffres, encadrement du graph, banner, son, clignotement full combo, faire bouger le fond</t>
-  </si>
-  <si>
     <t>"CubeScore" (Wister idea)</t>
   </si>
   <si>
@@ -241,13 +235,22 @@
   </si>
   <si>
     <t>Cube ? RenderTOCubemap</t>
+  </si>
+  <si>
+    <t>Apparition des petits écrans</t>
+  </si>
+  <si>
+    <t>son, clignotement léger full combo</t>
+  </si>
+  <si>
+    <t>Correction de la detection de cross, sons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +261,20 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,13 +300,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,13 +656,13 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="1">
+        <v>71</v>
+      </c>
+      <c r="E4" s="4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -656,11 +675,11 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
+      <c r="E5" s="5">
+        <v>0.4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -685,7 +704,9 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1046,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -1058,10 +1079,10 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
         <v>69</v>
-      </c>
-      <c r="D34" t="s">
-        <v>70</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -1097,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 101] [Update] [NOT COMPILED] Ajout du script pour faire tourner les medailles empecher les spheres de rotate avec le reste Bouton stylé ajouté Script pour permettre l'affichage des medailles ajouté (non testé)
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -234,9 +234,6 @@
     <t>Medals</t>
   </si>
   <si>
-    <t>Cube ? RenderTOCubemap</t>
-  </si>
-  <si>
     <t>Apparition des petits écrans</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Correction de la detection de cross, sons</t>
+  </si>
+  <si>
+    <t>A intégrer</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +659,10 @@
         <v>71</v>
       </c>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>0.4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 200][Update] Ecran des scores 100% fonctionnel Next step : quit/retry dans l'écran de fail (+ son ?)
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -234,16 +234,16 @@
     <t>Medals</t>
   </si>
   <si>
-    <t>Apparition des petits écrans</t>
-  </si>
-  <si>
-    <t>son, clignotement léger full combo</t>
-  </si>
-  <si>
-    <t>Correction de la detection de cross, sons</t>
-  </si>
-  <si>
-    <t>A intégrer</t>
+    <t>Signaler les morts dans le graph</t>
+  </si>
+  <si>
+    <t>Baisser le volume doucement transition</t>
+  </si>
+  <si>
+    <t>Correction de la detection de cross, sons (partout), correction son wheel song</t>
+  </si>
+  <si>
+    <t>Si le temps : Faire le main son de la wheel song</t>
   </si>
 </sst>
 </file>
@@ -274,18 +274,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -300,15 +311,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,7 +627,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,61 +666,60 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
+      <c r="E4" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>200</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
+      <c r="E6" s="5">
+        <v>1</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -733,7 +746,9 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -748,7 +763,9 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1104,7 +1121,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1000</v>
       </c>

</xml_diff>

<commit_message>
[Build 201] Retry/Quit a tester "no mine" fait.
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>Stepchart</t>
   </si>
@@ -237,33 +237,9 @@
     <t>Correction de la detection de cross, sons (partout), correction son wheel song</t>
   </si>
   <si>
-    <t>Si le temps : Faire le main son de la wheel song</t>
-  </si>
-  <si>
-    <t>Sptechart</t>
-  </si>
-  <si>
     <t>Option "Display"</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Signaler les morts dans le graph, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> corriger le % de misteak qui est faux</t>
-    </r>
-  </si>
-  <si>
-    <t>Regarder aussi l'explosion bizarre full combo</t>
-  </si>
-  <si>
     <t>Rate</t>
   </si>
   <si>
@@ -277,13 +253,28 @@
   </si>
   <si>
     <t>Editor</t>
+  </si>
+  <si>
+    <t>Corriger les bugs des mines avec</t>
+  </si>
+  <si>
+    <t>Si le temps : Faire le main son de la wheel song correctement</t>
+  </si>
+  <si>
+    <t>Signaler les morts dans le graph</t>
+  </si>
+  <si>
+    <t>Regarder aussi l'explosion bizarre full combo, tester</t>
+  </si>
+  <si>
+    <t>Reflechir à un truc propre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +298,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -344,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,6 +358,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,27 +768,29 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
+      <c r="E8" s="12">
+        <v>0.7</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3"/>
+      <c r="E9" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -801,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -910,7 +912,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1155,7 +1157,9 @@
       <c r="E35" s="1">
         <v>0</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -1204,7 +1208,7 @@
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -1260,7 +1264,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>55</v>
@@ -1268,31 +1272,32 @@
       <c r="D43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2000</v>
-      </c>
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="1">
         <v>0</v>
       </c>
@@ -1300,10 +1305,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>3000</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>59</v>
+        <v>2000</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -1312,13 +1317,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -1327,13 +1329,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -1342,47 +1344,52 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>6000</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>7000</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C52" s="2"/>
       <c r="E52" s="1">
@@ -1391,11 +1398,8 @@
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>65</v>
-      </c>
       <c r="B53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="2"/>
       <c r="E53" s="1">
@@ -1405,10 +1409,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="2"/>
       <c r="E54" s="1">
@@ -1418,15 +1422,28 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C55" s="2"/>
       <c r="E55" s="1">
         <v>0</v>
       </c>
       <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 202] Save/Load profile ok Optim du graph de Score Reglage des boutons quit/retry Correction du bug des songs qui ne marchent pas D'autres corrections (voir Planning.xlsx)
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
   <si>
     <t>Stepchart</t>
   </si>
@@ -96,9 +96,6 @@
     <t>ProfilManager / ScoreScreen</t>
   </si>
   <si>
-    <t>Save/Load profil</t>
-  </si>
-  <si>
     <t>SplashScreen</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Vitesse molette</t>
   </si>
   <si>
-    <t>Mode tapis + raccourci</t>
-  </si>
-  <si>
     <t>Binding touches</t>
   </si>
   <si>
@@ -171,18 +165,12 @@
     <t>General</t>
   </si>
   <si>
-    <t>Correction générale</t>
-  </si>
-  <si>
     <t>Build</t>
   </si>
   <si>
     <t>Mode LAN</t>
   </si>
   <si>
-    <t>Do it</t>
-  </si>
-  <si>
     <t>LAN</t>
   </si>
   <si>
@@ -258,16 +246,55 @@
     <t>Corriger les bugs des mines avec</t>
   </si>
   <si>
-    <t>Si le temps : Faire le main son de la wheel song correctement</t>
-  </si>
-  <si>
-    <t>Signaler les morts dans le graph</t>
-  </si>
-  <si>
-    <t>Regarder aussi l'explosion bizarre full combo, tester</t>
-  </si>
-  <si>
-    <t>Reflechir à un truc propre</t>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Faire en sorte que InGameScript prenne 2 touches par bind</t>
+  </si>
+  <si>
+    <t>Ecran d'init de profile</t>
+  </si>
+  <si>
+    <t>Trucs à rajouter par la suite</t>
+  </si>
+  <si>
+    <t>stand by</t>
+  </si>
+  <si>
+    <t>Première phase de test privée</t>
+  </si>
+  <si>
+    <t>Mode "rapide"</t>
+  </si>
+  <si>
+    <t>Mettre la config du globaloffset second + les touches dans un txt</t>
+  </si>
+  <si>
+    <t>Load profile</t>
+  </si>
+  <si>
+    <t>Tester le son</t>
+  </si>
+  <si>
+    <t>Mode tapis + raccourci keyboard</t>
+  </si>
+  <si>
+    <t>Correction générale + optim</t>
+  </si>
+  <si>
+    <t>Deuxième phase de test publique</t>
+  </si>
+  <si>
+    <t>Transistion "splashcreen"</t>
+  </si>
+  <si>
+    <t>Tester des mix pour les graph, tester le nouveau graph</t>
+  </si>
+  <si>
+    <t>Tester quand même "My Name Is"</t>
+  </si>
+  <si>
+    <t>Regarder aussi l'explosion bizarre full combo, tester, bug au niveau de la disparition</t>
   </si>
 </sst>
 </file>
@@ -342,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -354,12 +381,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,18 +687,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
@@ -684,7 +710,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -704,11 +730,11 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -723,10 +749,10 @@
         <v>16</v>
       </c>
       <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>81</v>
+        <v>0.99</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -758,94 +784,103 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>82</v>
+      <c r="E8" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>83</v>
+      <c r="E9" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
       <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>80</v>
+        <v>89</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>300</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3"/>
+      <c r="E13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -861,7 +896,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -876,7 +911,7 @@
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -884,6 +919,9 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>400</v>
+      </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -896,77 +934,76 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>400</v>
-      </c>
       <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>500</v>
+      </c>
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>500</v>
-      </c>
       <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>600</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>600</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>32</v>
-      </c>
-      <c r="D23" t="s">
-        <v>34</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -975,13 +1012,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
         <v>31</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -989,32 +1026,32 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>700</v>
       </c>
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -1023,28 +1060,24 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
         <v>38</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" t="s">
-        <v>41</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -1053,13 +1086,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -1068,13 +1101,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -1083,13 +1116,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1098,28 +1131,30 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -1127,17 +1162,14 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>800</v>
-      </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -1146,27 +1178,28 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -1174,29 +1207,34 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>800</v>
+      </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>900</v>
-      </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -1205,85 +1243,78 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>20</v>
       </c>
-      <c r="C39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>900</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>1000</v>
       </c>
-      <c r="B40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>24</v>
+      <c r="B44" t="s">
+        <v>52</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -1295,20 +1326,25 @@
         <v>7</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E45" s="1">
         <v>0</v>
       </c>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2000</v>
-      </c>
-      <c r="B46" t="s">
-        <v>56</v>
+      <c r="B46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -1316,11 +1352,14 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>3000</v>
-      </c>
       <c r="B47" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -1328,14 +1367,14 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>4000</v>
-      </c>
       <c r="B48" s="2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -1343,15 +1382,13 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>5000</v>
-      </c>
       <c r="B49" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="1">
         <v>0</v>
       </c>
@@ -1359,13 +1396,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -1373,11 +1407,11 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3000</v>
+      </c>
       <c r="B51" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -1386,64 +1420,120 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>4000</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5000</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>6000</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>7000</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
+      <c r="C56" s="2"/>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="3"/>
+      <c r="B59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 203] [Update] Nombreux test effectués, planning a jour Debut du "splash song screen"
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>Stepchart</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Corriger les bugs des mines avec</t>
   </si>
   <si>
-    <t>Tester</t>
-  </si>
-  <si>
     <t>Faire en sorte que InGameScript prenne 2 touches par bind</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>Load profile</t>
   </si>
   <si>
-    <t>Tester le son</t>
-  </si>
-  <si>
     <t>Mode tapis + raccourci keyboard</t>
   </si>
   <si>
@@ -288,13 +282,10 @@
     <t>Transistion "splashcreen"</t>
   </si>
   <si>
-    <t>Tester des mix pour les graph, tester le nouveau graph</t>
-  </si>
-  <si>
-    <t>Tester quand même "My Name Is"</t>
-  </si>
-  <si>
-    <t>Regarder aussi l'explosion bizarre full combo, tester, bug au niveau de la disparition</t>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>Tester le son, particule moche : refaire, faire la transition vers la chart</t>
   </si>
 </sst>
 </file>
@@ -385,7 +376,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,19 +732,17 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -784,7 +773,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
@@ -794,12 +783,10 @@
       <c r="D8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
@@ -811,14 +798,12 @@
       <c r="D9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -826,13 +811,13 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -846,9 +831,7 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -876,10 +859,10 @@
         <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -962,7 +945,7 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -974,7 +957,7 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -1060,13 +1043,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1122,7 +1105,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1137,13 +1120,13 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1222,9 +1205,6 @@
       <c r="E37" s="1">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -1239,7 +1219,9 @@
       <c r="E38" s="1">
         <v>0</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -1299,37 +1281,31 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>48</v>
       </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>1000</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>52</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -1338,13 +1314,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -1353,7 +1329,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>51</v>
@@ -1368,7 +1344,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>51</v>
@@ -1383,24 +1359,27 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2000</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="D50" s="2"/>
       <c r="E50" s="1">
         <v>0</v>
       </c>
@@ -1408,10 +1387,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -1420,13 +1399,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -1435,13 +1411,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -1450,47 +1426,52 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>6000</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>7000</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C57" s="2"/>
       <c r="E57" s="1">
@@ -1499,11 +1480,8 @@
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>61</v>
-      </c>
       <c r="B58" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C58" s="2"/>
       <c r="E58" s="1">
@@ -1513,10 +1491,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" s="2"/>
       <c r="E59" s="1">
@@ -1526,12 +1504,25 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E61" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Build 204] [Update] Transistion wheelsong faite (un poil moche) Transistion dans le MainMenu.cs en cours
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -219,12 +219,6 @@
     <t>Medals</t>
   </si>
   <si>
-    <t>Baisser le volume doucement transition</t>
-  </si>
-  <si>
-    <t>Correction de la detection de cross, sons (partout), correction son wheel song</t>
-  </si>
-  <si>
     <t>Option "Display"</t>
   </si>
   <si>
@@ -285,7 +279,24 @@
     <t>Cache</t>
   </si>
   <si>
-    <t>Tester le son, particule moche : refaire, faire la transition vers la chart</t>
+    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code)</t>
+  </si>
+  <si>
+    <t>Baisser le volume doucement transition, Remttre les petits labels avant la remise de l'update MainMenu, faire une animation au passage de la souris sur le sous choix, faire la transition</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Son lancement : Pas assez fort et trop court, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Particle améliorable</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -680,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>24</v>
@@ -803,37 +814,37 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="C11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>300</v>
       </c>
@@ -843,11 +854,11 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1">
-        <v>0</v>
+      <c r="E12" s="10">
+        <v>0.7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,10 +870,10 @@
         <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,7 +932,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -945,7 +956,7 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -957,7 +968,7 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -1043,13 +1054,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,7 +1116,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1120,13 +1131,13 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1220,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1265,40 +1276,39 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -1390,7 +1400,7 @@
         <v>2000</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -1517,10 +1527,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
[build 400] [Update générale]
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
   <si>
     <t>Stepchart</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Spé</t>
   </si>
   <si>
-    <t>WHeelsong</t>
-  </si>
-  <si>
     <t>Display best scores</t>
   </si>
   <si>
@@ -246,12 +243,6 @@
     <t>Ecran d'init de profile</t>
   </si>
   <si>
-    <t>Trucs à rajouter par la suite</t>
-  </si>
-  <si>
-    <t>stand by</t>
-  </si>
-  <si>
     <t>Première phase de test privée</t>
   </si>
   <si>
@@ -279,10 +270,19 @@
     <t>Cache</t>
   </si>
   <si>
-    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code)</t>
-  </si>
-  <si>
-    <t>Baisser le volume doucement transition, Remttre les petits labels avant la remise de l'update MainMenu, faire une animation au passage de la souris sur le sous choix, faire la transition</t>
+    <t>Display records</t>
+  </si>
+  <si>
+    <t>Tester la souris (faut une vraie souris erf)</t>
+  </si>
+  <si>
+    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), peut être faire en sorte de voir les medailles dans la songlist ?</t>
+  </si>
+  <si>
+    <t>Verifier si la concurrence marche bien… (Quand la création de profil sera ok)</t>
+  </si>
+  <si>
+    <t>Le "cœur" a été desinné = A améliorer. Faire le cube team blui qui passe et qui s'écrase avec d'autres cubes, puis l'init des profiles</t>
   </si>
   <si>
     <r>
@@ -295,15 +295,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Particle améliorable</t>
+      <t>Particle  de fond améliorable</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,7 +477,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -512,7 +511,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -688,14 +686,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
@@ -705,14 +703,14 @@
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -730,19 +728,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -755,7 +753,7 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>200</v>
       </c>
@@ -771,7 +769,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
@@ -784,7 +782,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
@@ -799,12 +797,12 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>24</v>
@@ -814,12 +812,12 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5">
@@ -827,7 +825,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -835,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E11" s="7">
         <v>0.99</v>
@@ -844,167 +842,172 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>300</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="E14" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
+      <c r="E16" s="8">
+        <v>1</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:6" ht="30">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
         <v>400</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
+      <c r="E18" s="8">
+        <v>1</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>500</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30">
       <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>600</v>
-      </c>
+    <row r="22" spans="1:6">
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>600</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6">
       <c r="B24" t="s">
         <v>30</v>
       </c>
@@ -1012,14 +1015,14 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="B25" t="s">
         <v>30</v>
       </c>
@@ -1027,231 +1030,231 @@
         <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>700</v>
-      </c>
+    <row r="26" spans="1:6">
       <c r="B26" t="s">
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>700</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="B29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
         <v>31</v>
       </c>
       <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>800</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>800</v>
-      </c>
-      <c r="B37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
       <c r="E39" s="1">
         <v>0</v>
       </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>64</v>
@@ -1261,103 +1264,103 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>900</v>
-      </c>
+    <row r="41" spans="1:6">
       <c r="B41" t="s">
         <v>20</v>
       </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>900</v>
+      </c>
       <c r="B42" t="s">
         <v>20</v>
       </c>
-      <c r="C42" t="s">
-        <v>68</v>
+      <c r="D42" t="s">
+        <v>8</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6">
       <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="60">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
         <v>1000</v>
       </c>
-      <c r="B45" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>24</v>
@@ -1367,12 +1370,12 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="B49" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>24</v>
@@ -1382,116 +1385,121 @@
       </c>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="B50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="B51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="C51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
         <v>2000</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="B52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
         <v>3000</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="B53" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
         <v>4000</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>5000</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
       </c>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>6000</v>
+      </c>
       <c r="B56" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
       </c>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57" spans="1:6">
+      <c r="B57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
         <v>7000</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C58" s="2"/>
       <c r="E58" s="1">
@@ -1499,12 +1507,9 @@
       </c>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
+    <row r="59" spans="1:6">
       <c r="B59" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C59" s="2"/>
       <c r="E59" s="1">
@@ -1512,12 +1517,12 @@
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C60" s="2"/>
       <c r="E60" s="1">
@@ -1525,14 +1530,27 @@
       </c>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" s="1">
+      <c r="E62" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1543,24 +1561,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Build 401] [Update] login et compte commencé
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
   <si>
     <t>Stepchart</t>
   </si>
@@ -99,9 +99,6 @@
     <t>SplashScreen</t>
   </si>
   <si>
-    <t>Creation de profil</t>
-  </si>
-  <si>
     <t>MainMenu</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Faire en sorte que InGameScript prenne 2 touches par bind</t>
   </si>
   <si>
-    <t>Ecran d'init de profile</t>
-  </si>
-  <si>
     <t>Première phase de test privée</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t>Mettre la config du globaloffset second + les touches dans un txt</t>
   </si>
   <si>
-    <t>Load profile</t>
-  </si>
-  <si>
     <t>Mode tapis + raccourci keyboard</t>
   </si>
   <si>
@@ -280,9 +271,6 @@
   </si>
   <si>
     <t>Verifier si la concurrence marche bien… (Quand la création de profil sera ok)</t>
-  </si>
-  <si>
-    <t>Le "cœur" a été desinné = A améliorer. Faire le cube team blui qui passe et qui s'écrase avec d'autres cubes, puis l'init des profiles</t>
   </si>
   <si>
     <r>
@@ -298,12 +286,33 @@
       <t>Particle  de fond améliorable</t>
     </r>
   </si>
+  <si>
+    <t>Ajouter l'écran de ranking</t>
+  </si>
+  <si>
+    <t>Init de profile</t>
+  </si>
+  <si>
+    <t>Team Blui</t>
+  </si>
+  <si>
+    <t>Nouveau profil</t>
+  </si>
+  <si>
+    <t>Profil existant</t>
+  </si>
+  <si>
+    <t>Le "cœur" a été desinné = A améliorer. Faire le cube team blui qui passe et qui s'écrase avec d'autres cubes</t>
+  </si>
+  <si>
+    <t>Retrouver un profil pas save</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +486,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -511,6 +521,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -686,14 +697,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
@@ -703,14 +714,14 @@
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -728,19 +739,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -753,7 +764,7 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -769,7 +780,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
@@ -782,7 +793,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
@@ -797,12 +808,12 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>24</v>
@@ -812,12 +823,12 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5">
@@ -825,7 +836,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -833,32 +844,32 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E11" s="7">
         <v>0.99</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>300</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -871,7 +882,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -883,10 +894,10 @@
         <v>0.95</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -899,35 +910,35 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="8">
         <v>1</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E17" s="7">
         <v>0.99</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>400</v>
       </c>
@@ -943,57 +954,63 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>500</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="30">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>26</v>
       </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
       <c r="E20" s="10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
+      <c r="C21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>600</v>
       </c>
@@ -1001,63 +1018,63 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>31</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="B25" t="s">
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
-      </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>700</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
@@ -1070,163 +1087,163 @@
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" t="s">
-        <v>41</v>
-      </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" t="s">
-        <v>45</v>
-      </c>
       <c r="E37" s="1">
         <v>0</v>
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>800</v>
       </c>
       <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
         <v>42</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
       </c>
       <c r="D38" t="s">
         <v>24</v>
@@ -1235,12 +1252,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -1249,37 +1266,37 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>20</v>
       </c>
       <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
         <v>62</v>
       </c>
-      <c r="D41" t="s">
-        <v>63</v>
-      </c>
       <c r="E41" s="1">
         <v>0</v>
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>900</v>
       </c>
@@ -1294,73 +1311,73 @@
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" ht="60">
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1000</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="B48" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>24</v>
@@ -1370,12 +1387,12 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>24</v>
@@ -1385,12 +1402,12 @@
       </c>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>24</v>
@@ -1400,12 +1417,12 @@
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="1">
@@ -1413,103 +1430,106 @@
       </c>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>2000</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
+      <c r="B53" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>3000</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
+      <c r="B54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>4000</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55">
-        <v>5000</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
       </c>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
       </c>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>6000</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
       </c>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>7000</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="E58" s="1">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="B59" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C59" s="2"/>
       <c r="E59" s="1">
@@ -1517,12 +1537,9 @@
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C60" s="2"/>
       <c r="E60" s="1">
@@ -1530,12 +1547,12 @@
       </c>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C61" s="2"/>
       <c r="E61" s="1">
@@ -1543,14 +1560,27 @@
       </c>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E62" s="1">
+      <c r="E63" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1561,24 +1591,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Build 402] [Update] [Not compiled] Progression légère sur le cube a tester Ecriture du scenar d'intro
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>Stepchart</t>
   </si>
@@ -302,10 +302,37 @@
     <t>Profil existant</t>
   </si>
   <si>
-    <t>Le "cœur" a été desinné = A améliorer. Faire le cube team blui qui passe et qui s'écrase avec d'autres cubes</t>
-  </si>
-  <si>
     <t>Retrouver un profil pas save</t>
+  </si>
+  <si>
+    <t>Penser à faire une option "Récupérer tous les 20 profils, Récuperer tous les profils"</t>
+  </si>
+  <si>
+    <t>Ecriture du scnéario d'intro fini</t>
+  </si>
+  <si>
+    <t>Le "cœur" a été desinné = A améliorer. Tester le cube Blui. Faire d'autres cubes qui viennent s'écraser à tour de role</t>
+  </si>
+  <si>
+    <t>Date approx</t>
+  </si>
+  <si>
+    <t>Continuer demain à faire le squelette script et la GUI au moins</t>
+  </si>
+  <si>
+    <t>A faire surement ce week end !</t>
+  </si>
+  <si>
+    <t>debut decembre</t>
+  </si>
+  <si>
+    <t>Fin de l'année</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Mi-novembre / Fin novembre</t>
   </si>
 </sst>
 </file>
@@ -348,7 +375,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +394,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -380,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -397,6 +430,18 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,14 +757,15 @@
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -738,8 +784,11 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
@@ -751,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -764,7 +813,7 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -780,7 +829,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
@@ -793,7 +842,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
@@ -808,7 +857,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>0</v>
       </c>
@@ -823,7 +872,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
@@ -836,7 +885,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -853,7 +902,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>300</v>
       </c>
@@ -869,7 +918,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -882,7 +931,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -897,7 +946,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -910,7 +959,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
@@ -923,7 +972,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
@@ -938,7 +987,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>400</v>
       </c>
@@ -954,77 +1003,92 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>500</v>
       </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>600</v>
-      </c>
+      <c r="G22" s="14">
+        <v>41189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="G23" s="14">
+        <v>41193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>29</v>
       </c>
@@ -1032,14 +1096,17 @@
         <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="14">
+        <v>41194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>29</v>
       </c>
@@ -1047,58 +1114,68 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="14">
+        <v>41195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>600</v>
+      </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="14">
+        <v>41196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="14">
+        <v>41202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>700</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>73</v>
+      <c r="D28" t="s">
+        <v>36</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -1106,14 +1183,14 @@
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>35</v>
       </c>
@@ -1121,14 +1198,14 @@
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>35</v>
       </c>
@@ -1136,14 +1213,14 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>35</v>
       </c>
@@ -1151,14 +1228,16 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>35</v>
       </c>
@@ -1166,16 +1245,14 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>35</v>
       </c>
@@ -1183,14 +1260,16 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>35</v>
       </c>
@@ -1198,46 +1277,46 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D36" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="D36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="21">
         <v>0</v>
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="1">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="13">
         <v>0</v>
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
@@ -1251,8 +1330,11 @@
       <c r="E38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1351,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -1281,7 +1363,7 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>20</v>
       </c>
@@ -1296,9 +1378,9 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -1310,8 +1392,11 @@
         <v>0</v>
       </c>
       <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>20</v>
       </c>
@@ -1322,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>80</v>
       </c>
@@ -1331,56 +1416,61 @@
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>900</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D45" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1000</v>
       </c>
       <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="19"/>
+      <c r="G47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -1389,7 +1479,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>49</v>
@@ -1404,7 +1494,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>49</v>
@@ -1419,12 +1509,14 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E51" s="1">
         <v>0</v>
       </c>
@@ -1432,12 +1524,12 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="1">
         <v>0</v>
       </c>
@@ -1448,34 +1540,35 @@
         <v>2000</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="17"/>
+      <c r="B54" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>3000</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18">
+        <v>0</v>
+      </c>
+      <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -1484,13 +1577,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -1499,47 +1592,52 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>6000</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="1">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>7000</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C60" s="2"/>
       <c r="E60" s="1">
@@ -1548,11 +1646,8 @@
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>59</v>
-      </c>
       <c r="B61" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" s="2"/>
       <c r="E61" s="1">
@@ -1562,10 +1657,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" s="2"/>
       <c r="E62" s="1">
@@ -1575,12 +1670,25 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E64" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Build 404] [Update] Continuité de l'intro, loin d'être fini Ajout des 4 flèches + de la particule d'explode
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
   <si>
     <t>Stepchart</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>Mode "rapide"</t>
-  </si>
-  <si>
-    <t>Mettre la config du globaloffset second + les touches dans un txt</t>
   </si>
   <si>
     <t>Mode tapis + raccourci keyboard</t>
@@ -299,30 +296,15 @@
     <t>Nouveau profil</t>
   </si>
   <si>
-    <t>Profil existant</t>
-  </si>
-  <si>
     <t>Retrouver un profil pas save</t>
   </si>
   <si>
     <t>Penser à faire une option "Récupérer tous les 20 profils, Récuperer tous les profils"</t>
   </si>
   <si>
-    <t>Ecriture du scnéario d'intro fini</t>
-  </si>
-  <si>
-    <t>Le "cœur" a été desinné = A améliorer. Tester le cube Blui. Faire d'autres cubes qui viennent s'écraser à tour de role</t>
-  </si>
-  <si>
     <t>Date approx</t>
   </si>
   <si>
-    <t>Continuer demain à faire le squelette script et la GUI au moins</t>
-  </si>
-  <si>
-    <t>A faire surement ce week end !</t>
-  </si>
-  <si>
     <t>debut decembre</t>
   </si>
   <si>
@@ -333,6 +315,18 @@
   </si>
   <si>
     <t>Mi-novembre / Fin novembre</t>
+  </si>
+  <si>
+    <t>Ok jusqu'à l'explosion de la particule question 1</t>
+  </si>
+  <si>
+    <t>Entrée dans le jeu et trans</t>
+  </si>
+  <si>
+    <t>Mettre la config du globaloffset second + les touches dans un txt + petit debugging général</t>
+  </si>
+  <si>
+    <t>Faire d'autres cubes qui viennent s'écraser à tour de role</t>
   </si>
 </sst>
 </file>
@@ -413,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +436,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +783,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -893,13 +891,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="7">
         <v>0.99</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -943,7 +941,7 @@
         <v>0.95</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,13 +976,13 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="7">
         <v>0.99</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,22 +1001,22 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="G19" s="23">
+        <v>41189</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1026,31 +1024,31 @@
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E20" s="8">
         <v>1</v>
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="10">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="3" t="s">
         <v>96</v>
+      </c>
+      <c r="G21" s="22">
+        <v>41187</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,68 +1059,62 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="G22" s="14">
-        <v>41189</v>
+        <v>41192</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="1">
-        <v>0</v>
+      <c r="E23" s="8">
+        <v>1</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="14">
-        <v>41193</v>
-      </c>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="1">
-        <v>0</v>
+      <c r="E24" s="8">
+        <v>1</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="14">
-        <v>41194</v>
-      </c>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="1">
-        <v>0</v>
+      <c r="E25" s="8">
+        <v>1</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="14">
-        <v>41195</v>
-      </c>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1145,7 +1137,7 @@
         <v>41196</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>73</v>
@@ -1154,7 +1146,7 @@
       <c r="D27" s="17"/>
       <c r="E27" s="18"/>
       <c r="F27" s="19" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="G27" s="14">
         <v>41202</v>
@@ -1228,7 +1220,7 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -1266,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,7 +1299,7 @@
         <v>24</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E37" s="13">
         <v>0</v>
@@ -1331,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1393,7 +1385,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1409,7 +1401,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -1440,13 +1432,13 @@
         <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1459,7 +1451,7 @@
       <c r="E47" s="18"/>
       <c r="F47" s="19"/>
       <c r="G47" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,7 +1536,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -1554,7 +1546,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>

</xml_diff>

<commit_message>
[Build 405] [Maj Planning]
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>Stepchart</t>
   </si>
@@ -323,10 +323,16 @@
     <t>Entrée dans le jeu et trans</t>
   </si>
   <si>
-    <t>Mettre la config du globaloffset second + les touches dans un txt + petit debugging général</t>
-  </si>
-  <si>
     <t>Faire d'autres cubes qui viennent s'écraser à tour de role</t>
+  </si>
+  <si>
+    <t>5 au 7 octobre</t>
+  </si>
+  <si>
+    <t>Faire un petit effet de particule (explosion), un scale du gros cube comme un heartbeat et un zoom</t>
+  </si>
+  <si>
+    <t>Mettre la config du globaloffset second (assez bidon) + les touches dans un txt (assez bidon avec TryParse) + petit debugging général</t>
   </si>
 </sst>
 </file>
@@ -743,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,10 +1019,10 @@
         <v>0.7</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="G19" s="23">
-        <v>41189</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1048,10 +1054,10 @@
         <v>96</v>
       </c>
       <c r="G21" s="22">
-        <v>41187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>500</v>
       </c>
@@ -1063,6 +1069,9 @@
       </c>
       <c r="E22" s="1">
         <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="G22" s="14">
         <v>41192</v>
@@ -1146,7 +1155,7 @@
       <c r="D27" s="17"/>
       <c r="E27" s="18"/>
       <c r="F27" s="19" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G27" s="14">
         <v>41202</v>

</xml_diff>

<commit_message>
[Build 500] [Update] Intro finie. Corriger le texte et le zoom de fin est améliorable
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
   <si>
     <t>Stepchart</t>
   </si>
@@ -317,29 +317,23 @@
     <t>Mi-novembre / Fin novembre</t>
   </si>
   <si>
-    <t>Ok jusqu'à l'explosion de la particule question 1</t>
-  </si>
-  <si>
     <t>Entrée dans le jeu et trans</t>
   </si>
   <si>
     <t>Faire d'autres cubes qui viennent s'écraser à tour de role</t>
   </si>
   <si>
-    <t>5 au 7 octobre</t>
-  </si>
-  <si>
-    <t>Faire un petit effet de particule (explosion), un scale du gros cube comme un heartbeat et un zoom</t>
-  </si>
-  <si>
     <t>Mettre la config du globaloffset second (assez bidon) + les touches dans un txt (assez bidon avec TryParse) + petit debugging général</t>
+  </si>
+  <si>
+    <t>Améliorable l'effet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,13 +357,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -428,7 +415,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -749,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,13 +833,13 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="5">
@@ -862,13 +848,13 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="5">
@@ -1019,10 +1005,10 @@
         <v>0.7</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="G19" s="22">
+        <v>41187</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1041,41 +1027,37 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="22">
-        <v>41186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="4"/>
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>500</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
+      <c r="C22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5">
+        <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="14">
-        <v>41192</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -1091,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -1107,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="14"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -1123,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1142,23 +1124,23 @@
         <v>0</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
+        <v>41192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="13">
         <v>41196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" s="14">
-        <v>41202</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1295,22 +1277,22 @@
       <c r="D36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>0</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="12">
         <v>0</v>
       </c>
       <c r="F37" s="3"/>
@@ -1421,14 +1403,14 @@
       <c r="A45">
         <v>900</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="16">
+      <c r="D45" s="14"/>
+      <c r="E45" s="15">
         <v>0</v>
       </c>
       <c r="F45" s="3"/>
@@ -1451,14 +1433,14 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="19"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="18"/>
       <c r="G47" t="s">
         <v>93</v>
       </c>
@@ -1553,16 +1535,16 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="20" t="s">
+      <c r="A54" s="16"/>
+      <c r="B54" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="18">
-        <v>0</v>
-      </c>
-      <c r="F54" s="19"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="17">
+        <v>0</v>
+      </c>
+      <c r="F54" s="18"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">

</xml_diff>

<commit_message>
[Build 600] [Update] Première version stable à débugger ce week end. Si possible de faire le startNumber qui marche d'ici ce week end = cool.
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
   <si>
     <t>Stepchart</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Corriger les bugs des mines avec</t>
   </si>
   <si>
-    <t>Faire en sorte que InGameScript prenne 2 touches par bind</t>
-  </si>
-  <si>
     <t>Première phase de test privée</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
   </si>
   <si>
     <t>Tester la souris (faut une vraie souris erf)</t>
-  </si>
-  <si>
-    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), peut être faire en sorte de voir les medailles dans la songlist ?</t>
   </si>
   <si>
     <t>Verifier si la concurrence marche bien… (Quand la création de profil sera ok)</t>
@@ -320,13 +314,13 @@
     <t>Entrée dans le jeu et trans</t>
   </si>
   <si>
-    <t>Faire d'autres cubes qui viennent s'écraser à tour de role</t>
-  </si>
-  <si>
-    <t>Mettre la config du globaloffset second (assez bidon) + les touches dans un txt (assez bidon avec TryParse) + petit debugging général</t>
-  </si>
-  <si>
     <t>Améliorable l'effet</t>
+  </si>
+  <si>
+    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), augmenter l'explosion lors de l'impact (chart), faire en sorte que l'echap débouche sur le mainmenu déjà press start, peut être faire en sorte de voir les medailles dans la songlist ?</t>
+  </si>
+  <si>
+    <t>petit debugging général + regler le "startNumber" songlist</t>
   </si>
 </sst>
 </file>
@@ -735,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -883,13 +877,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="7">
         <v>0.99</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -933,7 +927,7 @@
         <v>0.95</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,13 +962,13 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" s="7">
         <v>0.99</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -994,32 +988,28 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="22">
-        <v>41187</v>
-      </c>
+      <c r="C19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" s="8">
         <v>1</v>
@@ -1031,7 +1021,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5">
@@ -1048,14 +1038,14 @@
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G22" s="13"/>
     </row>
@@ -1111,36 +1101,34 @@
       <c r="A26">
         <v>600</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
+      <c r="E26" s="5">
+        <v>1</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="13">
-        <v>41192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="17"/>
       <c r="F27" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G27" s="13">
-        <v>41196</v>
+        <v>41189</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1196,7 +1184,7 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1211,14 +1199,12 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -1249,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1290,7 +1276,7 @@
         <v>24</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E37" s="12">
         <v>0</v>
@@ -1314,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1376,7 +1362,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1392,7 +1378,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -1415,7 +1401,7 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1000</v>
       </c>
@@ -1423,13 +1409,13 @@
         <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1442,7 +1428,7 @@
       <c r="E47" s="17"/>
       <c r="F47" s="18"/>
       <c r="G47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,7 +1513,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -1537,7 +1523,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
       <c r="B54" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>

</xml_diff>

<commit_message>
[Build 601][Update] For release
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="128">
   <si>
     <t>Stepchart</t>
   </si>
@@ -322,12 +322,102 @@
   <si>
     <t>petit debugging général + regler le "startNumber" songlist</t>
   </si>
+  <si>
+    <t>Alpha test, retours</t>
+  </si>
+  <si>
+    <t>Fautes d'orthographe</t>
+  </si>
+  <si>
+    <t>Quand la musique commence, si la chart est pile sur le 0, ça freeze et ça n'avance pas.</t>
+  </si>
+  <si>
+    <t>Seriosité</t>
+  </si>
+  <si>
+    <t>Faible</t>
+  </si>
+  <si>
+    <t>Grave</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Moi-même</t>
+  </si>
+  <si>
+    <t>Le speedmod revient à 2 si nouvelle song</t>
+  </si>
+  <si>
+    <t>Passer le texte rapidement</t>
+  </si>
+  <si>
+    <t>Indiquer "appuyez sur entrée"</t>
+  </si>
+  <si>
+    <t>Possible de mettre aucun pseudo</t>
+  </si>
+  <si>
+    <t>Moyen</t>
+  </si>
+  <si>
+    <t>Ca brille trop</t>
+  </si>
+  <si>
+    <t>On confond les rouges et les mines</t>
+  </si>
+  <si>
+    <t>Trop petit</t>
+  </si>
+  <si>
+    <t>Différence entre roll et freeze bof</t>
+  </si>
+  <si>
+    <t>Quitter quand on joue</t>
+  </si>
+  <si>
+    <t>Trop tot ou trop tard pas assez visible</t>
+  </si>
+  <si>
+    <t>24th en turquoise</t>
+  </si>
+  <si>
+    <t>Aucun</t>
+  </si>
+  <si>
+    <t>Musique stressante</t>
+  </si>
+  <si>
+    <t>Rentrer directement la valeur du BPM</t>
+  </si>
+  <si>
+    <t>NayKid</t>
+  </si>
+  <si>
+    <t>Faire le "bump" quand on appuie sur une touche</t>
+  </si>
+  <si>
+    <t>A mettre dans lesoptions</t>
+  </si>
+  <si>
+    <t>zoom dans les options ?</t>
+  </si>
+  <si>
+    <t>mettre une petite loupiote</t>
+  </si>
+  <si>
+    <t>Faire une option pour choisir</t>
+  </si>
+  <si>
+    <t>Permettre de changer le speedmod/skin à l'écran de fail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +441,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,6 +542,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,6 +569,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="smile"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1057275" y="20393025"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,6 +933,7 @@
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="61.85546875" customWidth="1"/>
     <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1661,9 +1853,377 @@
         <v>0</v>
       </c>
     </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" t="s">
+        <v>102</v>
+      </c>
+      <c r="D73" s="26"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C74" t="s">
+        <v>102</v>
+      </c>
+      <c r="D74" s="26"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" s="26"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" s="26"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>121</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D79" s="26"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>121</v>
+      </c>
+      <c r="B80" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D80" s="25"/>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>121</v>
+      </c>
+      <c r="B82" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D82" s="25"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>121</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C83" t="s">
+        <v>118</v>
+      </c>
+      <c r="D83" s="26"/>
+    </row>
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>121</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C84" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D84" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+      <c r="B85" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D85" s="26"/>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>104</v>
+      </c>
+      <c r="B86" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D86" s="25"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="26"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="25"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="26"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="25"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="26"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="25"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="26"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="26"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="26"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="26"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="27"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="23"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="23"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="23"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="23"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="23"/>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="23"/>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="23"/>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="23"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="23"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="23"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="23"/>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="23"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="23"/>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="23"/>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="23"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="23"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="23"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="23"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="23"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="23"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="23"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="23"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="23"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="23"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="23"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="23"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="23"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="23"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="23"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="23"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="23"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="23"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="23"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="23"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="23"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="23"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="23"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="23"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[Update] [Build 601] Correction des bugs facilement resolvable repportés lors de l'alpha test
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
   <si>
     <t>Stepchart</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Audio</t>
-  </si>
-  <si>
-    <t>Video ??</t>
   </si>
   <si>
     <t>Mine</t>
@@ -317,12 +314,6 @@
     <t>Améliorable l'effet</t>
   </si>
   <si>
-    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), augmenter l'explosion lors de l'impact (chart), faire en sorte que l'echap débouche sur le mainmenu déjà press start, peut être faire en sorte de voir les medailles dans la songlist ?</t>
-  </si>
-  <si>
-    <t>petit debugging général + regler le "startNumber" songlist</t>
-  </si>
-  <si>
     <t>Alpha test, retours</t>
   </si>
   <si>
@@ -411,6 +402,45 @@
   </si>
   <si>
     <t>Permettre de changer le speedmod/skin à l'écran de fail</t>
+  </si>
+  <si>
+    <t>Facilité à résoudre</t>
+  </si>
+  <si>
+    <t>Facile</t>
+  </si>
+  <si>
+    <t>Difficile</t>
+  </si>
+  <si>
+    <t>Moyen/Facile</t>
+  </si>
+  <si>
+    <t>Moyen/Difficile</t>
+  </si>
+  <si>
+    <t>facile</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Moyen/difficile</t>
+  </si>
+  <si>
+    <t>A faire quand je ferai le panneau d'option</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Activer / Desactiver le bloom</t>
+  </si>
+  <si>
+    <t>Mettre Speedmod ou BPM dans les options</t>
+  </si>
+  <si>
+    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), augmenter l'explosion lors de l'impact (chart), faire en sorte que l'echap débouche sur le mainmenu déjà press start, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
   </si>
 </sst>
 </file>
@@ -465,14 +495,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +525,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -510,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -545,7 +579,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
@@ -554,7 +587,32 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -920,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +1001,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -961,7 +1019,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -970,7 +1028,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -1038,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>24</v>
@@ -1053,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5">
@@ -1069,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="7">
         <v>0.99</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1119,7 +1177,7 @@
         <v>0.95</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1154,13 +1212,13 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="7">
         <v>0.99</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1184,7 +1242,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="5">
@@ -1198,10 +1256,10 @@
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="8">
         <v>1</v>
@@ -1213,7 +1271,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5">
@@ -1230,14 +1288,14 @@
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22" s="13"/>
     </row>
@@ -1311,14 +1369,12 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="F27" s="18"/>
       <c r="G27" s="13">
         <v>41189</v>
       </c>
@@ -1351,7 +1407,9 @@
       <c r="E29" s="1">
         <v>0</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -1369,16 +1427,16 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="20">
         <v>0</v>
       </c>
       <c r="F31" s="3"/>
@@ -1391,7 +1449,7 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -1427,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1446,29 +1504,31 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="20">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3"/>
+      <c r="D36" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E37" s="12">
         <v>0</v>
@@ -1492,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1500,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -1509,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -1529,10 +1589,10 @@
         <v>20</v>
       </c>
       <c r="C41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" t="s">
         <v>61</v>
-      </c>
-      <c r="D41" t="s">
-        <v>62</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -1554,7 +1614,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1562,7 +1622,7 @@
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -1570,7 +1630,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -1582,10 +1642,10 @@
         <v>900</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="15">
@@ -1593,34 +1653,34 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1000</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
       <c r="E47" s="17"/>
       <c r="F47" s="18"/>
       <c r="G47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,7 +1688,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>30</v>
@@ -1643,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>24</v>
@@ -1658,7 +1718,7 @@
         <v>20</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>24</v>
@@ -1673,7 +1733,7 @@
         <v>27</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>24</v>
@@ -1688,7 +1748,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="1">
@@ -1705,7 +1765,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -1715,7 +1775,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
       <c r="B54" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
@@ -1729,7 +1789,7 @@
         <v>3000</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -1744,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -1774,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -1786,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -1808,7 +1868,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" s="2"/>
       <c r="E61" s="1">
@@ -1818,10 +1878,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" s="2"/>
       <c r="E62" s="1">
@@ -1831,10 +1891,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C63" s="2"/>
       <c r="E63" s="1">
@@ -1844,264 +1904,323 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E64" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" t="s">
         <v>98</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B70" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="B70" s="23" t="s">
+      <c r="C73" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C70" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="D73" s="32"/>
+      <c r="E73" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="C74" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D74" s="29"/>
+      <c r="E74" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D75" s="36"/>
+      <c r="E75" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="25"/>
+      <c r="E77" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D79" s="25"/>
+      <c r="E79" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C80" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C71" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>105</v>
-      </c>
-      <c r="B72" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>121</v>
-      </c>
-      <c r="B73" s="23" t="s">
+      <c r="D80" s="38"/>
+      <c r="E80" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>118</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C73" t="s">
-        <v>102</v>
-      </c>
-      <c r="D73" s="26"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>121</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C74" t="s">
-        <v>102</v>
-      </c>
-      <c r="D74" s="26"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>121</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>121</v>
-      </c>
-      <c r="B76" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C76" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D76" s="25" t="s">
+      <c r="D81" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E81" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C82" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="38"/>
+      <c r="E82" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C83" t="s">
+        <v>115</v>
+      </c>
+      <c r="D83" s="25"/>
+      <c r="E83" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>118</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" s="24" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>121</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C77" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D77" s="26"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>121</v>
-      </c>
-      <c r="B78" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D78" s="25" t="s">
+      <c r="E84" t="s">
+        <v>127</v>
+      </c>
+      <c r="F84" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" s="36"/>
+      <c r="E85" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="23" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>121</v>
-      </c>
-      <c r="B79" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D79" s="26"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>121</v>
-      </c>
-      <c r="B80" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D80" s="25"/>
-    </row>
-    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>121</v>
-      </c>
-      <c r="B81" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C81" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>121</v>
-      </c>
-      <c r="B82" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C82" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D82" s="25"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>121</v>
-      </c>
-      <c r="B83" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C83" t="s">
-        <v>118</v>
-      </c>
-      <c r="D83" s="26"/>
-    </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>121</v>
-      </c>
-      <c r="B84" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C84" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D84" s="25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>104</v>
-      </c>
-      <c r="B85" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="C85" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D85" s="26"/>
-    </row>
-    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>104</v>
-      </c>
-      <c r="B86" s="23" t="s">
-        <v>127</v>
-      </c>
       <c r="C86" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D86" s="25"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="26"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="25"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="26"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="25"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="26"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="25"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="26"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="26"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="26"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="26"/>
+        <v>99</v>
+      </c>
+      <c r="D86" s="24"/>
+      <c r="E86" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D87" s="25"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D88" s="24"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="25"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D90" s="24"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D91" s="25"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D92" s="24"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D93" s="25"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="25"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="25"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D96" s="25"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="27"/>
+      <c r="D97" s="26"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="23"/>

</xml_diff>

<commit_message>
[Build b602] [Update] Correction et verification des bugs
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="147">
   <si>
     <t>Stepchart</t>
   </si>
@@ -441,6 +441,33 @@
   </si>
   <si>
     <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), augmenter l'explosion lors de l'impact (chart), faire en sorte que l'echap débouche sur le mainmenu déjà press start, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
+  </si>
+  <si>
+    <t>Problème avec Fraps, plante au lancement de la chart</t>
+  </si>
+  <si>
+    <t>On peut appuyer sur les boutons Retry/Quit avant qu'ils n'apparaissent.</t>
+  </si>
+  <si>
+    <t>Ecran noir sur ???</t>
+  </si>
+  <si>
+    <t>Parfois le titre de la chanson reste sur le coté lors de la selection</t>
+  </si>
+  <si>
+    <t>La musique de base du menu ne s'efface pas complètement si on appuie vite sur "option"</t>
+  </si>
+  <si>
+    <t>Panneau d'option</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>On peut appuyer sur Play si aucun speedmod n'est choisi</t>
+  </si>
+  <si>
+    <t>Gravissime</t>
   </si>
 </sst>
 </file>
@@ -500,7 +527,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,12 +549,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,27 +614,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E85" sqref="A85:E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,47 +1962,47 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="37" t="s">
+      <c r="C71" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D71" s="33"/>
-      <c r="E71" s="33" t="s">
+      <c r="D71" s="4"/>
+      <c r="E71" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B72" s="34" t="s">
+      <c r="B72" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C72" s="33" t="s">
+      <c r="C72" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D72" s="33"/>
-      <c r="E72" s="33" t="s">
+      <c r="D72" s="4"/>
+      <c r="E72" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
+      <c r="A73" s="10" t="s">
         <v>118</v>
       </c>
       <c r="B73" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="30" t="s">
+      <c r="C73" s="10" t="s">
         <v>99</v>
       </c>
       <c r="D73" s="32"/>
-      <c r="E73" s="30" t="s">
+      <c r="E73" s="10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1999,17 +2022,17 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="34" t="s">
+      <c r="B75" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C75" s="35" t="s">
+      <c r="C75" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D75" s="36"/>
-      <c r="E75" s="33" t="s">
+      <c r="D75" s="35"/>
+      <c r="E75" s="4" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2078,17 +2101,17 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="33" t="s">
+      <c r="A80" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B80" s="34" t="s">
+      <c r="B80" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C80" s="37" t="s">
+      <c r="C80" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D80" s="38"/>
-      <c r="E80" s="33" t="s">
+      <c r="D80" s="37"/>
+      <c r="E80" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2102,7 +2125,7 @@
       <c r="C81" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="39" t="s">
+      <c r="D81" s="30" t="s">
         <v>122</v>
       </c>
       <c r="E81" t="s">
@@ -2110,17 +2133,17 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+      <c r="A82" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="34" t="s">
+      <c r="B82" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C82" s="37" t="s">
+      <c r="C82" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D82" s="38"/>
-      <c r="E82" s="33" t="s">
+      <c r="D82" s="37"/>
+      <c r="E82" s="4" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2160,17 +2183,17 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="33" t="s">
+      <c r="A85" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="34" t="s">
+      <c r="B85" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="C85" s="35" t="s">
+      <c r="C85" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D85" s="36"/>
-      <c r="E85" s="33" t="s">
+      <c r="D85" s="35"/>
+      <c r="E85" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2189,37 +2212,112 @@
         <v>132</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
       <c r="D87" s="25"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D88" s="24"/>
+      <c r="E87" t="s">
+        <v>107</v>
+      </c>
+      <c r="F87" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B88" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C88" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D88" s="37"/>
+      <c r="E88" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C89" s="38"/>
       <c r="D89" s="25"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C90" s="38" t="s">
+        <v>100</v>
+      </c>
       <c r="D90" s="24"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D91" s="25"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D92" s="24"/>
+      <c r="E90" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D91" s="35"/>
+      <c r="E91" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B92" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C92" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D92" s="37"/>
+      <c r="E92" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="3"/>
       <c r="D93" s="25"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="3"/>
       <c r="D94" s="25"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="3"/>
       <c r="D95" s="25"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="3"/>
       <c r="D96" s="25"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="3"/>
       <c r="D97" s="26"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[build 604] [Update] Ajout d'un changement speedmod/bpm dans les options de song
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="148">
   <si>
     <t>Stepchart</t>
   </si>
@@ -416,9 +416,6 @@
     <t>Moyen/Facile</t>
   </si>
   <si>
-    <t>Moyen/Difficile</t>
-  </si>
-  <si>
     <t>facile</t>
   </si>
   <si>
@@ -428,9 +425,6 @@
     <t>Moyen/difficile</t>
   </si>
   <si>
-    <t>A faire quand je ferai le panneau d'option</t>
-  </si>
-  <si>
     <t>Video</t>
   </si>
   <si>
@@ -471,6 +465,12 @@
   </si>
   <si>
     <t>Les mines ne marchent pas</t>
+  </si>
+  <si>
+    <t>Pas reproductible</t>
+  </si>
+  <si>
+    <t>Faire une simple particule qui se play, besoin de tester</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +561,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -574,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -617,9 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -656,6 +659,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E93" sqref="A93:E93"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1552,13 +1564,13 @@
         <v>30</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E36" s="12">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1708,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1954,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>95</v>
       </c>
@@ -1965,7 +1977,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>101</v>
       </c>
@@ -1979,14 +1991,14 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B71" s="31" t="s">
+      <c r="B71" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="34" t="s">
+      <c r="C71" s="33" t="s">
         <v>100</v>
       </c>
       <c r="D71" s="4"/>
@@ -1994,11 +2006,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B72" s="31" t="s">
+      <c r="B72" s="30" t="s">
         <v>103</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -2009,52 +2021,52 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B73" s="29" t="s">
+      <c r="B73" s="28" t="s">
         <v>104</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D73" s="30"/>
+      <c r="D73" s="29"/>
       <c r="E73" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="38" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="39" t="s">
+      <c r="B74" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C74" s="38" t="s">
+      <c r="C74" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D74" s="42"/>
-      <c r="E74" s="38" t="s">
+      <c r="D74" s="41"/>
+      <c r="E74" s="37" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="31" t="s">
+      <c r="B75" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C75" s="32" t="s">
+      <c r="C75" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D75" s="33"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>118</v>
       </c>
@@ -2070,8 +2082,11 @@
       <c r="E76" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>118</v>
       </c>
@@ -2086,7 +2101,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>118</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>118</v>
       </c>
@@ -2118,51 +2133,54 @@
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B80" s="31" t="s">
+      <c r="B80" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C80" s="34" t="s">
+      <c r="C80" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D80" s="35"/>
+      <c r="D80" s="34"/>
       <c r="E80" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="B81" s="23" t="s">
+      <c r="B81" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="C81" s="27" t="s">
+      <c r="C81" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="28" t="s">
+      <c r="D81" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="E81" t="s">
-        <v>129</v>
+      <c r="E81" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F81" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C82" s="34" t="s">
+      <c r="C82" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D82" s="35"/>
+      <c r="D82" s="34"/>
       <c r="E82" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2177,57 +2195,54 @@
       </c>
       <c r="D83" s="25"/>
       <c r="E83" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="23" t="s">
+      <c r="B84" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="C84" s="27" t="s">
+      <c r="C84" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="D84" s="24" t="s">
+      <c r="D84" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="37" t="s">
         <v>127</v>
-      </c>
-      <c r="F84" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="31" t="s">
+      <c r="B85" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="C85" s="32" t="s">
+      <c r="C85" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D85" s="33"/>
+      <c r="D85" s="32"/>
       <c r="E85" s="4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="38" t="s">
+      <c r="A86" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B86" s="39" t="s">
+      <c r="B86" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="C86" s="40" t="s">
+      <c r="C86" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="D86" s="41"/>
-      <c r="E86" s="38" t="s">
-        <v>132</v>
+      <c r="D86" s="40"/>
+      <c r="E86" s="37" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2235,7 +2250,7 @@
         <v>118</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C87" t="s">
         <v>99</v>
@@ -2245,20 +2260,20 @@
         <v>107</v>
       </c>
       <c r="F87" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B88" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="C88" s="34" t="s">
+      <c r="B88" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D88" s="35"/>
+      <c r="D88" s="34"/>
       <c r="E88" s="4" t="s">
         <v>126</v>
       </c>
@@ -2268,9 +2283,9 @@
         <v>118</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C89" s="36"/>
+        <v>138</v>
+      </c>
+      <c r="C89" s="35"/>
       <c r="D89" s="25"/>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2278,27 +2293,30 @@
         <v>102</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C90" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C90" s="35" t="s">
         <v>100</v>
       </c>
       <c r="D90" s="24"/>
       <c r="E90" t="s">
-        <v>144</v>
+        <v>142</v>
+      </c>
+      <c r="F90" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B91" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="C91" s="34" t="s">
+      <c r="B91" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C91" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D91" s="33"/>
+      <c r="D91" s="32"/>
       <c r="E91" s="4" t="s">
         <v>107</v>
       </c>
@@ -2307,29 +2325,29 @@
       <c r="A92" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B92" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="C92" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="D92" s="35"/>
+      <c r="B92" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D92" s="34"/>
       <c r="E92" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="38" t="s">
+      <c r="A93" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="B93" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="C93" s="44" t="s">
+      <c r="B93" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D93" s="42"/>
-      <c r="E93" s="38" t="s">
+      <c r="D93" s="41"/>
+      <c r="E93" s="37" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Build 614] [Update] Ajout du squelette des options
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="131">
   <si>
     <t>Stepchart</t>
   </si>
@@ -240,20 +240,6 @@
     <t>Verifier si la concurrence marche bien… (Quand la création de profil sera ok)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Son lancement : Pas assez fort et trop court, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Particle  de fond améliorable</t>
-    </r>
-  </si>
-  <si>
     <t>Ajouter l'écran de ranking</t>
   </si>
   <si>
@@ -380,9 +366,6 @@
     <t>Profiles</t>
   </si>
   <si>
-    <t>nom, Start with, difficulté</t>
-  </si>
-  <si>
     <t>Ajouter quand une faute est fait droite</t>
   </si>
   <si>
@@ -398,15 +381,9 @@
     <t>Scene</t>
   </si>
   <si>
-    <t>Correction de la detection de cross, sons (partout), correction son wheel song, optim du mainmenu (code), mettre si un score est legit ou non, optim le graphique de song (comme au score screen), faire en sorte que l'echap débouche sur le mainmenu déjà press start, regler le "startNumber" songlist, créer les 5 packs de base, peut être faire en sorte de voir les medailles dans la songlist ?</t>
-  </si>
-  <si>
     <t>Terminée : Tester soi même la dernière build !</t>
   </si>
   <si>
-    <t>Avant le 21 octobre</t>
-  </si>
-  <si>
     <t>GlobalOffset, Vitesse molette, mode tapis, mode debug offbeat</t>
   </si>
   <si>
@@ -417,6 +394,21 @@
   </si>
   <si>
     <t>La GUI à faire, la transition</t>
+  </si>
+  <si>
+    <t>Correction de la detection de cross, sons (partout), optim du mainmenu (code), mettre si un score est legit ou non, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
+  </si>
+  <si>
+    <t>Tester, rajouter le bouton GUI, rajouter la gestion de l'erreur</t>
+  </si>
+  <si>
+    <t>Trouver un doubleur</t>
+  </si>
+  <si>
+    <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage, à faire plus tard ?</t>
+  </si>
+  <si>
+    <t>Particle  de fond améliorable</t>
   </si>
 </sst>
 </file>
@@ -478,7 +470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +495,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -516,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -536,7 +540,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -563,7 +566,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +977,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1068,21 +1077,21 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>74</v>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1189,24 +1198,24 @@
         <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="5">
         <v>0.8</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="22"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="8">
         <v>1</v>
@@ -1218,14 +1227,14 @@
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5">
         <v>1</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="21"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1235,14 +1244,14 @@
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G22" s="13"/>
     </row>
@@ -1315,41 +1324,37 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>125</v>
-      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="30">
+      <c r="D28" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="33">
         <v>0.5</v>
       </c>
-      <c r="F28" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" s="13">
-        <v>41203</v>
-      </c>
+      <c r="F28" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -1365,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1378,7 +1383,7 @@
       <c r="D30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="19">
         <v>0</v>
       </c>
       <c r="F30" s="3"/>
@@ -1397,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1408,13 +1413,13 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1440,18 +1445,18 @@
         <v>30</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E34" s="12">
         <v>0</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>30</v>
@@ -1463,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1474,7 +1479,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36" s="12">
         <v>0</v>
@@ -1498,56 +1503,56 @@
         <v>0</v>
       </c>
       <c r="G37" s="13">
-        <v>41217</v>
+        <v>41231</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="1">
-        <v>0</v>
+      <c r="E38" s="8">
+        <v>1</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="13">
-        <v>41224</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="30">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="G39" s="13">
-        <v>41231</v>
+        <v>41245</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
-        <v>118</v>
-      </c>
-      <c r="E40" s="1">
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="19">
         <v>0</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="13">
-        <v>41238</v>
-      </c>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
@@ -1559,7 +1564,7 @@
       <c r="D41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="19">
         <v>0</v>
       </c>
       <c r="F41" s="3"/>
@@ -1568,20 +1573,21 @@
       <c r="A42">
         <v>800</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="1">
-        <v>0</v>
+      <c r="E42" s="7">
+        <v>0.6</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="G42" s="13">
-        <v>41245</v>
+        <v>41252</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1595,10 +1601,13 @@
         <v>0</v>
       </c>
       <c r="G43" s="13">
-        <v>41252</v>
+        <v>41259</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>900</v>
+      </c>
       <c r="B44" t="s">
         <v>71</v>
       </c>
@@ -1606,32 +1615,32 @@
         <v>0</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G44" s="13">
-        <v>41259</v>
+        <v>41266</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>900</v>
-      </c>
-      <c r="B45" s="14" t="s">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="15">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="13">
-        <v>41266</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="D45" s="29"/>
+      <c r="E45" s="30">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1000</v>
       </c>
@@ -1645,21 +1654,21 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G46" s="13">
         <v>40914</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16" t="s">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="18"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -1743,7 +1752,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -1751,16 +1760,16 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="19" t="s">
+      <c r="A54" s="15"/>
+      <c r="B54" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="17">
-        <v>0</v>
-      </c>
-      <c r="F54" s="18"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="16">
+        <v>0</v>
+      </c>
+      <c r="F54" s="17"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -1893,284 +1902,284 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>90</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B71" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C71" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D71" s="24" t="s">
-        <v>100</v>
-      </c>
       <c r="E71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>99</v>
-      </c>
-      <c r="B72" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C72" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="25"/>
+        <v>98</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" s="24"/>
       <c r="E72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>99</v>
-      </c>
-      <c r="B73" s="23" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D73" s="24" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>99</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D74" s="25"/>
+        <v>87</v>
+      </c>
+      <c r="D74" s="24"/>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>99</v>
-      </c>
-      <c r="B75" s="23" t="s">
         <v>98</v>
       </c>
+      <c r="B75" s="22" t="s">
+        <v>97</v>
+      </c>
       <c r="C75" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="25"/>
+        <v>96</v>
+      </c>
+      <c r="D75" s="24"/>
       <c r="E75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" s="3"/>
-      <c r="D76" s="25"/>
+      <c r="D76" s="24"/>
       <c r="F76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77" s="24"/>
+      <c r="E77" t="s">
+        <v>108</v>
+      </c>
+      <c r="F77" t="s">
         <v>113</v>
-      </c>
-      <c r="C77" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D77" s="25"/>
-      <c r="E77" t="s">
-        <v>109</v>
-      </c>
-      <c r="F77" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C78" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D78" s="24"/>
+        <v>106</v>
+      </c>
+      <c r="C78" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="23"/>
       <c r="E78" t="s">
+        <v>108</v>
+      </c>
+      <c r="F78" t="s">
         <v>109</v>
-      </c>
-      <c r="F78" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" t="s">
+        <v>108</v>
+      </c>
+      <c r="D79" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="C79" t="s">
-        <v>109</v>
-      </c>
-      <c r="D79" s="26" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="23"/>
+      <c r="B80" s="22"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="23"/>
+      <c r="B81" s="22"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="23"/>
+      <c r="B82" s="22"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="23"/>
+      <c r="B83" s="22"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="23"/>
+      <c r="B84" s="22"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="23"/>
+      <c r="B85" s="22"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="23"/>
+      <c r="B86" s="22"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="23"/>
+      <c r="B87" s="22"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="23"/>
+      <c r="B88" s="22"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="23"/>
+      <c r="B89" s="22"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="23"/>
+      <c r="B90" s="22"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="23"/>
+      <c r="B91" s="22"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="23"/>
+      <c r="B92" s="22"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="23"/>
+      <c r="B93" s="22"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="23"/>
+      <c r="B94" s="22"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="23"/>
+      <c r="B95" s="22"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="23"/>
+      <c r="B96" s="22"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="23"/>
+      <c r="B97" s="22"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="23"/>
+      <c r="B98" s="22"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="23"/>
+      <c r="B99" s="22"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="23"/>
+      <c r="B100" s="22"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="23"/>
+      <c r="B101" s="22"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="23"/>
+      <c r="B102" s="22"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="23"/>
+      <c r="B103" s="22"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="23"/>
+      <c r="B104" s="22"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="23"/>
+      <c r="B105" s="22"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="23"/>
+      <c r="B106" s="22"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="23"/>
+      <c r="B107" s="22"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="23"/>
+      <c r="B108" s="22"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="23"/>
+      <c r="B109" s="22"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="23"/>
+      <c r="B110" s="22"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="23"/>
+      <c r="B111" s="22"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="23"/>
+      <c r="B112" s="22"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="23"/>
+      <c r="B113" s="22"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="23"/>
+      <c r="B114" s="22"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="23"/>
+      <c r="B115" s="22"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="23"/>
+      <c r="B116" s="22"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="23"/>
+      <c r="B117" s="22"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="23"/>
+      <c r="B118" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 615] [Update] Creation du cache Gestion du cache A tester
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -387,9 +387,6 @@
     <t>GlobalOffset, Vitesse molette, mode tapis, mode debug offbeat</t>
   </si>
   <si>
-    <t>Faire un objet "SongSerializable"</t>
-  </si>
-  <si>
     <t>Reload / Actualiser, Supprimer, reload à chaque redemarrage</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>Correction de la detection de cross, sons (partout), optim du mainmenu (code), mettre si un score est legit ou non, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
   </si>
   <si>
-    <t>Tester, rajouter le bouton GUI, rajouter la gestion de l'erreur</t>
-  </si>
-  <si>
     <t>Trouver un doubleur</t>
   </si>
   <si>
@@ -409,6 +403,12 @@
   </si>
   <si>
     <t>Particle  de fond améliorable</t>
+  </si>
+  <si>
+    <t>Tester, rajouter le bouton GUI, rajouter la gestion de l'erreur via un script à part</t>
+  </si>
+  <si>
+    <t>SongSerializable Ok : Il faut tester</t>
   </si>
 </sst>
 </file>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>0.5</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" s="13"/>
     </row>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G39" s="13">
         <v>41245</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>800</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>0.6</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G42" s="13">
         <v>41252</v>
@@ -1608,14 +1608,16 @@
       <c r="A44">
         <v>900</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E44" s="1">
-        <v>0</v>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7">
+        <v>0.9</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="G44" s="13">
         <v>41266</v>
@@ -1636,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G45" s="13"/>
     </row>
@@ -1654,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G46" s="13">
         <v>40914</v>

</xml_diff>

<commit_message>
[Build 618] [Update] Mise en place GUI pour General et Network
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -390,9 +390,6 @@
     <t>Reload / Actualiser, Supprimer, reload à chaque redemarrage</t>
   </si>
   <si>
-    <t>La GUI à faire, la transition</t>
-  </si>
-  <si>
     <t>Correction de la detection de cross, sons (partout), optim du mainmenu (code), mettre si un score est legit ou non, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>SongSerializable Ok : Il faut tester</t>
+  </si>
+  <si>
+    <t>Faire le bouton retour</t>
   </si>
 </sst>
 </file>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1349,10 +1349,10 @@
         <v>120</v>
       </c>
       <c r="E28" s="33">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G28" s="13"/>
     </row>
@@ -1374,16 +1374,16 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="12">
         <v>0</v>
       </c>
       <c r="F30" s="3"/>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G39" s="13">
         <v>41245</v>
@@ -1584,7 +1584,7 @@
         <v>0.6</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G42" s="13">
         <v>41252</v>
@@ -1617,7 +1617,7 @@
         <v>0.9</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G44" s="13">
         <v>41266</v>
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G45" s="13"/>
     </row>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G46" s="13">
         <v>40914</v>

</xml_diff>

<commit_message>
[Build 622] [Update] Fix Planning.xlsx Rajout d'un bouton pour changer de profile Modification dans le profileManager en conséquence
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="128">
   <si>
     <t>Stepchart</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Retrouver un profil pas save</t>
   </si>
   <si>
-    <t>Penser à faire une option "Récupérer tous les 20 profils, Récuperer tous les profils"</t>
-  </si>
-  <si>
     <t>Date approx</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
     <t>Pas reproduit</t>
   </si>
   <si>
-    <t>Activer / Desactiver le bloom, Activer / Desactiver flou</t>
-  </si>
-  <si>
     <t>Profiles</t>
   </si>
   <si>
@@ -375,21 +369,12 @@
     <t>Option Screen</t>
   </si>
   <si>
-    <t>Avec test</t>
-  </si>
-  <si>
     <t>Scene</t>
   </si>
   <si>
     <t>Terminée : Tester soi même la dernière build !</t>
   </si>
   <si>
-    <t>GlobalOffset, Vitesse molette, mode tapis, mode debug offbeat</t>
-  </si>
-  <si>
-    <t>Reload / Actualiser, Supprimer, reload à chaque redemarrage</t>
-  </si>
-  <si>
     <t>Correction de la detection de cross, sons (partout), optim du mainmenu (code), mettre si un score est legit ou non, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
   </si>
   <si>
@@ -409,6 +394,12 @@
   </si>
   <si>
     <t>Faire le bouton retour</t>
+  </si>
+  <si>
+    <t>WheelSong / Stepchart</t>
+  </si>
+  <si>
+    <t>Mode debug offbeat</t>
   </si>
 </sst>
 </file>
@@ -503,7 +494,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -573,6 +564,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,13 +587,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -934,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +971,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1091,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1244,14 +1238,14 @@
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" s="13"/>
     </row>
@@ -1333,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G27" s="13"/>
     </row>
@@ -1346,130 +1340,120 @@
         <v>30</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E28" s="33">
         <v>0.9</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="E29" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="12">
-        <v>0</v>
+      <c r="E30" s="36">
+        <v>0.5</v>
       </c>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="E31" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D32" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="D32" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="B33" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="1">
-        <v>0</v>
+      <c r="E33" s="34">
+        <v>0.5</v>
       </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E34" s="12">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="D34" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="B35" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="12">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="E35" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
@@ -1479,7 +1463,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E36" s="12">
         <v>0</v>
@@ -1487,215 +1471,215 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="B37" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="12">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>700</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>39</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="13">
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="13">
         <v>41231</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="4" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="8">
-        <v>1</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E39" s="30">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G39" s="13">
+      <c r="E39" s="8">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="30">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G40" s="13">
         <v>41245</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" s="19">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="19">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="19">
-        <v>0</v>
-      </c>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="E42" s="19">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>800</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6" t="s">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E43" s="7">
         <v>0.6</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G42" s="13">
+      <c r="F43" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G43" s="13">
         <v>41252</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>20</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" s="13">
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="13">
         <v>41259</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>900</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="7">
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7">
         <v>0.9</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G44" s="13">
+      <c r="F45" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="13">
         <v>41266</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="29" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C46" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="30">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G45" s="13"/>
-    </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="D46" s="29"/>
+      <c r="E46" s="30">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>1000</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>42</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>68</v>
       </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G46" s="13">
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G47" s="13">
         <v>40914</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="3"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -1704,7 +1688,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>45</v>
@@ -1719,7 +1703,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>45</v>
@@ -1734,66 +1718,66 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="D53" s="2"/>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>2000</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="18" t="s">
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="16">
-        <v>0</v>
-      </c>
-      <c r="F54" s="17"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>3000</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="F55" s="3"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="16">
+        <v>0</v>
+      </c>
+      <c r="F55" s="17"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -1802,13 +1786,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -1817,47 +1801,52 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
+        <v>5000</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>6000</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="B59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E58" s="1">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>7000</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="E60" s="1">
-        <v>0</v>
-      </c>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C61" s="2"/>
       <c r="E61" s="1">
@@ -1866,11 +1855,8 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>55</v>
-      </c>
       <c r="B62" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C62" s="2"/>
       <c r="E62" s="1">
@@ -1880,10 +1866,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63" s="2"/>
       <c r="E63" s="1">
@@ -1893,181 +1879,191 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C69" t="s">
-        <v>86</v>
-      </c>
-      <c r="E69" t="s">
-        <v>101</v>
+      <c r="E65" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>89</v>
-      </c>
-      <c r="B70" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" t="s">
         <v>85</v>
       </c>
-      <c r="C70" t="s">
-        <v>87</v>
-      </c>
       <c r="E70" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D72" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="E72" t="s">
+        <v>102</v>
+      </c>
+      <c r="F72" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D71" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E71" t="s">
-        <v>103</v>
-      </c>
-      <c r="F71" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C72" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D72" s="24"/>
-      <c r="E72" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>98</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>100</v>
-      </c>
+      <c r="C73" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" s="24"/>
       <c r="E73" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B74" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D74" s="24"/>
+      <c r="D74" s="23" t="s">
+        <v>99</v>
+      </c>
       <c r="E74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="D75" s="24"/>
       <c r="E75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" t="s">
+        <v>95</v>
+      </c>
       <c r="D76" s="24"/>
-      <c r="F76" t="s">
+      <c r="E76" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="D77" s="24"/>
+      <c r="F77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C78" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D78" s="24"/>
+      <c r="E78" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>98</v>
-      </c>
-      <c r="B77" s="3" t="s">
+      <c r="F78" t="s">
         <v>112</v>
-      </c>
-      <c r="C77" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D77" s="24"/>
-      <c r="E77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F77" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>90</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C78" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D78" s="23"/>
-      <c r="E78" t="s">
-        <v>108</v>
-      </c>
-      <c r="F78" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D79" s="23"/>
+      <c r="E79" t="s">
+        <v>107</v>
+      </c>
+      <c r="F79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C79" t="s">
-        <v>108</v>
-      </c>
-      <c r="D79" s="25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="22"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="22"/>
@@ -2182,6 +2178,9 @@
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="22"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 624] [Add/Update] Lien du panneau d'option avec le MainMenu.cs Correction du bruit des Mine Ajout du bouton de tri
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t>Stepchart</t>
   </si>
@@ -288,36 +288,12 @@
     <t>Moi-même</t>
   </si>
   <si>
-    <t>Moyen</t>
-  </si>
-  <si>
-    <t>Ca brille trop</t>
-  </si>
-  <si>
-    <t>On confond les rouges et les mines</t>
-  </si>
-  <si>
-    <t>Trop petit</t>
-  </si>
-  <si>
     <t>Différence entre roll et freeze bof</t>
   </si>
   <si>
-    <t>Aucun</t>
-  </si>
-  <si>
-    <t>Musique stressante</t>
-  </si>
-  <si>
     <t>NayKid</t>
   </si>
   <si>
-    <t>A mettre dans lesoptions</t>
-  </si>
-  <si>
-    <t>zoom dans les options ?</t>
-  </si>
-  <si>
     <t>Facilité à résoudre</t>
   </si>
   <si>
@@ -336,9 +312,6 @@
     <t>Parfois le titre de la chanson reste sur le coté lors de la selection</t>
   </si>
   <si>
-    <t>Panneau d'option</t>
-  </si>
-  <si>
     <t>??</t>
   </si>
   <si>
@@ -387,9 +360,6 @@
     <t>Particle  de fond améliorable</t>
   </si>
   <si>
-    <t>Tester, rajouter le bouton GUI, rajouter la gestion de l'erreur via un script à part</t>
-  </si>
-  <si>
     <t>SongSerializable Ok : Il faut tester</t>
   </si>
   <si>
@@ -400,13 +370,25 @@
   </si>
   <si>
     <t>Mode debug offbeat</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>A tester</t>
+  </si>
+  <si>
+    <t>Diminuer le temps de clear, diminuer les transitions (toutes), son du fail pas assez fort</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +430,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +473,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -511,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -552,7 +533,6 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -563,10 +543,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,13 +569,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -928,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,8 +1066,8 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>122</v>
+      <c r="F11" s="30" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1326,375 +1308,376 @@
       <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="28" t="s">
-        <v>118</v>
+      <c r="F27" s="27" t="s">
+        <v>109</v>
       </c>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="33">
+      <c r="D28" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="32">
         <v>0.9</v>
       </c>
-      <c r="F28" s="28" t="s">
-        <v>125</v>
+      <c r="F28" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="32">
         <v>0.5</v>
       </c>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="32">
         <v>0.5</v>
       </c>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="34">
+      <c r="E31" s="32">
         <v>0.5</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="E32" s="34">
+      <c r="D32" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="32">
         <v>0.5</v>
       </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>0.5</v>
       </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="36">
+      <c r="D34" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="32">
         <v>0.5</v>
       </c>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="35" t="s">
+      <c r="B35" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="32">
         <v>0.5</v>
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="12">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3"/>
+      <c r="C36" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="12">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="12">
-        <v>0</v>
-      </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="D38" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>700</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="13">
+      <c r="E39" s="37">
+        <v>0.9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>119</v>
+      </c>
+      <c r="G39" s="13">
         <v>41231</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="4" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="8">
-        <v>1</v>
-      </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" s="30">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G40" s="13">
+      <c r="E40" s="8">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" s="29">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41" s="13">
         <v>41245</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41" s="19">
-        <v>0</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="19">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="19">
-        <v>0</v>
-      </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="E43" s="19">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>800</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6" t="s">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G43" s="13">
+      <c r="E44" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="13">
         <v>41252</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>20</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="G44" s="13">
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="13">
         <v>41259</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>900</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7">
         <v>0.9</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G45" s="13">
+      <c r="F46" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" s="13">
         <v>41266</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" s="29" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C47" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="29"/>
-      <c r="E46" s="30">
-        <v>0</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G46" s="13"/>
-    </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="D47" s="28"/>
+      <c r="E47" s="29">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>1000</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>42</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>68</v>
       </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G47" s="13">
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G48" s="13">
         <v>40914</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
+      <c r="B49" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="17"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
-      <c r="F49" s="3"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -1703,7 +1686,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>45</v>
@@ -1718,7 +1701,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>45</v>
@@ -1733,66 +1716,66 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="D54" s="2"/>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>2000</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="18" t="s">
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="15"/>
+      <c r="B56" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="16">
-        <v>0</v>
-      </c>
-      <c r="F55" s="17"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>3000</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="3"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="16">
+        <v>0</v>
+      </c>
+      <c r="F56" s="17"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -1801,13 +1784,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -1816,47 +1799,52 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
+        <v>5000</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>6000</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="B60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E60" s="1">
-        <v>0</v>
-      </c>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>7000</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="E61" s="1">
-        <v>0</v>
-      </c>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C62" s="2"/>
       <c r="E62" s="1">
@@ -1865,11 +1853,8 @@
       <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>55</v>
-      </c>
       <c r="B63" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C63" s="2"/>
       <c r="E63" s="1">
@@ -1879,10 +1864,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C64" s="2"/>
       <c r="E64" s="1">
@@ -1892,178 +1877,129 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>56</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" t="s">
-        <v>85</v>
-      </c>
-      <c r="E70" t="s">
-        <v>100</v>
+      <c r="E66" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B72" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="26" t="s">
+      <c r="B73" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="E72" t="s">
-        <v>102</v>
-      </c>
-      <c r="F72" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>97</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C73" s="26" t="s">
-        <v>90</v>
+      <c r="C73" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="D73" s="24"/>
       <c r="E73" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="24"/>
+      <c r="E74" t="s">
+        <v>98</v>
+      </c>
+      <c r="F74" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D74" s="23" t="s">
+      <c r="C75" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" s="23"/>
+      <c r="E75" t="s">
+        <v>98</v>
+      </c>
+      <c r="F75" t="s">
         <v>99</v>
       </c>
-      <c r="E74" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D75" s="24"/>
-      <c r="E75" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
-      </c>
-      <c r="D76" s="24"/>
-      <c r="E76" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-      <c r="D77" s="24"/>
-      <c r="F77" t="s">
-        <v>106</v>
-      </c>
+      <c r="B77" s="22"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>97</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C78" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D78" s="24"/>
-      <c r="E78" t="s">
-        <v>107</v>
-      </c>
-      <c r="F78" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>89</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C79" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D79" s="23"/>
-      <c r="E79" t="s">
-        <v>107</v>
-      </c>
-      <c r="F79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>97</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C80" t="s">
-        <v>107</v>
-      </c>
-      <c r="D80" s="25" t="s">
-        <v>110</v>
-      </c>
+      <c r="B78" s="22"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="22"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="22"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="22"/>
@@ -2169,18 +2105,6 @@
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="22"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="22"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="22"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="22"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 625] [Update] Finalisation du panneau d'option niveau code Next step : Travailler la scene Unity
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="121">
   <si>
     <t>Stepchart</t>
   </si>
@@ -345,9 +345,6 @@
     <t>Scene</t>
   </si>
   <si>
-    <t>Terminée : Tester soi même la dernière build !</t>
-  </si>
-  <si>
     <t>Correction de la detection de cross, sons (partout), optim du mainmenu (code), mettre si un score est legit ou non, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
     <t>SongSerializable Ok : Il faut tester</t>
   </si>
   <si>
-    <t>Faire le bouton retour</t>
-  </si>
-  <si>
     <t>WheelSong / Stepchart</t>
   </si>
   <si>
@@ -382,6 +376,9 @@
   </si>
   <si>
     <t>Tester</t>
+  </si>
+  <si>
+    <t>Placer dans Unity</t>
   </si>
 </sst>
 </file>
@@ -912,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,9 +1305,7 @@
       <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="27" t="s">
-        <v>109</v>
-      </c>
+      <c r="F27" s="27"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1328,7 +1323,7 @@
         <v>0.9</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G28" s="13"/>
     </row>
@@ -1343,9 +1338,11 @@
         <v>36</v>
       </c>
       <c r="E29" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F29" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="33" t="s">
@@ -1358,9 +1355,11 @@
         <v>67</v>
       </c>
       <c r="E30" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F30" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="31" t="s">
@@ -1373,9 +1372,11 @@
         <v>37</v>
       </c>
       <c r="E31" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F31" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="31" t="s">
@@ -1388,9 +1389,11 @@
         <v>104</v>
       </c>
       <c r="E32" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F32" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="31" t="s">
@@ -1403,9 +1406,11 @@
         <v>40</v>
       </c>
       <c r="E33" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="33" t="s">
@@ -1418,9 +1423,11 @@
         <v>96</v>
       </c>
       <c r="E34" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="33" t="s">
@@ -1433,21 +1440,23 @@
         <v>71</v>
       </c>
       <c r="E35" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="34" t="s">
         <v>42</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D36" s="34"/>
       <c r="E36" s="35"/>
       <c r="F36" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1467,13 +1476,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E38" s="12">
         <v>0</v>
@@ -1497,7 +1506,7 @@
         <v>0.9</v>
       </c>
       <c r="F39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G39" s="13">
         <v>41231</v>
@@ -1531,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G41" s="13">
         <v>41245</v>
@@ -1581,7 +1590,7 @@
         <v>0.9</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G44" s="13">
         <v>41252</v>
@@ -1614,7 +1623,7 @@
         <v>0.9</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G46" s="13">
         <v>41266</v>
@@ -1635,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G47" s="13"/>
     </row>
@@ -1653,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G48" s="13">
         <v>40914</v>

</xml_diff>

<commit_message>
[Build 627] [Update] Avancement de ce qui reste avant la release Il ne reste plus que le Rate à programmer Et changer la barre de vie / bar de progress dans la chartScene
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740"/>
+    <workbookView xWindow="600" yWindow="210" windowWidth="12915" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="128">
   <si>
     <t>Stepchart</t>
   </si>
@@ -345,15 +345,9 @@
     <t>Scene</t>
   </si>
   <si>
-    <t>Correction de la detection de cross, sons (partout), optim du mainmenu (code), mettre si un score est legit ou non, regler le "startNumber" songlist, peut être faire en sorte de voir les medailles dans la songlist ?</t>
-  </si>
-  <si>
     <t>Trouver un doubleur</t>
   </si>
   <si>
-    <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage, à faire plus tard ?</t>
-  </si>
-  <si>
     <t>Particle  de fond améliorable</t>
   </si>
   <si>
@@ -372,20 +366,66 @@
     <t>A tester</t>
   </si>
   <si>
-    <t>Diminuer le temps de clear, diminuer les transitions (toutes), son du fail pas assez fort</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
     <t>Placer dans Unity</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t>Barre de vie à modifier</t>
+  </si>
+  <si>
+    <t>Time bar à modifier</t>
+  </si>
+  <si>
+    <t>Faire 2 cubes, relié par un fil, et une petite boule de particule qui monte. Tube relié aux targets qui change de couleur en fonction du score. Faire un tube qui sort de l'écran. Super fil bleu si FFC, fil jaune si FPC, fil vert si FC, cassage sinon</t>
+  </si>
+  <si>
+    <t>Background à modifier</t>
+  </si>
+  <si>
+    <t>Faire une sorte de pile de cube. Une seule particule. Retirer un effet de bloom sur le 2 = ++ perf</t>
+  </si>
+  <si>
+    <t>Pas encore d'idée</t>
+  </si>
+  <si>
+    <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage : A faire pour plus tard</t>
+  </si>
+  <si>
+    <t>Diminuer le temps de clear, diminuer les transitions (toutes), son du fail pas assez fort, mettre le "DebugOffset" dans InGameScript (engine), mettre le "ErrorLabel" dans WheelSS (engine), tester le startNumber, tester le "not legit !"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Correction de la detection de cross</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, peut être faire en sorte de voir les medailles dans la songlist ?</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +468,13 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -506,7 +553,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -546,6 +592,9 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,13 +615,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -907,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,8 +1112,8 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="30" t="s">
-        <v>112</v>
+      <c r="F11" s="29" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1178,7 +1227,7 @@
         <v>0.8</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -1207,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="20"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1226,7 +1275,7 @@
       <c r="F22" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -1242,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -1258,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="13"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -1274,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="13"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1293,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="13"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="4" t="s">
         <v>66</v>
       </c>
@@ -1305,210 +1354,214 @@
       <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="13"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="31">
         <v>0.9</v>
       </c>
-      <c r="F28" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="13"/>
+      <c r="F28" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="31">
         <v>0.7</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="31">
         <v>0.7</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="31">
         <v>0.7</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="31">
         <v>0.7</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <v>0.7</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="31">
         <v>0.7</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="31">
         <v>0.7</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B36" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
+      <c r="C36" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="33"/>
+      <c r="E36" s="34"/>
       <c r="F36" s="3" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="12">
-        <v>0</v>
-      </c>
-      <c r="F37" s="3"/>
+      <c r="E37" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="11" t="s">
+      <c r="B38" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="12">
-        <v>0</v>
-      </c>
-      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>700</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="37">
+      <c r="E39" s="36">
         <v>0.9</v>
       </c>
       <c r="F39" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="13">
+        <v>115</v>
+      </c>
+      <c r="G39" s="12">
         <v>41231</v>
       </c>
     </row>
@@ -1526,23 +1579,23 @@
         <v>1</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="13"/>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
+      <c r="B41" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="29">
+      <c r="E41" s="28">
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G41" s="13">
+        <v>125</v>
+      </c>
+      <c r="G41" s="12">
         <v>41245</v>
       </c>
     </row>
@@ -1554,11 +1607,11 @@
       <c r="D42" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E42" s="19">
+      <c r="E42" s="18">
         <v>0</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="13"/>
+      <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -1570,7 +1623,7 @@
       <c r="D43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="19">
+      <c r="E43" s="18">
         <v>0</v>
       </c>
       <c r="F43" s="3"/>
@@ -1579,20 +1632,20 @@
       <c r="A44">
         <v>800</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6" t="s">
+      <c r="C44" s="35"/>
+      <c r="D44" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="36">
         <v>0.9</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G44" s="13">
+        <v>116</v>
+      </c>
+      <c r="G44" s="12">
         <v>41252</v>
       </c>
     </row>
@@ -1606,7 +1659,7 @@
       <c r="E45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="12">
         <v>41259</v>
       </c>
     </row>
@@ -1614,18 +1667,18 @@
       <c r="A46">
         <v>900</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="7">
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="36">
         <v>0.9</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G46" s="13">
+        <v>111</v>
+      </c>
+      <c r="G46" s="12">
         <v>41266</v>
       </c>
     </row>
@@ -1633,263 +1686,281 @@
       <c r="A47" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="29">
+      <c r="D47" s="27"/>
+      <c r="E47" s="28">
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G47" s="13"/>
-    </row>
-    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48">
+        <v>109</v>
+      </c>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="38">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B49" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="38">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="38">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>1000</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>42</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G48" s="13">
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="12">
         <v>40914</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="17"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="16"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="2"/>
       <c r="E54" s="1">
         <v>0</v>
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>2000</v>
-      </c>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2000</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18" t="s">
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="16">
-        <v>0</v>
-      </c>
-      <c r="F56" s="17"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="15">
+        <v>0</v>
+      </c>
+      <c r="F59" s="16"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>3000</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>4000</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="B61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E58" s="1">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>5000</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="B62" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>6000</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="B63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E60" s="1">
-        <v>0</v>
-      </c>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E61" s="1">
-        <v>0</v>
-      </c>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>7000</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="E62" s="1">
-        <v>0</v>
-      </c>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>55</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>56</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C65" s="2"/>
       <c r="E65" s="1">
@@ -1898,222 +1969,258 @@
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="E68" s="1">
+        <v>0</v>
+      </c>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E66" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" t="s">
-        <v>85</v>
-      </c>
-      <c r="E71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>88</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" t="s">
-        <v>86</v>
-      </c>
-      <c r="E72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>91</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D73" s="24"/>
-      <c r="E73" t="s">
-        <v>94</v>
+      <c r="E69" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C74" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" t="s">
+        <v>85</v>
+      </c>
+      <c r="E74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" t="s">
         <v>86</v>
       </c>
-      <c r="D74" s="24"/>
-      <c r="E74" t="s">
-        <v>98</v>
-      </c>
-      <c r="F74" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>89</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D75" s="23"/>
       <c r="E75" t="s">
-        <v>98</v>
-      </c>
-      <c r="F75" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>91</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D76" s="23"/>
+      <c r="E76" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D77" s="23"/>
+      <c r="E77" t="s">
+        <v>98</v>
+      </c>
+      <c r="F77" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" t="s">
+        <v>98</v>
+      </c>
+      <c r="F78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C79" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="25" t="s">
+      <c r="D79" s="24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="22"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="22"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="22"/>
-    </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="22"/>
+      <c r="B80" s="21"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="22"/>
+      <c r="B81" s="21"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="22"/>
+      <c r="B82" s="21"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="22"/>
+      <c r="B83" s="21"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="22"/>
+      <c r="B84" s="21"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="22"/>
+      <c r="B85" s="21"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="22"/>
+      <c r="B86" s="21"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="22"/>
+      <c r="B87" s="21"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="22"/>
+      <c r="B88" s="21"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="22"/>
+      <c r="B89" s="21"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="22"/>
+      <c r="B90" s="21"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="22"/>
+      <c r="B91" s="21"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="22"/>
+      <c r="B92" s="21"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="22"/>
+      <c r="B93" s="21"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="22"/>
+      <c r="B94" s="21"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="22"/>
+      <c r="B95" s="21"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="22"/>
+      <c r="B96" s="21"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="22"/>
+      <c r="B97" s="21"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="22"/>
+      <c r="B98" s="21"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="22"/>
+      <c r="B99" s="21"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="22"/>
+      <c r="B100" s="21"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="22"/>
+      <c r="B101" s="21"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="22"/>
+      <c r="B102" s="21"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="22"/>
+      <c r="B103" s="21"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="22"/>
+      <c r="B104" s="21"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="22"/>
+      <c r="B105" s="21"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="22"/>
+      <c r="B106" s="21"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="22"/>
+      <c r="B107" s="21"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="22"/>
+      <c r="B108" s="21"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="22"/>
+      <c r="B109" s="21"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="22"/>
+      <c r="B110" s="21"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="22"/>
+      <c r="B111" s="21"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="22"/>
+      <c r="B112" s="21"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="22"/>
+      <c r="B113" s="21"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="22"/>
+      <c r="B114" s="21"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="22"/>
+      <c r="B115" s="21"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="21"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="21"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 627] [Fix planning]
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="210" windowWidth="12915" windowHeight="7560"/>
+    <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="131">
   <si>
     <t>Stepchart</t>
   </si>
@@ -381,16 +381,10 @@
     <t>Time bar à modifier</t>
   </si>
   <si>
-    <t>Faire 2 cubes, relié par un fil, et une petite boule de particule qui monte. Tube relié aux targets qui change de couleur en fonction du score. Faire un tube qui sort de l'écran. Super fil bleu si FFC, fil jaune si FPC, fil vert si FC, cassage sinon</t>
-  </si>
-  <si>
     <t>Background à modifier</t>
   </si>
   <si>
     <t>Faire une sorte de pile de cube. Une seule particule. Retirer un effet de bloom sur le 2 = ++ perf</t>
-  </si>
-  <si>
-    <t>Pas encore d'idée</t>
   </si>
   <si>
     <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage : A faire pour plus tard</t>
@@ -419,6 +413,21 @@
       </rPr>
       <t>, peut être faire en sorte de voir les medailles dans la songlist ?</t>
     </r>
+  </si>
+  <si>
+    <t>Faire 2 cubes, relié par un fil, et une petite boule de particule qui monte. Tube relié aux targets qui change de couleur en fonction du score. Faire un tube qui sort de l'écran. Super fil bleu si FFC, super fil jaune si FPC, fil vert si vie à fond ou entrain de remonter, cassage sinon. +2 particules jouées ensemble</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Augmenter les perfs</t>
+  </si>
+  <si>
+    <t>Mettre un seul cache au lieu d'un, mettre moins de cube dans le bg</t>
+  </si>
+  <si>
+    <t>Leger bump de scale à voir si ça affecte pas les perfs</t>
   </si>
 </sst>
 </file>
@@ -615,13 +624,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -956,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1514,7 @@
       <c r="D36" s="33"/>
       <c r="E36" s="34"/>
       <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1593,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G41" s="12">
         <v>41245</v>
@@ -1715,11 +1724,11 @@
         <v>0</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B49" s="37" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G49" s="12"/>
     </row>
@@ -1745,70 +1754,73 @@
         <v>118</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E50" s="38">
         <v>0</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G50" s="12"/>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="38">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>1000</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>42</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G51" s="12">
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" s="12">
         <v>40914</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="16"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="16"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -1817,7 +1829,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>45</v>
@@ -1832,7 +1844,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>45</v>
@@ -1847,66 +1859,66 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="D58" s="2"/>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>2000</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="1">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17" t="s">
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="15">
-        <v>0</v>
-      </c>
-      <c r="F59" s="16"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>3000</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E60" s="1">
-        <v>0</v>
-      </c>
-      <c r="F60" s="3"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="15">
+        <v>0</v>
+      </c>
+      <c r="F60" s="16"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
@@ -1915,13 +1927,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
@@ -1930,47 +1942,52 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
+        <v>5000</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>6000</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="B64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>7000</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C66" s="2"/>
       <c r="E66" s="1">
@@ -1979,11 +1996,8 @@
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>55</v>
-      </c>
       <c r="B67" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" s="2"/>
       <c r="E67" s="1">
@@ -1993,10 +2007,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="2"/>
       <c r="E68" s="1">
@@ -2006,107 +2020,117 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E69" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" t="s">
-        <v>85</v>
-      </c>
-      <c r="E74" t="s">
-        <v>92</v>
+      <c r="E70" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
-      </c>
-      <c r="B75" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C76" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C76" t="s">
         <v>86</v>
       </c>
-      <c r="D76" s="23"/>
       <c r="E76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C77" s="25" t="s">
+      <c r="B77" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>86</v>
       </c>
       <c r="D77" s="23"/>
       <c r="E77" t="s">
-        <v>98</v>
-      </c>
-      <c r="F77" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D78" s="22"/>
+        <v>86</v>
+      </c>
+      <c r="D78" s="23"/>
       <c r="E78" t="s">
         <v>98</v>
       </c>
       <c r="F78" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" t="s">
+        <v>98</v>
+      </c>
+      <c r="F79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>91</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>98</v>
       </c>
-      <c r="D79" s="24" t="s">
+      <c r="D80" s="24" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="21"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="21"/>
@@ -2221,6 +2245,9 @@
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="21"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Build 629] [Add/Update] Preparation du rate. Appel du process ok Reste : Le programme à compiler et l'application sur la stepchart
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="132">
   <si>
     <t>Stepchart</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>Leger bump de scale à voir si ça affecte pas les perfs</t>
+  </si>
+  <si>
+    <t>Rate placé, programme placer. Programme à compiler, à tester. Rate à installer sur la lecture de chart.</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,13 +525,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -594,16 +591,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1226,7 @@
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="20"/>
@@ -1368,16 +1361,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="7">
         <v>0.9</v>
       </c>
       <c r="F28" s="26" t="s">
@@ -1386,16 +1379,16 @@
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="31">
+      <c r="E29" s="7">
         <v>0.7</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -1403,16 +1396,16 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="7">
         <v>0.7</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -1420,16 +1413,16 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="31">
+      <c r="E31" s="7">
         <v>0.7</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -1437,16 +1430,16 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="7">
         <v>0.7</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -1454,16 +1447,16 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="7">
         <v>0.7</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1471,16 +1464,16 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="7">
         <v>0.7</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -1488,16 +1481,16 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="7">
         <v>0.7</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -1505,29 +1498,29 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="34"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
       <c r="F36" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="39" t="s">
+      <c r="D37" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E37" s="7">
         <v>0.9</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1535,16 +1528,16 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E38" s="7">
         <v>0.9</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -1555,16 +1548,16 @@
       <c r="A39">
         <v>700</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E39" s="7">
         <v>0.9</v>
       </c>
       <c r="F39" t="s">
@@ -1641,14 +1634,14 @@
       <c r="A44">
         <v>800</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35" t="s">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="36">
+      <c r="E44" s="7">
         <v>0.9</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -1658,15 +1651,19 @@
         <v>41252</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="1">
-        <v>0</v>
+      <c r="D45" s="34"/>
+      <c r="E45" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="G45" s="12">
         <v>41259</v>
@@ -1676,12 +1673,12 @@
       <c r="A46">
         <v>900</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="36">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7">
         <v>0.9</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1711,16 +1708,16 @@
       <c r="G47" s="12"/>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="37" t="s">
+      <c r="B48" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="E48" s="38">
+      <c r="E48" s="33">
         <v>0</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -1729,16 +1726,16 @@
       <c r="G48" s="12"/>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B49" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="37" t="s">
+      <c r="B49" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="E49" s="38">
+      <c r="E49" s="33">
         <v>0</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -1747,16 +1744,16 @@
       <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="37" t="s">
+      <c r="B50" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="E50" s="38">
+      <c r="E50" s="33">
         <v>0</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -1765,16 +1762,16 @@
       <c r="G50" s="12"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="37" t="s">
+      <c r="B51" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="38">
+      <c r="E51" s="33">
         <v>0</v>
       </c>
       <c r="F51" s="3" t="s">

</xml_diff>

<commit_message>
[Build 630] [Update] Fin du rate. Fin du code (sauf update graphique) non testé de la version 1000. Reste : Tout à tester, et faire l'update graphique avant la release
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -430,14 +430,14 @@
     <t>Leger bump de scale à voir si ça affecte pas les perfs</t>
   </si>
   <si>
-    <t>Rate placé, programme placer. Programme à compiler, à tester. Rate à installer sur la lecture de chart.</t>
+    <t>Rate placé, programme placé. Programme à compiler, à tester. Rate à tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,20 +479,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="3" tint="0.39997558519241921"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,12 +516,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -542,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -595,8 +582,6 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -960,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,15 +1637,15 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35">
-        <v>0.3</v>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7">
+        <v>0.8</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
[Build 631] [Update] Début placage panneau d'option dans Unity
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="7500"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
   <si>
     <t>Stepchart</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Première phase de test privée</t>
-  </si>
-  <si>
-    <t>Mode "rapide"</t>
   </si>
   <si>
     <t>Correction générale + optim</t>
@@ -431,6 +428,15 @@
   </si>
   <si>
     <t>Rate placé, programme placé. Programme à compiler, à tester. Rate à tester</t>
+  </si>
+  <si>
+    <t>A tester, implémenter le mode rapide</t>
+  </si>
+  <si>
+    <t>Mode "rapide"/Mode tapis</t>
+  </si>
+  <si>
+    <t>Sera fait plus tard</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +522,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -529,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -582,6 +594,8 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,7 +960,7 @@
   <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +1000,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1094,13 +1108,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1177,13 +1191,13 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="7">
         <v>0.99</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1207,7 +1221,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="5">
@@ -1221,10 +1235,10 @@
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" s="8">
         <v>1</v>
@@ -1236,7 +1250,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5">
@@ -1253,14 +1267,14 @@
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="12"/>
     </row>
@@ -1353,13 +1367,13 @@
         <v>30</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E28" s="7">
         <v>0.9</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G28" s="12"/>
     </row>
@@ -1374,27 +1388,27 @@
         <v>36</v>
       </c>
       <c r="E29" s="7">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0.7</v>
+      <c r="D30" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="35">
+        <v>0.5</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1411,7 +1425,7 @@
         <v>0.7</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1422,13 +1436,13 @@
         <v>30</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" s="7">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1445,7 +1459,7 @@
         <v>0.7</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1456,30 +1470,30 @@
         <v>30</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E34" s="7">
         <v>0.7</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35" s="7">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1487,12 +1501,12 @@
         <v>42</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="31"/>
       <c r="F36" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1503,30 +1517,30 @@
         <v>24</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" s="7">
         <v>0.9</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E38" s="7">
         <v>0.9</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1546,7 +1560,7 @@
         <v>0.9</v>
       </c>
       <c r="F39" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="G39" s="12">
         <v>41231</v>
@@ -1574,13 +1588,13 @@
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E41" s="28">
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G41" s="12">
         <v>41245</v>
@@ -1592,7 +1606,7 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42" s="18">
         <v>0</v>
@@ -1630,7 +1644,7 @@
         <v>0.9</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G44" s="12">
         <v>41252</v>
@@ -1648,7 +1662,7 @@
         <v>0.8</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G45" s="12">
         <v>41259</v>
@@ -1659,7 +1673,7 @@
         <v>900</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -1667,7 +1681,7 @@
         <v>0.9</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G46" s="12">
         <v>41266</v>
@@ -1675,7 +1689,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="27" t="s">
         <v>42</v>
@@ -1688,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G47" s="12"/>
     </row>
@@ -1697,16 +1711,16 @@
         <v>0</v>
       </c>
       <c r="C48" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="32" t="s">
-        <v>119</v>
-      </c>
       <c r="E48" s="33">
         <v>0</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G48" s="12"/>
     </row>
@@ -1715,16 +1729,16 @@
         <v>0</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E49" s="33">
         <v>0</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G49" s="12"/>
     </row>
@@ -1733,16 +1747,16 @@
         <v>0</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E50" s="33">
         <v>0</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G50" s="12"/>
     </row>
@@ -1751,16 +1765,16 @@
         <v>0</v>
       </c>
       <c r="C51" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="32" t="s">
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="E51" s="33">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="G51" s="12"/>
     </row>
@@ -1772,13 +1786,13 @@
         <v>42</v>
       </c>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G52" s="12">
         <v>40914</v>
@@ -1876,7 +1890,7 @@
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -1886,7 +1900,7 @@
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -2026,92 +2040,92 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D77" s="23"/>
       <c r="E77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D78" s="23"/>
       <c r="E78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F78" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" t="s">
+        <v>97</v>
+      </c>
+      <c r="F79" t="s">
         <v>98</v>
-      </c>
-      <c r="F79" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" s="24" t="s">
         <v>100</v>
-      </c>
-      <c r="C80" t="s">
-        <v>98</v>
-      </c>
-      <c r="D80" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 634] [Update] Petite correction du cache, ajout d'un message de confirmation sur le cache etc
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="121">
   <si>
     <t>Stepchart</t>
   </si>
@@ -367,9 +367,6 @@
     <t>Rate placé, programme placé. Programme à compiler, à tester. Rate à tester</t>
   </si>
   <si>
-    <t>A tester, implémenter le mode rapide</t>
-  </si>
-  <si>
     <t>Mode "rapide"/Mode tapis</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>Verifier si la concurrence marche bien</t>
   </si>
   <si>
-    <t>Fade in : ok, fade out : bug</t>
-  </si>
-  <si>
     <t>Tester, faire le bouton rouge</t>
   </si>
   <si>
@@ -401,6 +395,9 @@
   </si>
   <si>
     <t>AVACEMENT PROJET</t>
+  </si>
+  <si>
+    <t>Améliorer le FadeOut peut être ?</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,13 +1087,13 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
         <v>113</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>114</v>
-      </c>
-      <c r="G3" t="s">
-        <v>115</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1383,7 +1380,7 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1605,16 +1602,13 @@
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
-        <v>631</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E28" s="33">
@@ -1623,15 +1617,18 @@
       <c r="F28" s="33">
         <v>1</v>
       </c>
-      <c r="G28" s="28">
-        <v>0.5</v>
+      <c r="G28" s="27">
+        <v>1</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="43">
+        <v>633</v>
+      </c>
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
@@ -1651,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1662,7 +1659,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" s="37">
         <v>0.2</v>
@@ -1674,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1876,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I39" s="8">
         <v>41231</v>
@@ -2210,15 +2207,15 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.6246666666666667</v>
+        <v>0.628</v>
       </c>
       <c r="E54" s="47">
         <f>SUM(E4:E53)/50</f>
@@ -2230,7 +2227,7 @@
       </c>
       <c r="G54" s="49">
         <f>SUM(G4:G53)/50</f>
-        <v>0.50800000000000001</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2240,13 +2237,13 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="G55" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2595,14 +2592,14 @@
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.44619047619047619</v>
+        <v>0.44857142857142857</v>
       </c>
       <c r="E75" s="47">
         <f>(SUM(E4:E73) - E54)/70</f>
@@ -2614,7 +2611,7 @@
       </c>
       <c r="G75" s="49">
         <f t="shared" si="0"/>
-        <v>0.36285714285714282</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 700] [Update] Panneau d'option : ok Tri des chansons : ok Tester la chart scene Tester les options générales Tester le rate
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="7500"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="121">
   <si>
     <t>Stepchart</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Date approx</t>
   </si>
   <si>
-    <t>Option</t>
-  </si>
-  <si>
     <t>Entrée dans le jeu et trans</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>Particle  de fond améliorable</t>
   </si>
   <si>
-    <t>SongSerializable Ok : Il faut tester</t>
-  </si>
-  <si>
     <t>WheelSong / Stepchart</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>Tester</t>
   </si>
   <si>
-    <t>Placer dans Unity</t>
-  </si>
-  <si>
     <t>Modification</t>
   </si>
   <si>
@@ -322,9 +313,6 @@
   </si>
   <si>
     <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage : A faire pour plus tard</t>
-  </si>
-  <si>
-    <t>Diminuer le temps de clear, diminuer les transitions (toutes), son du fail pas assez fort, mettre le "DebugOffset" dans InGameScript (engine), mettre le "ErrorLabel" dans WheelSS (engine), tester le startNumber, tester le "not legit !"</t>
   </si>
   <si>
     <r>
@@ -385,9 +373,6 @@
     <t>Verifier si la concurrence marche bien</t>
   </si>
   <si>
-    <t>Tester, faire le bouton rouge</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -397,7 +382,22 @@
     <t>AVACEMENT PROJET</t>
   </si>
   <si>
-    <t>Améliorer le FadeOut peut être ?</t>
+    <t>Tester in game</t>
+  </si>
+  <si>
+    <t>Petit problème avec x8 ?</t>
+  </si>
+  <si>
+    <t>OptionManager</t>
+  </si>
+  <si>
+    <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
+  </si>
+  <si>
+    <t>Diminuer le temps de clear, diminuer les transitions (toutes), son du fail pas assez fort, mettre le "DebugOffset" dans InGameScript (engine),  tester le startNumber, tester le "not legit !"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petit bug de transistion avec le Fade out </t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,6 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -689,6 +688,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,13 +1087,13 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1140,7 +1140,7 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
+      <c r="A6" s="41">
         <v>200</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1261,11 +1261,11 @@
         <v>1</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="42">
+      <c r="A12" s="41">
         <v>300</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1380,11 +1380,11 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="42">
+      <c r="A18" s="41">
         <v>400</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1467,14 +1467,14 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="42">
+      <c r="A22" s="41">
         <v>500</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="33">
@@ -1487,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I22" s="8"/>
     </row>
@@ -1558,7 +1558,7 @@
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="42">
+      <c r="A26" s="41">
         <v>600</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1602,14 +1602,14 @@
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>86</v>
+      <c r="D28" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="E28" s="33">
         <v>1</v>
@@ -1617,8 +1617,8 @@
       <c r="F28" s="33">
         <v>1</v>
       </c>
-      <c r="G28" s="27">
-        <v>1</v>
+      <c r="G28" s="28">
+        <v>0.99</v>
       </c>
       <c r="H28" s="20" t="s">
         <v>120</v>
@@ -1626,9 +1626,7 @@
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
-        <v>633</v>
-      </c>
+      <c r="A29" s="42"/>
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
@@ -1641,14 +1639,14 @@
       <c r="E29" s="33">
         <v>1</v>
       </c>
-      <c r="F29" s="35">
-        <v>0.9</v>
-      </c>
-      <c r="G29" s="41">
-        <v>0</v>
+      <c r="F29" s="33">
+        <v>1</v>
+      </c>
+      <c r="G29" s="28">
+        <v>0.8</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1659,53 +1657,51 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" s="37">
+        <v>106</v>
+      </c>
+      <c r="E30" s="36">
         <v>0.2</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="36">
         <v>0.2</v>
       </c>
       <c r="G30" s="30">
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
       </c>
-      <c r="F31" s="40">
-        <v>0</v>
-      </c>
-      <c r="G31" s="41">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="F31" s="33">
+        <v>1</v>
+      </c>
+      <c r="G31" s="27">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>82</v>
+      <c r="D32" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E32" s="33">
         <v>1</v>
@@ -1713,67 +1709,63 @@
       <c r="F32" s="33">
         <v>1</v>
       </c>
-      <c r="G32" s="41">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="G32" s="27">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E33" s="33">
         <v>1</v>
       </c>
-      <c r="F33" s="40">
-        <v>0</v>
-      </c>
-      <c r="G33" s="41">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="F33" s="33">
+        <v>1</v>
+      </c>
+      <c r="G33" s="27">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="23" t="s">
-        <v>81</v>
+      <c r="D34" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="E34" s="33">
         <v>1</v>
       </c>
-      <c r="F34" s="40">
-        <v>0</v>
-      </c>
-      <c r="G34" s="41">
-        <v>0</v>
+      <c r="F34" s="33">
+        <v>1</v>
+      </c>
+      <c r="G34" s="27">
+        <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="23" t="s">
+      <c r="B35" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="6" t="s">
         <v>69</v>
       </c>
       <c r="E35" s="33">
@@ -1782,98 +1774,95 @@
       <c r="F35" s="33">
         <v>1</v>
       </c>
-      <c r="G35" s="41">
-        <v>0</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="G35" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="23"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="29"/>
       <c r="H36" s="2" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>77</v>
+      <c r="D37" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="E37" s="33">
         <v>1</v>
       </c>
-      <c r="F37" s="40">
-        <v>0</v>
-      </c>
-      <c r="G37" s="41">
-        <v>0</v>
+      <c r="F37" s="33">
+        <v>1</v>
+      </c>
+      <c r="G37" s="27">
+        <v>1</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="23" t="s">
+      <c r="B38" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="33">
+        <v>1</v>
+      </c>
+      <c r="F38" s="33">
+        <v>1</v>
+      </c>
+      <c r="G38" s="27">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E38" s="33">
-        <v>1</v>
-      </c>
-      <c r="F38" s="40">
-        <v>0</v>
-      </c>
-      <c r="G38" s="41">
-        <v>0</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="50">
         <v>700</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="33">
         <v>1</v>
       </c>
-      <c r="F39" s="40">
-        <v>0</v>
-      </c>
-      <c r="G39" s="41">
-        <v>0</v>
+      <c r="F39" s="33">
+        <v>1</v>
+      </c>
+      <c r="G39" s="27">
+        <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I39" s="8">
         <v>41231</v>
@@ -1907,19 +1896,19 @@
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="37">
-        <v>0</v>
-      </c>
-      <c r="F41" s="37">
-        <v>0</v>
-      </c>
-      <c r="G41" s="37">
+        <v>83</v>
+      </c>
+      <c r="E41" s="36">
+        <v>0</v>
+      </c>
+      <c r="F41" s="36">
+        <v>0</v>
+      </c>
+      <c r="G41" s="36">
         <v>0</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I41" s="8"/>
     </row>
@@ -1929,15 +1918,15 @@
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="38">
-        <v>0</v>
-      </c>
-      <c r="F42" s="38">
-        <v>0</v>
-      </c>
-      <c r="G42" s="38">
+        <v>82</v>
+      </c>
+      <c r="E42" s="37">
+        <v>0</v>
+      </c>
+      <c r="F42" s="37">
+        <v>0</v>
+      </c>
+      <c r="G42" s="37">
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
@@ -1953,13 +1942,13 @@
       <c r="D43" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="38">
-        <v>0</v>
-      </c>
-      <c r="F43" s="38">
-        <v>0</v>
-      </c>
-      <c r="G43" s="38">
+      <c r="E43" s="37">
+        <v>0</v>
+      </c>
+      <c r="F43" s="37">
+        <v>0</v>
+      </c>
+      <c r="G43" s="37">
         <v>0</v>
       </c>
       <c r="H43" s="2"/>
@@ -1968,24 +1957,24 @@
       <c r="A44">
         <v>800</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="33">
         <v>1</v>
       </c>
-      <c r="F44" s="40">
-        <v>0</v>
-      </c>
-      <c r="G44" s="41">
-        <v>0</v>
+      <c r="F44" s="33">
+        <v>1</v>
+      </c>
+      <c r="G44" s="27">
+        <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I44" s="8">
         <v>41238</v>
@@ -2002,14 +1991,14 @@
       <c r="E45" s="33">
         <v>1</v>
       </c>
-      <c r="F45" s="40">
-        <v>0</v>
-      </c>
-      <c r="G45" s="41">
+      <c r="F45" s="39">
+        <v>0</v>
+      </c>
+      <c r="G45" s="40">
         <v>0</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I45" s="8">
         <v>41245</v>
@@ -2019,22 +2008,22 @@
       <c r="A46">
         <v>900</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="33">
         <v>1</v>
       </c>
       <c r="F46" s="33">
         <v>1</v>
       </c>
-      <c r="G46" s="41">
-        <v>0</v>
+      <c r="G46" s="27">
+        <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="I46" s="8">
         <v>41252</v>
@@ -2042,7 +2031,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>41</v>
@@ -2051,17 +2040,17 @@
         <v>61</v>
       </c>
       <c r="D47" s="21"/>
-      <c r="E47" s="37">
-        <v>0</v>
-      </c>
-      <c r="F47" s="37">
-        <v>0</v>
-      </c>
-      <c r="G47" s="37">
+      <c r="E47" s="36">
+        <v>0</v>
+      </c>
+      <c r="F47" s="36">
+        <v>0</v>
+      </c>
+      <c r="G47" s="36">
         <v>0</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I47" s="8"/>
     </row>
@@ -2070,22 +2059,22 @@
         <v>0</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D48" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="38">
+        <v>0</v>
+      </c>
+      <c r="F48" s="38">
+        <v>0</v>
+      </c>
+      <c r="G48" s="38">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="E48" s="39">
-        <v>0</v>
-      </c>
-      <c r="F48" s="39">
-        <v>0</v>
-      </c>
-      <c r="G48" s="39">
-        <v>0</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="I48" s="8"/>
     </row>
@@ -2094,22 +2083,22 @@
         <v>0</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="39">
-        <v>0</v>
-      </c>
-      <c r="F49" s="39">
-        <v>0</v>
-      </c>
-      <c r="G49" s="39">
+        <v>95</v>
+      </c>
+      <c r="E49" s="38">
+        <v>0</v>
+      </c>
+      <c r="F49" s="38">
+        <v>0</v>
+      </c>
+      <c r="G49" s="38">
         <v>0</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I49" s="8"/>
     </row>
@@ -2118,22 +2107,22 @@
         <v>0</v>
       </c>
       <c r="C50" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="39">
-        <v>0</v>
-      </c>
-      <c r="F50" s="39">
-        <v>0</v>
-      </c>
-      <c r="G50" s="39">
+      <c r="E50" s="38">
+        <v>0</v>
+      </c>
+      <c r="F50" s="38">
+        <v>0</v>
+      </c>
+      <c r="G50" s="38">
         <v>0</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I50" s="8"/>
     </row>
@@ -2142,22 +2131,22 @@
         <v>0</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" s="39">
-        <v>0</v>
-      </c>
-      <c r="F51" s="39">
-        <v>0</v>
-      </c>
-      <c r="G51" s="39">
+        <v>102</v>
+      </c>
+      <c r="E51" s="38">
+        <v>0</v>
+      </c>
+      <c r="F51" s="38">
+        <v>0</v>
+      </c>
+      <c r="G51" s="38">
         <v>0</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I51" s="8"/>
     </row>
@@ -2171,17 +2160,17 @@
       <c r="D52" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="39">
-        <v>0</v>
-      </c>
-      <c r="F52" s="39">
-        <v>0</v>
-      </c>
-      <c r="G52" s="39">
+      <c r="E52" s="38">
+        <v>0</v>
+      </c>
+      <c r="F52" s="38">
+        <v>0</v>
+      </c>
+      <c r="G52" s="38">
         <v>0</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I52" s="8">
         <v>41259</v>
@@ -2194,40 +2183,40 @@
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="50">
-        <v>0</v>
-      </c>
-      <c r="F53" s="50">
-        <v>0</v>
-      </c>
-      <c r="G53" s="50">
+      <c r="E53" s="49">
+        <v>0</v>
+      </c>
+      <c r="F53" s="49">
+        <v>0</v>
+      </c>
+      <c r="G53" s="49">
         <v>0</v>
       </c>
       <c r="H53" s="11"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.628</v>
-      </c>
-      <c r="E54" s="47">
-        <f>SUM(E4:E53)/50</f>
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="F54" s="48">
-        <f>SUM(F4:F53)/50</f>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="G54" s="49">
-        <f>SUM(G4:G53)/50</f>
-        <v>0.51800000000000002</v>
+        <v>0.79496453900709219</v>
+      </c>
+      <c r="E54" s="46">
+        <f>SUM(E4:E53)/47</f>
+        <v>0.81276595744680857</v>
+      </c>
+      <c r="F54" s="46">
+        <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/47</f>
+        <v>0.79148936170212769</v>
+      </c>
+      <c r="G54" s="46">
+        <f t="shared" si="0"/>
+        <v>0.7806382978723404</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2237,13 +2226,13 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G55" s="31" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2252,9 +2241,9 @@
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="46"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
       <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2267,13 +2256,13 @@
       <c r="D57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="44">
-        <v>0</v>
-      </c>
-      <c r="F57" s="44">
-        <v>0</v>
-      </c>
-      <c r="G57" s="44">
+      <c r="E57" s="43">
+        <v>0</v>
+      </c>
+      <c r="F57" s="43">
+        <v>0</v>
+      </c>
+      <c r="G57" s="43">
         <v>0</v>
       </c>
       <c r="H57" s="2"/>
@@ -2288,13 +2277,13 @@
       <c r="D58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="44">
-        <v>0</v>
-      </c>
-      <c r="F58" s="44">
-        <v>0</v>
-      </c>
-      <c r="G58" s="44">
+      <c r="E58" s="43">
+        <v>0</v>
+      </c>
+      <c r="F58" s="43">
+        <v>0</v>
+      </c>
+      <c r="G58" s="43">
         <v>0</v>
       </c>
       <c r="H58" s="2"/>
@@ -2309,13 +2298,13 @@
       <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E59" s="44">
-        <v>0</v>
-      </c>
-      <c r="F59" s="44">
-        <v>0</v>
-      </c>
-      <c r="G59" s="44">
+      <c r="E59" s="43">
+        <v>0</v>
+      </c>
+      <c r="F59" s="43">
+        <v>0</v>
+      </c>
+      <c r="G59" s="43">
         <v>0</v>
       </c>
       <c r="H59" s="2"/>
@@ -2330,13 +2319,13 @@
       <c r="D60" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E60" s="44">
-        <v>0</v>
-      </c>
-      <c r="F60" s="44">
-        <v>0</v>
-      </c>
-      <c r="G60" s="44">
+      <c r="E60" s="43">
+        <v>0</v>
+      </c>
+      <c r="F60" s="43">
+        <v>0</v>
+      </c>
+      <c r="G60" s="43">
         <v>0</v>
       </c>
       <c r="H60" s="2"/>
@@ -2349,13 +2338,13 @@
         <v>50</v>
       </c>
       <c r="D61" s="1"/>
-      <c r="E61" s="44">
-        <v>0</v>
-      </c>
-      <c r="F61" s="44">
-        <v>0</v>
-      </c>
-      <c r="G61" s="44">
+      <c r="E61" s="43">
+        <v>0</v>
+      </c>
+      <c r="F61" s="43">
+        <v>0</v>
+      </c>
+      <c r="G61" s="43">
         <v>0</v>
       </c>
       <c r="H61" s="2"/>
@@ -2371,13 +2360,13 @@
       <c r="D62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E62" s="44">
-        <v>0</v>
-      </c>
-      <c r="F62" s="44">
-        <v>0</v>
-      </c>
-      <c r="G62" s="44">
+      <c r="E62" s="43">
+        <v>0</v>
+      </c>
+      <c r="F62" s="43">
+        <v>0</v>
+      </c>
+      <c r="G62" s="43">
         <v>0</v>
       </c>
       <c r="H62" s="2"/>
@@ -2389,13 +2378,13 @@
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
-      <c r="E63" s="44">
-        <v>0</v>
-      </c>
-      <c r="F63" s="44">
-        <v>0</v>
-      </c>
-      <c r="G63" s="44">
+      <c r="E63" s="43">
+        <v>0</v>
+      </c>
+      <c r="F63" s="43">
+        <v>0</v>
+      </c>
+      <c r="G63" s="43">
         <v>0</v>
       </c>
       <c r="H63" s="11"/>
@@ -2407,13 +2396,13 @@
       <c r="B64" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="44">
-        <v>0</v>
-      </c>
-      <c r="F64" s="44">
-        <v>0</v>
-      </c>
-      <c r="G64" s="44">
+      <c r="E64" s="43">
+        <v>0</v>
+      </c>
+      <c r="F64" s="43">
+        <v>0</v>
+      </c>
+      <c r="G64" s="43">
         <v>0</v>
       </c>
       <c r="H64" s="2"/>
@@ -2428,13 +2417,13 @@
       <c r="C65" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E65" s="44">
-        <v>0</v>
-      </c>
-      <c r="F65" s="44">
-        <v>0</v>
-      </c>
-      <c r="G65" s="44">
+      <c r="E65" s="43">
+        <v>0</v>
+      </c>
+      <c r="F65" s="43">
+        <v>0</v>
+      </c>
+      <c r="G65" s="43">
         <v>0</v>
       </c>
       <c r="H65" s="2"/>
@@ -2449,13 +2438,13 @@
       <c r="C66" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="44">
-        <v>0</v>
-      </c>
-      <c r="F66" s="44">
-        <v>0</v>
-      </c>
-      <c r="G66" s="44">
+      <c r="E66" s="43">
+        <v>0</v>
+      </c>
+      <c r="F66" s="43">
+        <v>0</v>
+      </c>
+      <c r="G66" s="43">
         <v>0</v>
       </c>
       <c r="H66" s="2"/>
@@ -2470,13 +2459,13 @@
       <c r="C67" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="44">
-        <v>0</v>
-      </c>
-      <c r="F67" s="44">
-        <v>0</v>
-      </c>
-      <c r="G67" s="44">
+      <c r="E67" s="43">
+        <v>0</v>
+      </c>
+      <c r="F67" s="43">
+        <v>0</v>
+      </c>
+      <c r="G67" s="43">
         <v>0</v>
       </c>
       <c r="H67" s="2"/>
@@ -2488,13 +2477,13 @@
       <c r="C68" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E68" s="44">
-        <v>0</v>
-      </c>
-      <c r="F68" s="44">
-        <v>0</v>
-      </c>
-      <c r="G68" s="44">
+      <c r="E68" s="43">
+        <v>0</v>
+      </c>
+      <c r="F68" s="43">
+        <v>0</v>
+      </c>
+      <c r="G68" s="43">
         <v>0</v>
       </c>
       <c r="H68" s="2"/>
@@ -2507,13 +2496,13 @@
         <v>3</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="E69" s="44">
-        <v>0</v>
-      </c>
-      <c r="F69" s="44">
-        <v>0</v>
-      </c>
-      <c r="G69" s="44">
+      <c r="E69" s="43">
+        <v>0</v>
+      </c>
+      <c r="F69" s="43">
+        <v>0</v>
+      </c>
+      <c r="G69" s="43">
         <v>0</v>
       </c>
       <c r="H69" s="2"/>
@@ -2523,13 +2512,13 @@
         <v>51</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="E70" s="44">
-        <v>0</v>
-      </c>
-      <c r="F70" s="44">
-        <v>0</v>
-      </c>
-      <c r="G70" s="44">
+      <c r="E70" s="43">
+        <v>0</v>
+      </c>
+      <c r="F70" s="43">
+        <v>0</v>
+      </c>
+      <c r="G70" s="43">
         <v>0</v>
       </c>
       <c r="H70" s="2"/>
@@ -2542,13 +2531,13 @@
         <v>52</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="E71" s="44">
-        <v>0</v>
-      </c>
-      <c r="F71" s="44">
-        <v>0</v>
-      </c>
-      <c r="G71" s="44">
+      <c r="E71" s="43">
+        <v>0</v>
+      </c>
+      <c r="F71" s="43">
+        <v>0</v>
+      </c>
+      <c r="G71" s="43">
         <v>0</v>
       </c>
       <c r="H71" s="2"/>
@@ -2561,13 +2550,13 @@
         <v>53</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="E72" s="44">
-        <v>0</v>
-      </c>
-      <c r="F72" s="44">
-        <v>0</v>
-      </c>
-      <c r="G72" s="44">
+      <c r="E72" s="43">
+        <v>0</v>
+      </c>
+      <c r="F72" s="43">
+        <v>0</v>
+      </c>
+      <c r="G72" s="43">
         <v>0</v>
       </c>
       <c r="H72" s="2"/>
@@ -2579,39 +2568,39 @@
       <c r="B73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E73" s="45">
-        <v>0</v>
-      </c>
-      <c r="F73" s="45">
-        <v>0</v>
-      </c>
-      <c r="G73" s="45">
+      <c r="E73" s="44">
+        <v>0</v>
+      </c>
+      <c r="F73" s="44">
+        <v>0</v>
+      </c>
+      <c r="G73" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.44857142857142857</v>
-      </c>
-      <c r="E75" s="47">
+        <v>0.53376190476190477</v>
+      </c>
+      <c r="E75" s="46">
         <f>(SUM(E4:E73) - E54)/70</f>
         <v>0.54571428571428571</v>
       </c>
-      <c r="F75" s="48">
-        <f t="shared" ref="F75:G75" si="0">(SUM(F4:F73) - F54)/70</f>
-        <v>0.43</v>
-      </c>
-      <c r="G75" s="49">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
+      <c r="F75" s="47">
+        <f t="shared" ref="F75:G75" si="1">(SUM(F4:F73) - F54)/70</f>
+        <v>0.53142857142857147</v>
+      </c>
+      <c r="G75" s="48">
+        <f t="shared" si="1"/>
+        <v>0.52414285714285713</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 701] [Update] Correction bug mineurs
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="7500"/>
+    <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
   <si>
     <t>Stepchart</t>
   </si>
@@ -382,9 +382,6 @@
     <t>AVACEMENT PROJET</t>
   </si>
   <si>
-    <t>Tester in game</t>
-  </si>
-  <si>
     <t>Petit problème avec x8 ?</t>
   </si>
   <si>
@@ -394,10 +391,7 @@
     <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
   </si>
   <si>
-    <t>Diminuer le temps de clear, diminuer les transitions (toutes), son du fail pas assez fort, mettre le "DebugOffset" dans InGameScript (engine),  tester le startNumber, tester le "not legit !"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petit bug de transistion avec le Fade out </t>
+    <t>diminuer les transitions (toutes), son du fail pas assez fort,  tester le startNumber, tester le "not legit !", le cube n'apparait pas lors du "startNumber" souvenir, le debugOffset toujours en dessous</t>
   </si>
 </sst>
 </file>
@@ -1052,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,13 +1596,13 @@
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E28" s="33">
@@ -1617,23 +1611,21 @@
       <c r="F28" s="33">
         <v>1</v>
       </c>
-      <c r="G28" s="28">
-        <v>0.99</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="G28" s="27">
+        <v>1</v>
+      </c>
+      <c r="H28" s="20"/>
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="42"/>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="33">
@@ -1642,12 +1634,10 @@
       <c r="F29" s="33">
         <v>1</v>
       </c>
-      <c r="G29" s="28">
-        <v>0.8</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="G29" s="27">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
@@ -1755,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1790,7 +1780,7 @@
       <c r="F36" s="35"/>
       <c r="G36" s="29"/>
       <c r="H36" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1801,7 +1791,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E37" s="33">
         <v>1</v>
@@ -2023,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I46" s="8">
         <v>41252</v>
@@ -2204,7 +2194,7 @@
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.79496453900709219</v>
+        <v>0.79645390070921984</v>
       </c>
       <c r="E54" s="46">
         <f>SUM(E4:E53)/47</f>
@@ -2216,7 +2206,7 @@
       </c>
       <c r="G54" s="46">
         <f t="shared" si="0"/>
-        <v>0.7806382978723404</v>
+        <v>0.78510638297872337</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2588,7 +2578,7 @@
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.53376190476190477</v>
+        <v>0.53476190476190477</v>
       </c>
       <c r="E75" s="46">
         <f>(SUM(E4:E73) - E54)/70</f>
@@ -2600,7 +2590,7 @@
       </c>
       <c r="G75" s="48">
         <f t="shared" si="1"/>
-        <v>0.52414285714285713</v>
+        <v>0.52714285714285714</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 702] [Update] Correction de bugs mineurs Nouvelle barre de vie : code fait
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -309,10 +309,55 @@
     <t>Background à modifier</t>
   </si>
   <si>
-    <t>Faire une sorte de pile de cube. Une seule particule. Retirer un effet de bloom sur le 2 = ++ perf</t>
-  </si>
-  <si>
     <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage : A faire pour plus tard</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Augmenter les perfs</t>
+  </si>
+  <si>
+    <t>Rate placé, programme placé. Programme à compiler, à tester. Rate à tester</t>
+  </si>
+  <si>
+    <t>Mode "rapide"/Mode tapis</t>
+  </si>
+  <si>
+    <t>Sera fait plus tard</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Unity</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Verifier si la concurrence marche bien</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>AVANCEMENT DU PROJET : BUILD 1000</t>
+  </si>
+  <si>
+    <t>AVACEMENT PROJET</t>
+  </si>
+  <si>
+    <t>Petit problème avec x8 ?</t>
+  </si>
+  <si>
+    <t>OptionManager</t>
+  </si>
+  <si>
+    <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
+  </si>
+  <si>
+    <t>Pas d'idée particulière</t>
   </si>
   <si>
     <r>
@@ -333,72 +378,88 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, peut être faire en sorte de voir les medailles dans la songlist ?</t>
+      <t xml:space="preserve">, </t>
     </r>
-  </si>
-  <si>
-    <t>Faire 2 cubes, relié par un fil, et une petite boule de particule qui monte. Tube relié aux targets qui change de couleur en fonction du score. Faire un tube qui sort de l'écran. Super fil bleu si FFC, super fil jaune si FPC, fil vert si vie à fond ou entrain de remonter, cassage sinon. +2 particules jouées ensemble</t>
-  </si>
-  <si>
-    <t>Performance</t>
-  </si>
-  <si>
-    <t>Augmenter les perfs</t>
-  </si>
-  <si>
-    <t>Mettre un seul cache au lieu d'un, mettre moins de cube dans le bg</t>
-  </si>
-  <si>
-    <t>Leger bump de scale à voir si ça affecte pas les perfs</t>
-  </si>
-  <si>
-    <t>Rate placé, programme placé. Programme à compiler, à tester. Rate à tester</t>
-  </si>
-  <si>
-    <t>Mode "rapide"/Mode tapis</t>
-  </si>
-  <si>
-    <t>Sera fait plus tard</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Unity</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Verifier si la concurrence marche bien</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>AVANCEMENT DU PROJET : BUILD 1000</t>
-  </si>
-  <si>
-    <t>AVACEMENT PROJET</t>
-  </si>
-  <si>
-    <t>Petit problème avec x8 ?</t>
-  </si>
-  <si>
-    <t>OptionManager</t>
-  </si>
-  <si>
-    <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
-  </si>
-  <si>
-    <t>diminuer les transitions (toutes), son du fail pas assez fort,  tester le startNumber, tester le "not legit !", le cube n'apparait pas lors du "startNumber" souvenir, le debugOffset toujours en dessous</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>peut être faire en sorte de voir les medailles dans la songlist ?</t>
+    </r>
+  </si>
+  <si>
+    <t>Faire 2 cubes, relié par un fil, et un petit cube/particule qui monte. Tube relié aux targets qui change de couleur en fonction du score. Faire un tube qui sort de l'écran. Super fil bleu si FFC, super fil jaune si FPC, fil vert petit si vie à fond ou entrain de remonter, fil super gros + explosion si 100 combo, cassage sinon. +2 particules jouées ensemble</t>
+  </si>
+  <si>
+    <t>Faire une sorte de pile de cube. Une seule particule joué ensemble. Retirer un effet de bloom sur le 2 = ++ perf</t>
+  </si>
+  <si>
+    <t>Mettre un seul cache-chart au lieu d'un</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">diminuer les transitions (toutes), augmenter la taille de l'effet d'input, son du fail pas assez fort, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tester le "not legit !"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> le cube n'apparait pas lors du "startNumber" souvenir</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> le debugOffset toujours en dessous</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,8 +520,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +562,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -671,7 +745,6 @@
     <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -683,6 +756,8 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,13 +1156,13 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1134,7 +1209,7 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="41">
+      <c r="A6" s="40">
         <v>200</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1259,7 +1334,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="41">
+      <c r="A12" s="40">
         <v>300</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1374,11 +1449,11 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+      <c r="A18" s="40">
         <v>400</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1461,7 +1536,7 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="41">
+      <c r="A22" s="40">
         <v>500</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1552,7 +1627,7 @@
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="41">
+      <c r="A26" s="40">
         <v>600</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1618,7 +1693,7 @@
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="3" t="s">
         <v>34</v>
       </c>
@@ -1647,19 +1722,19 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E30" s="36">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F30" s="36">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G30" s="30">
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1745,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1768,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>41</v>
       </c>
@@ -1791,7 +1866,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E37" s="33">
         <v>1</v>
@@ -1830,7 +1905,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="50">
+      <c r="A39" s="49">
         <v>700</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1898,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I41" s="8"/>
     </row>
@@ -1981,14 +2056,14 @@
       <c r="E45" s="33">
         <v>1</v>
       </c>
-      <c r="F45" s="39">
-        <v>0</v>
-      </c>
-      <c r="G45" s="40">
+      <c r="F45" s="33">
+        <v>1</v>
+      </c>
+      <c r="G45" s="39">
         <v>0</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I45" s="8">
         <v>41245</v>
@@ -2013,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I46" s="8">
         <v>41252</v>
@@ -2045,30 +2120,30 @@
       <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="24" t="s">
+      <c r="B48" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="38">
-        <v>0</v>
-      </c>
-      <c r="F48" s="38">
-        <v>0</v>
-      </c>
-      <c r="G48" s="38">
+      <c r="E48" s="51">
+        <v>1</v>
+      </c>
+      <c r="F48" s="51">
+        <v>0</v>
+      </c>
+      <c r="G48" s="51">
         <v>0</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B49" s="24" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="I49" s="8"/>
     </row>
@@ -2112,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="I50" s="8"/>
     </row>
@@ -2121,10 +2196,10 @@
         <v>0</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E51" s="38">
         <v>0</v>
@@ -2136,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="I51" s="8"/>
     </row>
@@ -2160,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="I52" s="8">
         <v>41259</v>
@@ -2173,40 +2248,34 @@
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="49">
-        <v>0</v>
-      </c>
-      <c r="F53" s="49">
-        <v>0</v>
-      </c>
-      <c r="G53" s="49">
-        <v>0</v>
-      </c>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
       <c r="H53" s="11"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.79645390070921984</v>
-      </c>
-      <c r="E54" s="46">
-        <f>SUM(E4:E53)/47</f>
-        <v>0.81276595744680857</v>
-      </c>
-      <c r="F54" s="46">
-        <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/47</f>
-        <v>0.79148936170212769</v>
-      </c>
-      <c r="G54" s="46">
+        <v>0.88294573643410856</v>
+      </c>
+      <c r="E54" s="45">
+        <f>SUM(E4:E53)/43</f>
+        <v>0.90697674418604646</v>
+      </c>
+      <c r="F54" s="45">
+        <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/43</f>
+        <v>0.88372093023255816</v>
+      </c>
+      <c r="G54" s="45">
         <f t="shared" si="0"/>
-        <v>0.78510638297872337</v>
+        <v>0.85813953488372086</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2216,13 +2285,13 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G55" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2231,9 +2300,9 @@
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
       <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2246,13 +2315,13 @@
       <c r="D57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="43">
-        <v>0</v>
-      </c>
-      <c r="F57" s="43">
-        <v>0</v>
-      </c>
-      <c r="G57" s="43">
+      <c r="E57" s="42">
+        <v>0</v>
+      </c>
+      <c r="F57" s="42">
+        <v>0</v>
+      </c>
+      <c r="G57" s="42">
         <v>0</v>
       </c>
       <c r="H57" s="2"/>
@@ -2267,13 +2336,13 @@
       <c r="D58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="43">
-        <v>0</v>
-      </c>
-      <c r="F58" s="43">
-        <v>0</v>
-      </c>
-      <c r="G58" s="43">
+      <c r="E58" s="42">
+        <v>0</v>
+      </c>
+      <c r="F58" s="42">
+        <v>0</v>
+      </c>
+      <c r="G58" s="42">
         <v>0</v>
       </c>
       <c r="H58" s="2"/>
@@ -2288,13 +2357,13 @@
       <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E59" s="43">
-        <v>0</v>
-      </c>
-      <c r="F59" s="43">
-        <v>0</v>
-      </c>
-      <c r="G59" s="43">
+      <c r="E59" s="42">
+        <v>0</v>
+      </c>
+      <c r="F59" s="42">
+        <v>0</v>
+      </c>
+      <c r="G59" s="42">
         <v>0</v>
       </c>
       <c r="H59" s="2"/>
@@ -2309,13 +2378,13 @@
       <c r="D60" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E60" s="43">
-        <v>0</v>
-      </c>
-      <c r="F60" s="43">
-        <v>0</v>
-      </c>
-      <c r="G60" s="43">
+      <c r="E60" s="42">
+        <v>0</v>
+      </c>
+      <c r="F60" s="42">
+        <v>0</v>
+      </c>
+      <c r="G60" s="42">
         <v>0</v>
       </c>
       <c r="H60" s="2"/>
@@ -2328,13 +2397,13 @@
         <v>50</v>
       </c>
       <c r="D61" s="1"/>
-      <c r="E61" s="43">
-        <v>0</v>
-      </c>
-      <c r="F61" s="43">
-        <v>0</v>
-      </c>
-      <c r="G61" s="43">
+      <c r="E61" s="42">
+        <v>0</v>
+      </c>
+      <c r="F61" s="42">
+        <v>0</v>
+      </c>
+      <c r="G61" s="42">
         <v>0</v>
       </c>
       <c r="H61" s="2"/>
@@ -2350,13 +2419,13 @@
       <c r="D62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E62" s="43">
-        <v>0</v>
-      </c>
-      <c r="F62" s="43">
-        <v>0</v>
-      </c>
-      <c r="G62" s="43">
+      <c r="E62" s="42">
+        <v>0</v>
+      </c>
+      <c r="F62" s="42">
+        <v>0</v>
+      </c>
+      <c r="G62" s="42">
         <v>0</v>
       </c>
       <c r="H62" s="2"/>
@@ -2368,13 +2437,13 @@
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
-      <c r="E63" s="43">
-        <v>0</v>
-      </c>
-      <c r="F63" s="43">
-        <v>0</v>
-      </c>
-      <c r="G63" s="43">
+      <c r="E63" s="42">
+        <v>0</v>
+      </c>
+      <c r="F63" s="42">
+        <v>0</v>
+      </c>
+      <c r="G63" s="42">
         <v>0</v>
       </c>
       <c r="H63" s="11"/>
@@ -2386,13 +2455,13 @@
       <c r="B64" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="43">
-        <v>0</v>
-      </c>
-      <c r="F64" s="43">
-        <v>0</v>
-      </c>
-      <c r="G64" s="43">
+      <c r="E64" s="42">
+        <v>0</v>
+      </c>
+      <c r="F64" s="42">
+        <v>0</v>
+      </c>
+      <c r="G64" s="42">
         <v>0</v>
       </c>
       <c r="H64" s="2"/>
@@ -2407,13 +2476,13 @@
       <c r="C65" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E65" s="43">
-        <v>0</v>
-      </c>
-      <c r="F65" s="43">
-        <v>0</v>
-      </c>
-      <c r="G65" s="43">
+      <c r="E65" s="42">
+        <v>0</v>
+      </c>
+      <c r="F65" s="42">
+        <v>0</v>
+      </c>
+      <c r="G65" s="42">
         <v>0</v>
       </c>
       <c r="H65" s="2"/>
@@ -2428,13 +2497,13 @@
       <c r="C66" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="43">
-        <v>0</v>
-      </c>
-      <c r="F66" s="43">
-        <v>0</v>
-      </c>
-      <c r="G66" s="43">
+      <c r="E66" s="42">
+        <v>0</v>
+      </c>
+      <c r="F66" s="42">
+        <v>0</v>
+      </c>
+      <c r="G66" s="42">
         <v>0</v>
       </c>
       <c r="H66" s="2"/>
@@ -2449,13 +2518,13 @@
       <c r="C67" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="43">
-        <v>0</v>
-      </c>
-      <c r="F67" s="43">
-        <v>0</v>
-      </c>
-      <c r="G67" s="43">
+      <c r="E67" s="42">
+        <v>0</v>
+      </c>
+      <c r="F67" s="42">
+        <v>0</v>
+      </c>
+      <c r="G67" s="42">
         <v>0</v>
       </c>
       <c r="H67" s="2"/>
@@ -2467,13 +2536,13 @@
       <c r="C68" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E68" s="43">
-        <v>0</v>
-      </c>
-      <c r="F68" s="43">
-        <v>0</v>
-      </c>
-      <c r="G68" s="43">
+      <c r="E68" s="42">
+        <v>0</v>
+      </c>
+      <c r="F68" s="42">
+        <v>0</v>
+      </c>
+      <c r="G68" s="42">
         <v>0</v>
       </c>
       <c r="H68" s="2"/>
@@ -2486,13 +2555,13 @@
         <v>3</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="E69" s="43">
-        <v>0</v>
-      </c>
-      <c r="F69" s="43">
-        <v>0</v>
-      </c>
-      <c r="G69" s="43">
+      <c r="E69" s="42">
+        <v>0</v>
+      </c>
+      <c r="F69" s="42">
+        <v>0</v>
+      </c>
+      <c r="G69" s="42">
         <v>0</v>
       </c>
       <c r="H69" s="2"/>
@@ -2502,13 +2571,13 @@
         <v>51</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="E70" s="43">
-        <v>0</v>
-      </c>
-      <c r="F70" s="43">
-        <v>0</v>
-      </c>
-      <c r="G70" s="43">
+      <c r="E70" s="42">
+        <v>0</v>
+      </c>
+      <c r="F70" s="42">
+        <v>0</v>
+      </c>
+      <c r="G70" s="42">
         <v>0</v>
       </c>
       <c r="H70" s="2"/>
@@ -2521,13 +2590,13 @@
         <v>52</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="E71" s="43">
-        <v>0</v>
-      </c>
-      <c r="F71" s="43">
-        <v>0</v>
-      </c>
-      <c r="G71" s="43">
+      <c r="E71" s="42">
+        <v>0</v>
+      </c>
+      <c r="F71" s="42">
+        <v>0</v>
+      </c>
+      <c r="G71" s="42">
         <v>0</v>
       </c>
       <c r="H71" s="2"/>
@@ -2540,13 +2609,13 @@
         <v>53</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="E72" s="43">
-        <v>0</v>
-      </c>
-      <c r="F72" s="43">
-        <v>0</v>
-      </c>
-      <c r="G72" s="43">
+      <c r="E72" s="42">
+        <v>0</v>
+      </c>
+      <c r="F72" s="42">
+        <v>0</v>
+      </c>
+      <c r="G72" s="42">
         <v>0</v>
       </c>
       <c r="H72" s="2"/>
@@ -2558,37 +2627,37 @@
       <c r="B73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E73" s="44">
-        <v>0</v>
-      </c>
-      <c r="F73" s="44">
-        <v>0</v>
-      </c>
-      <c r="G73" s="44">
+      <c r="E73" s="43">
+        <v>0</v>
+      </c>
+      <c r="F73" s="43">
+        <v>0</v>
+      </c>
+      <c r="G73" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.53476190476190477</v>
-      </c>
-      <c r="E75" s="46">
+        <v>0.54238095238095241</v>
+      </c>
+      <c r="E75" s="45">
         <f>(SUM(E4:E73) - E54)/70</f>
-        <v>0.54571428571428571</v>
-      </c>
-      <c r="F75" s="47">
+        <v>0.55714285714285716</v>
+      </c>
+      <c r="F75" s="46">
         <f t="shared" ref="F75:G75" si="1">(SUM(F4:F73) - F54)/70</f>
-        <v>0.53142857142857147</v>
-      </c>
-      <c r="G75" s="48">
+        <v>0.54285714285714282</v>
+      </c>
+      <c r="G75" s="47">
         <f t="shared" si="1"/>
         <v>0.52714285714285714</v>
       </c>

</xml_diff>

<commit_message>
[Build 902] [Fix] Fix planning et Combo pour timebar : 40 -> 25
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
   <si>
     <t>Stepchart</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>Background à modifier</t>
-  </si>
-  <si>
-    <t>Faire 6 cubes de couleur qui grossissent en fonction de leur pourcentage : A faire pour plus tard</t>
   </si>
   <si>
     <t>Performance</t>
@@ -381,15 +378,6 @@
       </rPr>
       <t>peut être faire en sorte de voir les medailles dans la songlist ?</t>
     </r>
-  </si>
-  <si>
-    <t>Faire 2 cubes, relié par un fil, et un petit cube/particule qui monte. Tube relié aux targets qui change de couleur en fonction du score. Faire un tube qui sort de l'écran. Super fil bleu si FFC, super fil jaune si FPC, fil vert petit si vie à fond ou entrain de remonter, fil super gros + explosion si 100 combo, cassage sinon. +2 particules jouées ensemble</t>
-  </si>
-  <si>
-    <t>Faire une sorte de pile de cube. Une seule particule joué ensemble. Retirer un effet de bloom sur le 2 = ++ perf</t>
-  </si>
-  <si>
-    <t>Mettre un seul cache-chart au lieu d'un</t>
   </si>
   <si>
     <r>
@@ -428,12 +416,15 @@
   <si>
     <t>Compiler le programme une nouvelle fois et retester vite fait</t>
   </si>
+  <si>
+    <t>A tester</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -725,6 +716,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +758,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -785,7 +778,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -874,6 +867,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -908,6 +902,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1083,14 +1078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
@@ -1102,12 +1097,12 @@
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1121,13 +1116,13 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
         <v>100</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>101</v>
-      </c>
-      <c r="G3" t="s">
-        <v>102</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1136,7 +1131,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30.75" customHeight="1">
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1173,7 +1168,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>200</v>
       </c>
@@ -1195,7 +1190,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1214,7 +1209,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1230,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1251,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1270,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1298,7 +1293,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>300</v>
       </c>
@@ -1320,7 +1315,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
@@ -1339,7 +1334,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
@@ -1358,7 +1353,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1377,7 +1372,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1391,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1414,10 +1409,10 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
         <v>400</v>
       </c>
@@ -1439,7 +1434,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
@@ -1459,7 +1454,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
@@ -1480,7 +1475,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1500,7 +1495,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>500</v>
       </c>
@@ -1525,7 +1520,7 @@
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
@@ -1547,7 +1542,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>28</v>
       </c>
@@ -1569,7 +1564,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1591,7 +1586,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
         <v>600</v>
       </c>
@@ -1616,7 +1611,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
         <v>65</v>
@@ -1635,7 +1630,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
@@ -1657,7 +1652,7 @@
       <c r="H28" s="20"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
       <c r="B29" s="3" t="s">
         <v>34</v>
@@ -1679,7 +1674,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
         <v>34</v>
       </c>
@@ -1687,22 +1682,22 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="36">
+        <v>0</v>
+      </c>
+      <c r="F30" s="36">
+        <v>0</v>
+      </c>
+      <c r="G30" s="30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E30" s="36">
-        <v>0</v>
-      </c>
-      <c r="F30" s="36">
-        <v>0</v>
-      </c>
-      <c r="G30" s="30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
@@ -1723,7 +1718,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>34</v>
       </c>
@@ -1744,7 +1739,7 @@
       </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>34</v>
       </c>
@@ -1765,7 +1760,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>34</v>
       </c>
@@ -1785,10 +1780,10 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>84</v>
       </c>
@@ -1808,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="45">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>41</v>
       </c>
@@ -1820,10 +1815,10 @@
       <c r="F36" s="35"/>
       <c r="G36" s="29"/>
       <c r="H36" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>41</v>
       </c>
@@ -1831,7 +1826,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="33">
         <v>1</v>
@@ -1844,7 +1839,7 @@
       </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>88</v>
       </c>
@@ -1865,7 +1860,7 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="48">
         <v>700</v>
       </c>
@@ -1891,7 +1886,7 @@
         <v>41231</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>0</v>
       </c>
@@ -1913,29 +1908,27 @@
       <c r="H40" s="2"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
-      <c r="B41" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="36">
-        <v>0</v>
-      </c>
-      <c r="F41" s="36">
-        <v>0</v>
-      </c>
-      <c r="G41" s="36">
-        <v>0</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="E41" s="41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="41">
+        <v>0</v>
+      </c>
+      <c r="G41" s="41">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1948,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>19</v>
       </c>
@@ -1976,8 +1969,8 @@
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="39">
         <v>800</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -2001,7 +1994,7 @@
         <v>41238</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>19</v>
       </c>
@@ -2019,14 +2012,14 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I45" s="8">
         <v>41245</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="39">
         <v>900</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -2044,13 +2037,13 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I46" s="8">
         <v>41252</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -2075,31 +2068,32 @@
       </c>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
-      <c r="B48" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="49" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="49" t="s">
+      <c r="D48" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E48" s="50">
-        <v>1</v>
-      </c>
-      <c r="F48" s="50">
-        <v>0</v>
-      </c>
-      <c r="G48" s="50">
-        <v>0</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="E48" s="33">
+        <v>1</v>
+      </c>
+      <c r="F48" s="33">
+        <v>1</v>
+      </c>
+      <c r="G48" s="33">
+        <v>1</v>
+      </c>
+      <c r="H48" s="2"/>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="1:9" ht="90">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="52">
+        <v>901</v>
+      </c>
       <c r="B49" s="49" t="s">
         <v>0</v>
       </c>
@@ -2113,17 +2107,17 @@
         <v>1</v>
       </c>
       <c r="F49" s="50">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G49" s="50">
         <v>0</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" s="24" t="s">
         <v>0</v>
       </c>
@@ -2143,20 +2137,20 @@
         <v>0</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I50" s="8"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="24" t="s">
-        <v>97</v>
-      </c>
       <c r="E51" s="38">
         <v>0</v>
       </c>
@@ -2166,12 +2160,10 @@
       <c r="G51" s="38">
         <v>0</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="H51" s="2"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1000</v>
       </c>
@@ -2191,13 +2183,13 @@
         <v>0</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I52" s="8">
         <v>41259</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1">
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>45</v>
@@ -2209,17 +2201,17 @@
       <c r="G53" s="47"/>
       <c r="H53" s="11"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1">
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="24" t="s">
         <v>104</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.89844961240310084</v>
+        <v>0.91782945736434096</v>
       </c>
       <c r="E54" s="44">
         <f>SUM(E4:E53)/43</f>
@@ -2227,31 +2219,31 @@
       </c>
       <c r="F54" s="44">
         <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/43</f>
-        <v>0.88372093023255816</v>
+        <v>0.91860465116279066</v>
       </c>
       <c r="G54" s="44">
         <f t="shared" si="0"/>
-        <v>0.88139534883720927</v>
+        <v>0.90465116279069768</v>
       </c>
       <c r="H54" s="20"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="G55" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="G55" s="31" t="s">
-        <v>102</v>
-      </c>
       <c r="H55" s="20"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -2261,7 +2253,7 @@
       <c r="G56" s="43"/>
       <c r="H56" s="20"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2274,7 @@
       </c>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2295,7 @@
       </c>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>19</v>
       </c>
@@ -2324,7 +2316,7 @@
       </c>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>26</v>
       </c>
@@ -2345,7 +2337,7 @@
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>6</v>
       </c>
@@ -2364,7 +2356,7 @@
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2000</v>
       </c>
@@ -2386,7 +2378,7 @@
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="12" t="s">
         <v>67</v>
@@ -2404,7 +2396,7 @@
       </c>
       <c r="H63" s="11"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3000</v>
       </c>
@@ -2422,7 +2414,7 @@
       </c>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4000</v>
       </c>
@@ -2443,7 +2435,7 @@
       </c>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5000</v>
       </c>
@@ -2464,7 +2456,7 @@
       </c>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>6000</v>
       </c>
@@ -2485,7 +2477,7 @@
       </c>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>0</v>
       </c>
@@ -2503,7 +2495,7 @@
       </c>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7000</v>
       </c>
@@ -2522,7 +2514,7 @@
       </c>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>51</v>
       </c>
@@ -2538,7 +2530,7 @@
       </c>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>54</v>
       </c>
@@ -2557,7 +2549,7 @@
       </c>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -2576,7 +2568,7 @@
       </c>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -2593,17 +2585,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="75" spans="1:8" ht="15.75" thickBot="1">
+    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.5519047619047619</v>
+        <v>0.56380952380952376</v>
       </c>
       <c r="E75" s="44">
         <f>(SUM(E4:E73) - E54)/70</f>
@@ -2611,150 +2603,150 @@
       </c>
       <c r="F75" s="45">
         <f t="shared" ref="F75:G75" si="1">(SUM(F4:F73) - F54)/70</f>
-        <v>0.54285714285714282</v>
+        <v>0.56428571428571428</v>
       </c>
       <c r="G75" s="46">
         <f t="shared" si="1"/>
-        <v>0.54142857142857137</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>0.55571428571428572</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" s="15"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" s="15"/>
       <c r="C80" s="7"/>
       <c r="D80" s="17"/>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="19"/>
       <c r="D81" s="17"/>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="19"/>
       <c r="D82" s="16"/>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="D83" s="18"/>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="15"/>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="15"/>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="15"/>
     </row>
-    <row r="87" spans="2:4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="15"/>
     </row>
-    <row r="88" spans="2:4">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="15"/>
     </row>
-    <row r="89" spans="2:4">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="15"/>
     </row>
-    <row r="90" spans="2:4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="15"/>
     </row>
-    <row r="91" spans="2:4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="15"/>
     </row>
-    <row r="92" spans="2:4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="15"/>
     </row>
-    <row r="93" spans="2:4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="15"/>
     </row>
-    <row r="94" spans="2:4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="15"/>
     </row>
-    <row r="95" spans="2:4">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="15"/>
     </row>
-    <row r="96" spans="2:4">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="15"/>
     </row>
-    <row r="97" spans="2:2">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="15"/>
     </row>
-    <row r="98" spans="2:2">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="15"/>
     </row>
-    <row r="99" spans="2:2">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="15"/>
     </row>
-    <row r="100" spans="2:2">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="15"/>
     </row>
-    <row r="101" spans="2:2">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="15"/>
     </row>
-    <row r="102" spans="2:2">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="15"/>
     </row>
-    <row r="103" spans="2:2">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="15"/>
     </row>
-    <row r="104" spans="2:2">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="15"/>
     </row>
-    <row r="105" spans="2:2">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="15"/>
     </row>
-    <row r="106" spans="2:2">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="15"/>
     </row>
-    <row r="107" spans="2:2">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="15"/>
     </row>
-    <row r="108" spans="2:2">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="15"/>
     </row>
-    <row r="109" spans="2:2">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" s="15"/>
     </row>
-    <row r="110" spans="2:2">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="15"/>
     </row>
-    <row r="111" spans="2:2">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="15"/>
     </row>
-    <row r="112" spans="2:2">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="15"/>
     </row>
-    <row r="113" spans="2:2">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="15"/>
     </row>
-    <row r="114" spans="2:2">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="15"/>
     </row>
-    <row r="115" spans="2:2">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="15"/>
     </row>
-    <row r="116" spans="2:2">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="15"/>
     </row>
-    <row r="117" spans="2:2">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="15"/>
     </row>
-    <row r="118" spans="2:2">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="15"/>
     </row>
-    <row r="119" spans="2:2">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="15"/>
     </row>
-    <row r="120" spans="2:2">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="15"/>
     </row>
-    <row r="121" spans="2:2">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="15"/>
     </row>
-    <row r="122" spans="2:2">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="15"/>
     </row>
   </sheetData>
@@ -3079,24 +3071,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Build 904] [Update] Ajout du quick mode, empechement de mettre 2 fois la même touche
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="116">
   <si>
     <t>Stepchart</t>
   </si>
@@ -309,9 +309,6 @@
     <t>Augmenter les perfs</t>
   </si>
   <si>
-    <t>Mode "rapide"/Mode tapis</t>
-  </si>
-  <si>
     <t>Sera fait plus tard</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Verifier si la concurrence marche bien</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -343,9 +337,6 @@
   </si>
   <si>
     <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
-  </si>
-  <si>
-    <t>Pas d'idée particulière</t>
   </si>
   <si>
     <r>
@@ -386,9 +377,6 @@
     <t>La brillance chie encore un peu</t>
   </si>
   <si>
-    <t>Pas sur que tout marche</t>
-  </si>
-  <si>
     <r>
       <t>son du fail pas assez fort,</t>
     </r>
@@ -419,8 +407,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, faire en sorte qu'on ne puisse pas attribuer 2 fois le meme input sur un seul truc</t>
+      <t xml:space="preserve">, </t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>faire en sorte qu'on ne puisse pas attribuer 2 fois le meme input sur un seul truc</t>
+    </r>
+  </si>
+  <si>
+    <t>Plus tard</t>
+  </si>
+  <si>
+    <t>Verifier si la concurrence marche bien (attendre le Online)</t>
+  </si>
+  <si>
+    <t>A tester</t>
+  </si>
+  <si>
+    <t>Mode "rapide"</t>
+  </si>
+  <si>
+    <t>Mode tapis</t>
   </si>
 </sst>
 </file>
@@ -649,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -721,6 +734,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,13 +755,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1082,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,13 +1133,13 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
         <v>99</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>100</v>
-      </c>
-      <c r="G3" t="s">
-        <v>101</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1412,7 +1426,7 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1685,41 +1699,43 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="36">
+        <v>0</v>
+      </c>
+      <c r="F30" s="36">
+        <v>0</v>
+      </c>
+      <c r="G30" s="30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="36">
-        <v>0</v>
-      </c>
-      <c r="F30" s="36">
-        <v>0</v>
-      </c>
-      <c r="G30" s="30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="33">
-        <v>1</v>
-      </c>
-      <c r="F31" s="33">
-        <v>1</v>
-      </c>
-      <c r="G31" s="27">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2"/>
+      <c r="D31" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="35">
+        <v>1</v>
+      </c>
+      <c r="F31" s="35">
+        <v>1</v>
+      </c>
+      <c r="G31" s="28">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
@@ -1729,7 +1745,7 @@
         <v>29</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E32" s="33">
         <v>1</v>
@@ -1750,7 +1766,7 @@
         <v>29</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="E33" s="33">
         <v>1</v>
@@ -1771,7 +1787,7 @@
         <v>29</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="E34" s="33">
         <v>1</v>
@@ -1782,170 +1798,169 @@
       <c r="G34" s="27">
         <v>1</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="33">
+        <v>1</v>
+      </c>
+      <c r="F35" s="33">
+        <v>1</v>
+      </c>
+      <c r="G35" s="27">
+        <v>1</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="33">
-        <v>1</v>
-      </c>
-      <c r="F35" s="33">
-        <v>1</v>
-      </c>
-      <c r="G35" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
+      <c r="E36" s="33">
+        <v>1</v>
+      </c>
+      <c r="F36" s="33">
+        <v>1</v>
+      </c>
+      <c r="G36" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C37" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="33">
-        <v>1</v>
-      </c>
-      <c r="F37" s="33">
-        <v>1</v>
-      </c>
-      <c r="G37" s="27">
-        <v>1</v>
-      </c>
-      <c r="H37" s="2"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="33">
+        <v>1</v>
+      </c>
+      <c r="F38" s="33">
+        <v>1</v>
+      </c>
+      <c r="G38" s="27">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="33">
-        <v>1</v>
-      </c>
-      <c r="F38" s="33">
-        <v>1</v>
-      </c>
-      <c r="G38" s="27">
-        <v>1</v>
-      </c>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="48">
+      <c r="E39" s="33">
+        <v>1</v>
+      </c>
+      <c r="F39" s="33">
+        <v>1</v>
+      </c>
+      <c r="G39" s="27">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="48">
         <v>700</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E39" s="33">
-        <v>1</v>
-      </c>
-      <c r="F39" s="33">
-        <v>1</v>
-      </c>
-      <c r="G39" s="27">
-        <v>1</v>
-      </c>
-      <c r="I39" s="8">
-        <v>41231</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="E40" s="33">
+        <v>1</v>
+      </c>
+      <c r="F40" s="33">
+        <v>1</v>
+      </c>
+      <c r="G40" s="27">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="34">
-        <v>1</v>
-      </c>
-      <c r="F40" s="34">
-        <v>1</v>
-      </c>
-      <c r="G40" s="34">
-        <v>1</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="E41" s="41">
-        <v>0</v>
-      </c>
-      <c r="F41" s="41">
-        <v>0</v>
-      </c>
-      <c r="G41" s="41">
-        <v>0</v>
+      <c r="E41" s="34">
+        <v>1</v>
+      </c>
+      <c r="F41" s="34">
+        <v>1</v>
+      </c>
+      <c r="G41" s="34">
+        <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="8"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="37">
-        <v>0</v>
-      </c>
-      <c r="F42" s="37">
-        <v>0</v>
-      </c>
-      <c r="G42" s="37">
+      <c r="B42" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="41">
+        <v>0</v>
+      </c>
+      <c r="F42" s="41">
+        <v>0</v>
+      </c>
+      <c r="G42" s="41">
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
@@ -1953,83 +1968,76 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="37">
+        <v>0</v>
+      </c>
+      <c r="F43" s="37">
+        <v>0</v>
+      </c>
+      <c r="G43" s="37">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="37">
-        <v>0</v>
-      </c>
-      <c r="F43" s="37">
-        <v>0</v>
-      </c>
-      <c r="G43" s="37">
-        <v>0</v>
-      </c>
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="39">
+      <c r="E44" s="37">
+        <v>0</v>
+      </c>
+      <c r="F44" s="37">
+        <v>0</v>
+      </c>
+      <c r="G44" s="37">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="39">
         <v>800</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6" t="s">
+      <c r="C45" s="6"/>
+      <c r="D45" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="33">
-        <v>1</v>
-      </c>
-      <c r="F44" s="33">
-        <v>1</v>
-      </c>
-      <c r="G44" s="27">
-        <v>1</v>
-      </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="8">
-        <v>41238</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
+      <c r="E45" s="33">
+        <v>1</v>
+      </c>
+      <c r="F45" s="33">
+        <v>1</v>
+      </c>
+      <c r="G45" s="27">
+        <v>1</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="33">
-        <v>1</v>
-      </c>
-      <c r="F45" s="33">
-        <v>1</v>
-      </c>
-      <c r="G45" s="27">
-        <v>1</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I45" s="8">
-        <v>41245</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="39">
-        <v>900</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
+      <c r="D46" s="3"/>
       <c r="E46" s="33">
         <v>1</v>
       </c>
@@ -2042,63 +2050,57 @@
       <c r="H46" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I46" s="8">
-        <v>41252</v>
-      </c>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="39">
+        <v>900</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="33">
+        <v>1</v>
+      </c>
+      <c r="F47" s="33">
+        <v>1</v>
+      </c>
+      <c r="G47" s="27">
+        <v>1</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B48" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C48" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="36">
-        <v>0</v>
-      </c>
-      <c r="F47" s="36">
-        <v>0</v>
-      </c>
-      <c r="G47" s="36">
-        <v>0</v>
-      </c>
-      <c r="H47" s="2" t="s">
+      <c r="D48" s="21"/>
+      <c r="E48" s="36">
+        <v>0</v>
+      </c>
+      <c r="F48" s="36">
+        <v>0</v>
+      </c>
+      <c r="G48" s="36">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" s="52">
-        <v>1</v>
-      </c>
-      <c r="F48" s="52">
-        <v>1</v>
-      </c>
-      <c r="G48" s="52">
-        <v>0.9</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="I48" s="8"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="50">
-        <v>901</v>
-      </c>
       <c r="B49" s="51" t="s">
         <v>0</v>
       </c>
@@ -2106,145 +2108,152 @@
         <v>91</v>
       </c>
       <c r="D49" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49" s="52">
+        <v>1</v>
+      </c>
+      <c r="F49" s="52">
+        <v>1</v>
+      </c>
+      <c r="G49" s="53">
+        <v>0.9</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="50">
+        <v>901</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="52">
-        <v>1</v>
-      </c>
-      <c r="F49" s="52">
-        <v>1</v>
-      </c>
-      <c r="G49" s="52">
-        <v>0.9</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="24" t="s">
+      <c r="E50" s="33">
+        <v>1</v>
+      </c>
+      <c r="F50" s="33">
+        <v>1</v>
+      </c>
+      <c r="G50" s="33">
+        <v>1</v>
+      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D50" s="24" t="s">
+      <c r="D51" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E50" s="38">
-        <v>0</v>
-      </c>
-      <c r="F50" s="38">
-        <v>0</v>
-      </c>
-      <c r="G50" s="38">
-        <v>0</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I50" s="8"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="24" t="s">
+      <c r="E51" s="36">
+        <v>1</v>
+      </c>
+      <c r="F51" s="36">
+        <v>1</v>
+      </c>
+      <c r="G51" s="36">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D52" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="38">
-        <v>0</v>
-      </c>
-      <c r="F51" s="38">
-        <v>0</v>
-      </c>
-      <c r="G51" s="38">
-        <v>0</v>
-      </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="8"/>
-    </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="E52" s="41">
+        <v>1</v>
+      </c>
+      <c r="F52" s="41">
+        <v>1</v>
+      </c>
+      <c r="G52" s="41">
+        <v>1</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>1000</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>41</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="38">
-        <v>0</v>
-      </c>
-      <c r="F52" s="38">
-        <v>0</v>
-      </c>
-      <c r="G52" s="38">
-        <v>0</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I52" s="8">
-        <v>41259</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10" t="s">
+      <c r="E53" s="38">
+        <v>0</v>
+      </c>
+      <c r="F53" s="38">
+        <v>0</v>
+      </c>
+      <c r="G53" s="38">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="11"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="25">
-        <f>SUM(E54:G54)/3</f>
-        <v>0.9279069767441861</v>
-      </c>
-      <c r="E54" s="44">
-        <f>SUM(E4:E53)/43</f>
-        <v>0.93023255813953487</v>
-      </c>
-      <c r="F54" s="44">
-        <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/43</f>
-        <v>0.93023255813953487</v>
-      </c>
-      <c r="G54" s="44">
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="11"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="25">
+        <f>SUM(E55:G55)/3</f>
+        <v>0.99069767441860457</v>
+      </c>
+      <c r="E55" s="44">
+        <f>SUM(E4:E54)/43</f>
+        <v>1</v>
+      </c>
+      <c r="F55" s="44">
+        <f t="shared" ref="F55:G55" si="0">SUM(F4:F54)/43</f>
+        <v>1</v>
+      </c>
+      <c r="G55" s="44">
         <f t="shared" si="0"/>
-        <v>0.92325581395348832</v>
-      </c>
-      <c r="H54" s="20"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F55" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>101</v>
+        <v>0.97209302325581393</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2253,41 +2262,36 @@
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="E56" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E57" s="41">
-        <v>0</v>
-      </c>
-      <c r="F57" s="41">
-        <v>0</v>
-      </c>
-      <c r="G57" s="41">
-        <v>0</v>
-      </c>
-      <c r="H57" s="2"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="20"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E58" s="41">
         <v>0</v>
@@ -2302,7 +2306,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>44</v>
@@ -2323,7 +2327,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>44</v>
@@ -2344,70 +2348,73 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="41">
+        <v>0</v>
+      </c>
+      <c r="F61" s="41">
+        <v>0</v>
+      </c>
+      <c r="G61" s="41">
+        <v>0</v>
+      </c>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="41">
-        <v>0</v>
-      </c>
-      <c r="F61" s="41">
-        <v>0</v>
-      </c>
-      <c r="G61" s="41">
-        <v>0</v>
-      </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="D62" s="1"/>
+      <c r="E62" s="41">
+        <v>0</v>
+      </c>
+      <c r="F62" s="41">
+        <v>0</v>
+      </c>
+      <c r="G62" s="41">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>2000</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E62" s="41">
-        <v>0</v>
-      </c>
-      <c r="F62" s="41">
-        <v>0</v>
-      </c>
-      <c r="G62" s="41">
-        <v>0</v>
-      </c>
-      <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-      <c r="B63" s="12" t="s">
+      <c r="E63" s="41">
+        <v>0</v>
+      </c>
+      <c r="F63" s="41">
+        <v>0</v>
+      </c>
+      <c r="G63" s="41">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="41">
-        <v>0</v>
-      </c>
-      <c r="F63" s="41">
-        <v>0</v>
-      </c>
-      <c r="G63" s="41">
-        <v>0</v>
-      </c>
-      <c r="H63" s="11"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>3000</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
       <c r="E64" s="41">
         <v>0</v>
       </c>
@@ -2417,17 +2424,14 @@
       <c r="G64" s="41">
         <v>0</v>
       </c>
-      <c r="H64" s="2"/>
+      <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E65" s="41">
         <v>0</v>
@@ -2442,13 +2446,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="E66" s="41">
         <v>0</v>
@@ -2463,65 +2467,70 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
+        <v>5000</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="41">
+        <v>0</v>
+      </c>
+      <c r="F67" s="41">
+        <v>0</v>
+      </c>
+      <c r="G67" s="41">
+        <v>0</v>
+      </c>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>6000</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="B68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="41">
-        <v>0</v>
-      </c>
-      <c r="F67" s="41">
-        <v>0</v>
-      </c>
-      <c r="G67" s="41">
-        <v>0</v>
-      </c>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="E68" s="41">
+        <v>0</v>
+      </c>
+      <c r="F68" s="41">
+        <v>0</v>
+      </c>
+      <c r="G68" s="41">
+        <v>0</v>
+      </c>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E68" s="41">
-        <v>0</v>
-      </c>
-      <c r="F68" s="41">
-        <v>0</v>
-      </c>
-      <c r="G68" s="41">
-        <v>0</v>
-      </c>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="E69" s="41">
+        <v>0</v>
+      </c>
+      <c r="F69" s="41">
+        <v>0</v>
+      </c>
+      <c r="G69" s="41">
+        <v>0</v>
+      </c>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>7000</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="E69" s="41">
-        <v>0</v>
-      </c>
-      <c r="F69" s="41">
-        <v>0</v>
-      </c>
-      <c r="G69" s="41">
-        <v>0</v>
-      </c>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C70" s="1"/>
       <c r="E70" s="41">
@@ -2536,11 +2545,8 @@
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>54</v>
-      </c>
       <c r="B71" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C71" s="1"/>
       <c r="E71" s="41">
@@ -2556,10 +2562,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C72" s="1"/>
       <c r="E72" s="41">
@@ -2575,70 +2581,86 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>55</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="E73" s="41">
+        <v>0</v>
+      </c>
+      <c r="F73" s="41">
+        <v>0</v>
+      </c>
+      <c r="G73" s="41">
+        <v>0</v>
+      </c>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>63</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E73" s="42">
-        <v>0</v>
-      </c>
-      <c r="F73" s="42">
-        <v>0</v>
-      </c>
-      <c r="G73" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="E74" s="42">
+        <v>0</v>
+      </c>
+      <c r="F74" s="42">
+        <v>0</v>
+      </c>
+      <c r="G74" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D75" s="25">
-        <f>SUM(E75:G75)/3</f>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E75" s="44">
-        <f>(SUM(E4:E73) - E54)/70</f>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F75" s="45">
-        <f t="shared" ref="F75:G75" si="1">(SUM(F4:F73) - F54)/70</f>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="G75" s="46">
+      <c r="D76" s="25">
+        <f>SUM(E76:G76)/3</f>
+        <v>0.60857142857142854</v>
+      </c>
+      <c r="E76" s="44">
+        <f>(SUM(E4:E74) - E55)/70</f>
+        <v>0.61428571428571432</v>
+      </c>
+      <c r="F76" s="45">
+        <f t="shared" ref="F76:G76" si="1">(SUM(F4:F74) - F55)/70</f>
+        <v>0.61428571428571432</v>
+      </c>
+      <c r="G76" s="46">
         <f t="shared" si="1"/>
-        <v>0.56714285714285706</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="15"/>
+        <v>0.59714285714285709</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" s="15"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="17"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="2"/>
-      <c r="C81" s="19"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="7"/>
       <c r="D81" s="17"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="19"/>
-      <c r="D82" s="16"/>
+      <c r="D82" s="17"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
-      <c r="D83" s="18"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="16"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="15"/>
+      <c r="B84" s="2"/>
+      <c r="D84" s="18"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="15"/>
@@ -2754,8 +2776,11 @@
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="15"/>
     </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="15"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E54:G54">
+  <conditionalFormatting sqref="E55:G55">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2817,7 +2842,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
+  <conditionalFormatting sqref="D55">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2831,7 +2856,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75:G75">
+  <conditionalFormatting sqref="E76:G76">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2893,7 +2918,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
+  <conditionalFormatting sqref="D76">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2974,7 +2999,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E54:G54</xm:sqref>
+          <xm:sqref>E55:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5A155569-3F76-4DAA-AF02-FE2CF93C93EA}">
@@ -2989,7 +3014,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D54</xm:sqref>
+          <xm:sqref>D55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{52C67A8B-2070-4790-AFC0-589F7B90CF9A}">
@@ -3052,7 +3077,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E75:G75</xm:sqref>
+          <xm:sqref>E76:G76</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0902D927-E259-4C22-AC26-A2682B1E694E}">
@@ -3067,7 +3092,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D75</xm:sqref>
+          <xm:sqref>D76</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
[Build 905] [Update] Correction des derniers bugs à tester et à faire des trucs dans Unity maintenant
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -333,10 +333,25 @@
     <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
   </si>
   <si>
-    <t>Compiler le programme une nouvelle fois et retester vite fait</t>
-  </si>
-  <si>
     <t>La brillance chie encore un peu</t>
+  </si>
+  <si>
+    <t>Plus tard</t>
+  </si>
+  <si>
+    <t>Verifier si la concurrence marche bien (attendre le Online)</t>
+  </si>
+  <si>
+    <t>A tester</t>
+  </si>
+  <si>
+    <t>Mode "rapide"</t>
+  </si>
+  <si>
+    <t>Mode tapis</t>
+  </si>
+  <si>
+    <t>Retester vite fait</t>
   </si>
   <si>
     <r>
@@ -369,36 +384,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t/>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>faire en sorte qu'on ne puisse pas attribuer 2 fois le meme input sur un seul truc</t>
-    </r>
-  </si>
-  <si>
-    <t>Plus tard</t>
-  </si>
-  <si>
-    <t>Verifier si la concurrence marche bien (attendre le Online)</t>
-  </si>
-  <si>
-    <t>A tester</t>
-  </si>
-  <si>
-    <t>Mode "rapide"</t>
-  </si>
-  <si>
-    <t>Mode tapis</t>
-  </si>
-  <si>
-    <t>Modifier les settings de qualité, corriger le problème des banners qui ne s'affichent pas, verifier que y a au moins un pack</t>
+  </si>
+  <si>
+    <t>Modifier les settings de qualité, corriger le problème des banners qui ne s'affichent pas</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1366,7 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1649,7 +1639,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E30" s="36">
         <v>0</v>
@@ -1672,7 +1662,7 @@
         <v>29</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
@@ -1684,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1793,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
         <v>41</v>
       </c>
@@ -1805,7 +1795,7 @@
       <c r="F37" s="35"/>
       <c r="G37" s="29"/>
       <c r="H37" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1995,10 +1985,10 @@
         <v>1</v>
       </c>
       <c r="G46" s="28">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="I46" s="8"/>
     </row>
@@ -2070,7 +2060,7 @@
         <v>0.9</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I49" s="8"/>
     </row>
@@ -2119,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I51" s="8"/>
     </row>
@@ -2169,7 +2159,7 @@
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.9446969696969697</v>
+        <v>0.94507575757575768</v>
       </c>
       <c r="E54" s="44">
         <f>SUM(E4:E53)/44</f>
@@ -2181,7 +2171,7 @@
       </c>
       <c r="G54" s="44">
         <f t="shared" si="0"/>
-        <v>0.92499999999999993</v>
+        <v>0.92613636363636365</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2553,7 +2543,7 @@
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.59380952380952379</v>
+        <v>0.59404761904761905</v>
       </c>
       <c r="E75" s="44">
         <f>(SUM(E4:E73) - E54)/70</f>
@@ -2565,7 +2555,7 @@
       </c>
       <c r="G75" s="46">
         <f>(SUM(G4:G73) - G54)/70</f>
-        <v>0.58142857142857141</v>
+        <v>0.58214285714285718</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 906] [Update] Correction de la brillance, reste 2 bugs
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
   <si>
     <t>Stepchart</t>
   </si>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>Peut être moyen d'optimiser ? 1750 song = 16 secondes</t>
-  </si>
-  <si>
-    <t>La brillance chie encore un peu</t>
   </si>
   <si>
     <t>Plus tard</t>
@@ -604,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -674,7 +671,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1362,7 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1639,7 +1635,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="36">
         <v>0</v>
@@ -1662,7 +1658,7 @@
         <v>29</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
@@ -1674,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1795,7 +1791,7 @@
       <c r="F37" s="35"/>
       <c r="G37" s="29"/>
       <c r="H37" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1988,7 +1984,7 @@
         <v>0.95</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I46" s="8"/>
     </row>
@@ -2041,13 +2037,13 @@
       <c r="I48" s="8"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="23" t="s">
+      <c r="B49" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="6" t="s">
         <v>92</v>
       </c>
       <c r="E49" s="33">
@@ -2056,17 +2052,15 @@
       <c r="F49" s="33">
         <v>1</v>
       </c>
-      <c r="G49" s="51">
-        <v>0.9</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="G49" s="33">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2"/>
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="50">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>0</v>
@@ -2109,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I51" s="8"/>
     </row>
@@ -2133,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I52" s="8"/>
     </row>
@@ -2159,7 +2153,7 @@
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.94507575757575768</v>
+        <v>0.94583333333333341</v>
       </c>
       <c r="E54" s="44">
         <f>SUM(E4:E53)/44</f>
@@ -2171,7 +2165,7 @@
       </c>
       <c r="G54" s="44">
         <f t="shared" si="0"/>
-        <v>0.92613636363636365</v>
+        <v>0.92840909090909096</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2543,7 +2537,7 @@
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.59404761904761905</v>
+        <v>0.59452380952380957</v>
       </c>
       <c r="E75" s="44">
         <f>(SUM(E4:E73) - E54)/70</f>
@@ -2555,7 +2549,7 @@
       </c>
       <c r="G75" s="46">
         <f>(SUM(G4:G73) - G54)/70</f>
-        <v>0.58214285714285718</v>
+        <v>0.58357142857142863</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build 907] [Update] Correction du rate, correction du baseCube Reste à corriger les banners qui n'apparaissent pas, la qualité et tester le mode rapide
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -348,31 +348,11 @@
     <t>Mode tapis</t>
   </si>
   <si>
-    <t>Retester vite fait</t>
+    <t>Modifier les settings de qualité, corriger le problème des banners qui ne s'affichent pas</t>
   </si>
   <si>
     <r>
-      <t>son du fail pas assez fort,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>le cube ne descend pas/n'apparait pas lors du "startNumber" souvenir</t>
+      <t>son du fail pas assez fort</t>
     </r>
     <r>
       <rPr>
@@ -385,14 +365,14 @@
     </r>
   </si>
   <si>
-    <t>Modifier les settings de qualité, corriger le problème des banners qui ne s'affichent pas</t>
+    <t>Tester en jeu mais normalement tout va bien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,13 +422,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1034,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
         <v>41</v>
       </c>
@@ -1981,10 +1954,10 @@
         <v>1</v>
       </c>
       <c r="G46" s="28">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I46" s="8"/>
     </row>
@@ -2127,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I52" s="8"/>
     </row>
@@ -2153,7 +2126,7 @@
       <c r="C54" s="9"/>
       <c r="D54" s="25">
         <f>SUM(E54:G54)/3</f>
-        <v>0.94583333333333341</v>
+        <v>0.94613636363636366</v>
       </c>
       <c r="E54" s="44">
         <f>SUM(E4:E53)/44</f>
@@ -2165,7 +2138,7 @@
       </c>
       <c r="G54" s="44">
         <f t="shared" si="0"/>
-        <v>0.92840909090909096</v>
+        <v>0.92931818181818182</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2537,7 +2510,7 @@
       </c>
       <c r="D75" s="25">
         <f>SUM(E75:G75)/3</f>
-        <v>0.59452380952380957</v>
+        <v>0.59471428571428575</v>
       </c>
       <c r="E75" s="44">
         <f>(SUM(E4:E73) - E54)/70</f>
@@ -2549,7 +2522,7 @@
       </c>
       <c r="G75" s="46">
         <f>(SUM(G4:G73) - G54)/70</f>
-        <v>0.58357142857142863</v>
+        <v>0.58414285714285719</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build Release Candidate] [Update] Correction des derniers bugs Reste le panneau qui se s'affiche pas quand on clique sur une fleche, le panneau incoming est manquant + le compte des Hands ne se fait pas bien
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="111">
   <si>
     <t>Stepchart</t>
   </si>
@@ -339,16 +339,10 @@
     <t>Verifier si la concurrence marche bien (attendre le Online)</t>
   </si>
   <si>
-    <t>A tester</t>
-  </si>
-  <si>
     <t>Mode "rapide"</t>
   </si>
   <si>
     <t>Mode tapis</t>
-  </si>
-  <si>
-    <t>Modifier les settings de qualité, corriger le problème des banners qui ne s'affichent pas</t>
   </si>
   <si>
     <r>
@@ -365,7 +359,7 @@
     </r>
   </si>
   <si>
-    <t>Tester en jeu mais normalement tout va bien</t>
+    <t>Corriger le problème des banners qui ne s'affichent pas, Les hands ne se comptent pas correctement</t>
   </si>
 </sst>
 </file>
@@ -574,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -616,19 +610,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1007,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,13 +1056,13 @@
       <c r="D4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="32">
-        <v>1</v>
-      </c>
-      <c r="F4" s="32">
-        <v>1</v>
-      </c>
-      <c r="G4" s="26">
+      <c r="E4" s="30">
+        <v>1</v>
+      </c>
+      <c r="F4" s="30">
+        <v>1</v>
+      </c>
+      <c r="G4" s="25">
         <v>1</v>
       </c>
     </row>
@@ -1083,19 +1074,19 @@
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="33">
-        <v>1</v>
-      </c>
-      <c r="F5" s="33">
-        <v>1</v>
-      </c>
-      <c r="G5" s="27">
+      <c r="E5" s="31">
+        <v>1</v>
+      </c>
+      <c r="F5" s="31">
+        <v>1</v>
+      </c>
+      <c r="G5" s="26">
         <v>1</v>
       </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="36">
         <v>200</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1105,13 +1096,13 @@
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="33">
-        <v>1</v>
-      </c>
-      <c r="F6" s="33">
-        <v>1</v>
-      </c>
-      <c r="G6" s="27">
+      <c r="E6" s="31">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31">
+        <v>1</v>
+      </c>
+      <c r="G6" s="26">
         <v>1</v>
       </c>
       <c r="H6" s="2"/>
@@ -1124,13 +1115,13 @@
       <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="33">
-        <v>1</v>
-      </c>
-      <c r="F7" s="33">
-        <v>1</v>
-      </c>
-      <c r="G7" s="27">
+      <c r="E7" s="31">
+        <v>1</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1</v>
+      </c>
+      <c r="G7" s="26">
         <v>1</v>
       </c>
       <c r="H7" s="2"/>
@@ -1145,13 +1136,13 @@
       <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="33">
-        <v>1</v>
-      </c>
-      <c r="F8" s="33">
-        <v>1</v>
-      </c>
-      <c r="G8" s="27">
+      <c r="E8" s="31">
+        <v>1</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="26">
         <v>1</v>
       </c>
       <c r="H8" s="5"/>
@@ -1166,13 +1157,13 @@
       <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="33">
-        <v>1</v>
-      </c>
-      <c r="F9" s="33">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27">
+      <c r="E9" s="31">
+        <v>1</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="26">
         <v>1</v>
       </c>
       <c r="H9" s="5"/>
@@ -1185,13 +1176,13 @@
         <v>62</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="33">
-        <v>1</v>
-      </c>
-      <c r="F10" s="33">
-        <v>1</v>
-      </c>
-      <c r="G10" s="27">
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" s="31">
+        <v>1</v>
+      </c>
+      <c r="G10" s="26">
         <v>1</v>
       </c>
       <c r="H10" s="2"/>
@@ -1206,13 +1197,13 @@
       <c r="D11" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="33">
-        <v>1</v>
-      </c>
-      <c r="F11" s="33">
-        <v>1</v>
-      </c>
-      <c r="G11" s="27">
+      <c r="E11" s="31">
+        <v>1</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1</v>
+      </c>
+      <c r="G11" s="26">
         <v>1</v>
       </c>
       <c r="H11" s="22" t="s">
@@ -1220,7 +1211,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="36">
         <v>300</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1230,13 +1221,13 @@
       <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="33">
-        <v>1</v>
-      </c>
-      <c r="F12" s="33">
-        <v>1</v>
-      </c>
-      <c r="G12" s="27">
+      <c r="E12" s="31">
+        <v>1</v>
+      </c>
+      <c r="F12" s="31">
+        <v>1</v>
+      </c>
+      <c r="G12" s="26">
         <v>1</v>
       </c>
       <c r="H12" s="2"/>
@@ -1249,13 +1240,13 @@
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="33">
-        <v>1</v>
-      </c>
-      <c r="F13" s="33">
-        <v>1</v>
-      </c>
-      <c r="G13" s="27">
+      <c r="E13" s="31">
+        <v>1</v>
+      </c>
+      <c r="F13" s="31">
+        <v>1</v>
+      </c>
+      <c r="G13" s="26">
         <v>1</v>
       </c>
       <c r="H13" s="2"/>
@@ -1268,13 +1259,13 @@
       <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="33">
-        <v>1</v>
-      </c>
-      <c r="F14" s="33">
-        <v>1</v>
-      </c>
-      <c r="G14" s="27">
+      <c r="E14" s="31">
+        <v>1</v>
+      </c>
+      <c r="F14" s="31">
+        <v>1</v>
+      </c>
+      <c r="G14" s="26">
         <v>1</v>
       </c>
       <c r="H14" s="2"/>
@@ -1287,13 +1278,13 @@
       <c r="D15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="33">
-        <v>1</v>
-      </c>
-      <c r="F15" s="33">
-        <v>1</v>
-      </c>
-      <c r="G15" s="27">
+      <c r="E15" s="31">
+        <v>1</v>
+      </c>
+      <c r="F15" s="31">
+        <v>1</v>
+      </c>
+      <c r="G15" s="26">
         <v>1</v>
       </c>
       <c r="H15" s="2"/>
@@ -1306,13 +1297,13 @@
       <c r="D16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="33">
-        <v>1</v>
-      </c>
-      <c r="F16" s="33">
-        <v>1</v>
-      </c>
-      <c r="G16" s="27">
+      <c r="E16" s="31">
+        <v>1</v>
+      </c>
+      <c r="F16" s="31">
+        <v>1</v>
+      </c>
+      <c r="G16" s="26">
         <v>1</v>
       </c>
       <c r="H16" s="2"/>
@@ -1325,13 +1316,13 @@
       <c r="D17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="33">
-        <v>1</v>
-      </c>
-      <c r="F17" s="33">
-        <v>1</v>
-      </c>
-      <c r="G17" s="28">
+      <c r="E17" s="31">
+        <v>1</v>
+      </c>
+      <c r="F17" s="31">
+        <v>1</v>
+      </c>
+      <c r="G17" s="27">
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -1339,7 +1330,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="36">
         <v>400</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1349,13 +1340,13 @@
       <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="34">
-        <v>1</v>
-      </c>
-      <c r="F18" s="33">
-        <v>1</v>
-      </c>
-      <c r="G18" s="33">
+      <c r="E18" s="32">
+        <v>1</v>
+      </c>
+      <c r="F18" s="31">
+        <v>1</v>
+      </c>
+      <c r="G18" s="31">
         <v>1</v>
       </c>
       <c r="H18" s="2"/>
@@ -1368,13 +1359,13 @@
         <v>73</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="33">
-        <v>1</v>
-      </c>
-      <c r="F19" s="33">
-        <v>1</v>
-      </c>
-      <c r="G19" s="33">
+      <c r="E19" s="31">
+        <v>1</v>
+      </c>
+      <c r="F19" s="31">
+        <v>1</v>
+      </c>
+      <c r="G19" s="31">
         <v>1</v>
       </c>
       <c r="H19" s="2"/>
@@ -1390,13 +1381,13 @@
       <c r="D20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="34">
-        <v>1</v>
-      </c>
-      <c r="F20" s="33">
-        <v>1</v>
-      </c>
-      <c r="G20" s="33">
+      <c r="E20" s="32">
+        <v>1</v>
+      </c>
+      <c r="F20" s="31">
+        <v>1</v>
+      </c>
+      <c r="G20" s="31">
         <v>1</v>
       </c>
       <c r="H20" s="2"/>
@@ -1409,20 +1400,20 @@
         <v>74</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="33">
-        <v>1</v>
-      </c>
-      <c r="F21" s="33">
-        <v>1</v>
-      </c>
-      <c r="G21" s="33">
+      <c r="E21" s="31">
+        <v>1</v>
+      </c>
+      <c r="F21" s="31">
+        <v>1</v>
+      </c>
+      <c r="G21" s="31">
         <v>1</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="36">
         <v>500</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1432,13 +1423,13 @@
         <v>77</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="33">
-        <v>1</v>
-      </c>
-      <c r="F22" s="33">
-        <v>1</v>
-      </c>
-      <c r="G22" s="33">
+      <c r="E22" s="31">
+        <v>1</v>
+      </c>
+      <c r="F22" s="31">
+        <v>1</v>
+      </c>
+      <c r="G22" s="31">
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -1456,13 +1447,13 @@
       <c r="D23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="34">
-        <v>1</v>
-      </c>
-      <c r="F23" s="33">
-        <v>1</v>
-      </c>
-      <c r="G23" s="33">
+      <c r="E23" s="32">
+        <v>1</v>
+      </c>
+      <c r="F23" s="31">
+        <v>1</v>
+      </c>
+      <c r="G23" s="31">
         <v>1</v>
       </c>
       <c r="H23" s="2"/>
@@ -1478,13 +1469,13 @@
       <c r="D24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="34">
-        <v>1</v>
-      </c>
-      <c r="F24" s="33">
-        <v>1</v>
-      </c>
-      <c r="G24" s="33">
+      <c r="E24" s="32">
+        <v>1</v>
+      </c>
+      <c r="F24" s="31">
+        <v>1</v>
+      </c>
+      <c r="G24" s="31">
         <v>1</v>
       </c>
       <c r="H24" s="2"/>
@@ -1500,20 +1491,20 @@
       <c r="D25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="34">
-        <v>1</v>
-      </c>
-      <c r="F25" s="33">
-        <v>1</v>
-      </c>
-      <c r="G25" s="33">
+      <c r="E25" s="32">
+        <v>1</v>
+      </c>
+      <c r="F25" s="31">
+        <v>1</v>
+      </c>
+      <c r="G25" s="31">
         <v>1</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="39">
+      <c r="A26" s="36">
         <v>600</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1525,13 +1516,13 @@
       <c r="D26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="33">
-        <v>1</v>
-      </c>
-      <c r="F26" s="33">
-        <v>1</v>
-      </c>
-      <c r="G26" s="33">
+      <c r="E26" s="31">
+        <v>1</v>
+      </c>
+      <c r="F26" s="31">
+        <v>1</v>
+      </c>
+      <c r="G26" s="31">
         <v>1</v>
       </c>
       <c r="H26" s="2"/>
@@ -1544,13 +1535,13 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="33">
-        <v>1</v>
-      </c>
-      <c r="F27" s="33">
-        <v>1</v>
-      </c>
-      <c r="G27" s="33">
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+      <c r="F27" s="31">
+        <v>1</v>
+      </c>
+      <c r="G27" s="31">
         <v>1</v>
       </c>
       <c r="H27" s="20"/>
@@ -1566,20 +1557,20 @@
       <c r="D28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="33">
-        <v>1</v>
-      </c>
-      <c r="F28" s="33">
-        <v>1</v>
-      </c>
-      <c r="G28" s="27">
+      <c r="E28" s="31">
+        <v>1</v>
+      </c>
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+      <c r="G28" s="26">
         <v>1</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="3" t="s">
         <v>34</v>
       </c>
@@ -1589,13 +1580,13 @@
       <c r="D29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="33">
-        <v>1</v>
-      </c>
-      <c r="F29" s="33">
-        <v>1</v>
-      </c>
-      <c r="G29" s="27">
+      <c r="E29" s="31">
+        <v>1</v>
+      </c>
+      <c r="F29" s="31">
+        <v>1</v>
+      </c>
+      <c r="G29" s="26">
         <v>1</v>
       </c>
       <c r="H29" s="2"/>
@@ -1608,15 +1599,15 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="36">
-        <v>0</v>
-      </c>
-      <c r="F30" s="36">
-        <v>0</v>
-      </c>
-      <c r="G30" s="30">
+        <v>108</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="28">
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -1624,27 +1615,25 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="33">
-        <v>1</v>
-      </c>
-      <c r="F31" s="33">
-        <v>1</v>
-      </c>
-      <c r="G31" s="28">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2" t="s">
+      <c r="D31" s="6" t="s">
         <v>107</v>
       </c>
+      <c r="E31" s="31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="26">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
@@ -1656,13 +1645,13 @@
       <c r="D32" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="33">
-        <v>1</v>
-      </c>
-      <c r="F32" s="33">
-        <v>1</v>
-      </c>
-      <c r="G32" s="27">
+      <c r="E32" s="31">
+        <v>1</v>
+      </c>
+      <c r="F32" s="31">
+        <v>1</v>
+      </c>
+      <c r="G32" s="26">
         <v>1</v>
       </c>
       <c r="H32" s="2"/>
@@ -1677,13 +1666,13 @@
       <c r="D33" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="33">
-        <v>1</v>
-      </c>
-      <c r="F33" s="33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="27">
+      <c r="E33" s="31">
+        <v>1</v>
+      </c>
+      <c r="F33" s="31">
+        <v>1</v>
+      </c>
+      <c r="G33" s="26">
         <v>1</v>
       </c>
       <c r="H33" s="2"/>
@@ -1698,13 +1687,13 @@
       <c r="D34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="33">
-        <v>1</v>
-      </c>
-      <c r="F34" s="33">
-        <v>1</v>
-      </c>
-      <c r="G34" s="27">
+      <c r="E34" s="31">
+        <v>1</v>
+      </c>
+      <c r="F34" s="31">
+        <v>1</v>
+      </c>
+      <c r="G34" s="26">
         <v>1</v>
       </c>
       <c r="H34" s="2"/>
@@ -1719,13 +1708,13 @@
       <c r="D35" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="33">
-        <v>1</v>
-      </c>
-      <c r="F35" s="33">
-        <v>1</v>
-      </c>
-      <c r="G35" s="27">
+      <c r="E35" s="31">
+        <v>1</v>
+      </c>
+      <c r="F35" s="31">
+        <v>1</v>
+      </c>
+      <c r="G35" s="26">
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -1742,29 +1731,29 @@
       <c r="D36" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="33">
-        <v>1</v>
-      </c>
-      <c r="F36" s="33">
-        <v>1</v>
-      </c>
-      <c r="G36" s="27">
+      <c r="E36" s="31">
+        <v>1</v>
+      </c>
+      <c r="F36" s="31">
+        <v>1</v>
+      </c>
+      <c r="G36" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="29"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="26"/>
       <c r="H37" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1777,13 +1766,13 @@
       <c r="D38" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E38" s="33">
-        <v>1</v>
-      </c>
-      <c r="F38" s="33">
-        <v>1</v>
-      </c>
-      <c r="G38" s="27">
+      <c r="E38" s="31">
+        <v>1</v>
+      </c>
+      <c r="F38" s="31">
+        <v>1</v>
+      </c>
+      <c r="G38" s="26">
         <v>1</v>
       </c>
       <c r="H38" s="2"/>
@@ -1798,19 +1787,19 @@
       <c r="D39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="33">
-        <v>1</v>
-      </c>
-      <c r="F39" s="33">
-        <v>1</v>
-      </c>
-      <c r="G39" s="27">
+      <c r="E39" s="31">
+        <v>1</v>
+      </c>
+      <c r="F39" s="31">
+        <v>1</v>
+      </c>
+      <c r="G39" s="26">
         <v>1</v>
       </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="48">
+      <c r="A40" s="45">
         <v>700</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -1822,13 +1811,13 @@
       <c r="D40" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="33">
-        <v>1</v>
-      </c>
-      <c r="F40" s="33">
-        <v>1</v>
-      </c>
-      <c r="G40" s="27">
+      <c r="E40" s="31">
+        <v>1</v>
+      </c>
+      <c r="F40" s="31">
+        <v>1</v>
+      </c>
+      <c r="G40" s="26">
         <v>1</v>
       </c>
       <c r="I40" s="8"/>
@@ -1843,33 +1832,33 @@
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="34">
-        <v>1</v>
-      </c>
-      <c r="F41" s="34">
-        <v>1</v>
-      </c>
-      <c r="G41" s="34">
+      <c r="E41" s="32">
+        <v>1</v>
+      </c>
+      <c r="F41" s="32">
+        <v>1</v>
+      </c>
+      <c r="G41" s="32">
         <v>1</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="8"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49" t="s">
+      <c r="B42" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="41">
-        <v>0</v>
-      </c>
-      <c r="F42" s="41">
-        <v>0</v>
-      </c>
-      <c r="G42" s="41">
+      <c r="E42" s="38">
+        <v>0</v>
+      </c>
+      <c r="F42" s="38">
+        <v>0</v>
+      </c>
+      <c r="G42" s="38">
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
@@ -1883,13 +1872,13 @@
       <c r="D43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="37">
-        <v>0</v>
-      </c>
-      <c r="F43" s="37">
-        <v>0</v>
-      </c>
-      <c r="G43" s="37">
+      <c r="E43" s="34">
+        <v>0</v>
+      </c>
+      <c r="F43" s="34">
+        <v>0</v>
+      </c>
+      <c r="G43" s="34">
         <v>0</v>
       </c>
       <c r="H43" s="2"/>
@@ -1905,19 +1894,19 @@
       <c r="D44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="37">
-        <v>0</v>
-      </c>
-      <c r="F44" s="37">
-        <v>0</v>
-      </c>
-      <c r="G44" s="37">
+      <c r="E44" s="34">
+        <v>0</v>
+      </c>
+      <c r="F44" s="34">
+        <v>0</v>
+      </c>
+      <c r="G44" s="34">
         <v>0</v>
       </c>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="39">
+      <c r="A45" s="36">
         <v>800</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -1927,42 +1916,40 @@
       <c r="D45" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="33">
-        <v>1</v>
-      </c>
-      <c r="F45" s="33">
-        <v>1</v>
-      </c>
-      <c r="G45" s="27">
+      <c r="E45" s="31">
+        <v>1</v>
+      </c>
+      <c r="F45" s="31">
+        <v>1</v>
+      </c>
+      <c r="G45" s="26">
         <v>1</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="8"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="33">
-        <v>1</v>
-      </c>
-      <c r="F46" s="33">
-        <v>1</v>
-      </c>
-      <c r="G46" s="28">
-        <v>0.99</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="31">
+        <v>1</v>
+      </c>
+      <c r="F46" s="31">
+        <v>1</v>
+      </c>
+      <c r="G46" s="26">
+        <v>1</v>
+      </c>
+      <c r="H46" s="2"/>
       <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="39">
+      <c r="A47" s="36">
         <v>900</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -1970,13 +1957,13 @@
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="33">
-        <v>1</v>
-      </c>
-      <c r="F47" s="33">
-        <v>1</v>
-      </c>
-      <c r="G47" s="27">
+      <c r="E47" s="31">
+        <v>1</v>
+      </c>
+      <c r="F47" s="31">
+        <v>1</v>
+      </c>
+      <c r="G47" s="26">
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
@@ -1995,13 +1982,13 @@
         <v>61</v>
       </c>
       <c r="D48" s="21"/>
-      <c r="E48" s="36">
-        <v>0</v>
-      </c>
-      <c r="F48" s="36">
-        <v>0</v>
-      </c>
-      <c r="G48" s="36">
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
+      <c r="G48" s="33">
         <v>0</v>
       </c>
       <c r="H48" s="2" t="s">
@@ -2019,20 +2006,20 @@
       <c r="D49" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E49" s="33">
-        <v>1</v>
-      </c>
-      <c r="F49" s="33">
-        <v>1</v>
-      </c>
-      <c r="G49" s="33">
+      <c r="E49" s="31">
+        <v>1</v>
+      </c>
+      <c r="F49" s="31">
+        <v>1</v>
+      </c>
+      <c r="G49" s="31">
         <v>1</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="50">
+      <c r="A50" s="47">
         <v>906</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -2044,13 +2031,13 @@
       <c r="D50" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E50" s="33">
-        <v>1</v>
-      </c>
-      <c r="F50" s="33">
-        <v>1</v>
-      </c>
-      <c r="G50" s="33">
+      <c r="E50" s="31">
+        <v>1</v>
+      </c>
+      <c r="F50" s="31">
+        <v>1</v>
+      </c>
+      <c r="G50" s="31">
         <v>1</v>
       </c>
       <c r="H50" s="2"/>
@@ -2066,13 +2053,13 @@
       <c r="D51" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="36">
-        <v>1</v>
-      </c>
-      <c r="F51" s="36">
-        <v>1</v>
-      </c>
-      <c r="G51" s="36">
+      <c r="E51" s="33">
+        <v>1</v>
+      </c>
+      <c r="F51" s="33">
+        <v>1</v>
+      </c>
+      <c r="G51" s="33">
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
@@ -2090,14 +2077,14 @@
       <c r="D52" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="38">
-        <v>0</v>
-      </c>
-      <c r="F52" s="38">
-        <v>0</v>
-      </c>
-      <c r="G52" s="38">
-        <v>0</v>
+      <c r="E52" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="G52" s="35">
+        <v>0.5</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>110</v>
@@ -2111,34 +2098,34 @@
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
       <c r="H53" s="11"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="23" t="s">
         <v>100</v>
       </c>
       <c r="C54" s="9"/>
-      <c r="D54" s="25">
+      <c r="D54" s="24">
         <f>SUM(E54:G54)/3</f>
-        <v>0.94613636363636366</v>
-      </c>
-      <c r="E54" s="44">
-        <f>SUM(E4:E53)/44</f>
-        <v>0.95454545454545459</v>
-      </c>
-      <c r="F54" s="44">
-        <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/44</f>
-        <v>0.95454545454545459</v>
-      </c>
-      <c r="G54" s="44">
+        <v>0.9875968992248062</v>
+      </c>
+      <c r="E54" s="41">
+        <f>SUM(E4:E53)/43</f>
+        <v>0.98837209302325579</v>
+      </c>
+      <c r="F54" s="41">
+        <f t="shared" ref="F54:G54" si="0">SUM(F4:F53)/43</f>
+        <v>0.98837209302325579</v>
+      </c>
+      <c r="G54" s="41">
         <f t="shared" si="0"/>
-        <v>0.92931818181818182</v>
+        <v>0.98604651162790691</v>
       </c>
       <c r="H54" s="20"/>
     </row>
@@ -2147,13 +2134,13 @@
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
-      <c r="E55" s="31" t="s">
+      <c r="E55" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="G55" s="31" t="s">
+      <c r="G55" s="29" t="s">
         <v>98</v>
       </c>
       <c r="H55" s="20"/>
@@ -2163,9 +2150,9 @@
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
       <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2178,13 +2165,13 @@
       <c r="D57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="41">
-        <v>0</v>
-      </c>
-      <c r="F57" s="41">
-        <v>0</v>
-      </c>
-      <c r="G57" s="41">
+      <c r="E57" s="38">
+        <v>0</v>
+      </c>
+      <c r="F57" s="38">
+        <v>0</v>
+      </c>
+      <c r="G57" s="38">
         <v>0</v>
       </c>
       <c r="H57" s="2"/>
@@ -2199,13 +2186,13 @@
       <c r="D58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="41">
-        <v>0</v>
-      </c>
-      <c r="F58" s="41">
-        <v>0</v>
-      </c>
-      <c r="G58" s="41">
+      <c r="E58" s="38">
+        <v>0</v>
+      </c>
+      <c r="F58" s="38">
+        <v>0</v>
+      </c>
+      <c r="G58" s="38">
         <v>0</v>
       </c>
       <c r="H58" s="2"/>
@@ -2220,13 +2207,13 @@
       <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E59" s="41">
-        <v>0</v>
-      </c>
-      <c r="F59" s="41">
-        <v>0</v>
-      </c>
-      <c r="G59" s="41">
+      <c r="E59" s="38">
+        <v>0</v>
+      </c>
+      <c r="F59" s="38">
+        <v>0</v>
+      </c>
+      <c r="G59" s="38">
         <v>0</v>
       </c>
       <c r="H59" s="2"/>
@@ -2241,13 +2228,13 @@
       <c r="D60" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E60" s="41">
-        <v>0</v>
-      </c>
-      <c r="F60" s="41">
-        <v>0</v>
-      </c>
-      <c r="G60" s="41">
+      <c r="E60" s="38">
+        <v>0</v>
+      </c>
+      <c r="F60" s="38">
+        <v>0</v>
+      </c>
+      <c r="G60" s="38">
         <v>0</v>
       </c>
       <c r="H60" s="2"/>
@@ -2260,13 +2247,13 @@
         <v>50</v>
       </c>
       <c r="D61" s="1"/>
-      <c r="E61" s="41">
-        <v>0</v>
-      </c>
-      <c r="F61" s="41">
-        <v>0</v>
-      </c>
-      <c r="G61" s="41">
+      <c r="E61" s="38">
+        <v>0</v>
+      </c>
+      <c r="F61" s="38">
+        <v>0</v>
+      </c>
+      <c r="G61" s="38">
         <v>0</v>
       </c>
       <c r="H61" s="2"/>
@@ -2282,13 +2269,13 @@
       <c r="D62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E62" s="41">
-        <v>0</v>
-      </c>
-      <c r="F62" s="41">
-        <v>0</v>
-      </c>
-      <c r="G62" s="41">
+      <c r="E62" s="38">
+        <v>0</v>
+      </c>
+      <c r="F62" s="38">
+        <v>0</v>
+      </c>
+      <c r="G62" s="38">
         <v>0</v>
       </c>
       <c r="H62" s="2"/>
@@ -2300,13 +2287,13 @@
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
-      <c r="E63" s="41">
-        <v>0</v>
-      </c>
-      <c r="F63" s="41">
-        <v>0</v>
-      </c>
-      <c r="G63" s="41">
+      <c r="E63" s="38">
+        <v>0</v>
+      </c>
+      <c r="F63" s="38">
+        <v>0</v>
+      </c>
+      <c r="G63" s="38">
         <v>0</v>
       </c>
       <c r="H63" s="11"/>
@@ -2318,13 +2305,13 @@
       <c r="B64" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="41">
-        <v>0</v>
-      </c>
-      <c r="F64" s="41">
-        <v>0</v>
-      </c>
-      <c r="G64" s="41">
+      <c r="E64" s="38">
+        <v>0</v>
+      </c>
+      <c r="F64" s="38">
+        <v>0</v>
+      </c>
+      <c r="G64" s="38">
         <v>0</v>
       </c>
       <c r="H64" s="2"/>
@@ -2339,13 +2326,13 @@
       <c r="C65" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E65" s="41">
-        <v>0</v>
-      </c>
-      <c r="F65" s="41">
-        <v>0</v>
-      </c>
-      <c r="G65" s="41">
+      <c r="E65" s="38">
+        <v>0</v>
+      </c>
+      <c r="F65" s="38">
+        <v>0</v>
+      </c>
+      <c r="G65" s="38">
         <v>0</v>
       </c>
       <c r="H65" s="2"/>
@@ -2360,13 +2347,13 @@
       <c r="C66" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="41">
-        <v>0</v>
-      </c>
-      <c r="F66" s="41">
-        <v>0</v>
-      </c>
-      <c r="G66" s="41">
+      <c r="E66" s="38">
+        <v>0</v>
+      </c>
+      <c r="F66" s="38">
+        <v>0</v>
+      </c>
+      <c r="G66" s="38">
         <v>0</v>
       </c>
       <c r="H66" s="2"/>
@@ -2381,13 +2368,13 @@
       <c r="C67" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="41">
-        <v>0</v>
-      </c>
-      <c r="F67" s="41">
-        <v>0</v>
-      </c>
-      <c r="G67" s="41">
+      <c r="E67" s="38">
+        <v>0</v>
+      </c>
+      <c r="F67" s="38">
+        <v>0</v>
+      </c>
+      <c r="G67" s="38">
         <v>0</v>
       </c>
       <c r="H67" s="2"/>
@@ -2399,13 +2386,13 @@
       <c r="C68" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E68" s="41">
-        <v>0</v>
-      </c>
-      <c r="F68" s="41">
-        <v>0</v>
-      </c>
-      <c r="G68" s="41">
+      <c r="E68" s="38">
+        <v>0</v>
+      </c>
+      <c r="F68" s="38">
+        <v>0</v>
+      </c>
+      <c r="G68" s="38">
         <v>0</v>
       </c>
       <c r="H68" s="2"/>
@@ -2418,13 +2405,13 @@
         <v>3</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="E69" s="41">
-        <v>0</v>
-      </c>
-      <c r="F69" s="41">
-        <v>0</v>
-      </c>
-      <c r="G69" s="41">
+      <c r="E69" s="38">
+        <v>0</v>
+      </c>
+      <c r="F69" s="38">
+        <v>0</v>
+      </c>
+      <c r="G69" s="38">
         <v>0</v>
       </c>
       <c r="H69" s="2"/>
@@ -2434,13 +2421,13 @@
         <v>51</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="E70" s="41">
-        <v>0</v>
-      </c>
-      <c r="F70" s="41">
-        <v>0</v>
-      </c>
-      <c r="G70" s="41">
+      <c r="E70" s="38">
+        <v>0</v>
+      </c>
+      <c r="F70" s="38">
+        <v>0</v>
+      </c>
+      <c r="G70" s="38">
         <v>0</v>
       </c>
       <c r="H70" s="2"/>
@@ -2453,13 +2440,13 @@
         <v>52</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="E71" s="41">
-        <v>0</v>
-      </c>
-      <c r="F71" s="41">
-        <v>0</v>
-      </c>
-      <c r="G71" s="41">
+      <c r="E71" s="38">
+        <v>0</v>
+      </c>
+      <c r="F71" s="38">
+        <v>0</v>
+      </c>
+      <c r="G71" s="38">
         <v>0</v>
       </c>
       <c r="H71" s="2"/>
@@ -2472,13 +2459,13 @@
         <v>53</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="E72" s="41">
-        <v>0</v>
-      </c>
-      <c r="F72" s="41">
-        <v>0</v>
-      </c>
-      <c r="G72" s="41">
+      <c r="E72" s="38">
+        <v>0</v>
+      </c>
+      <c r="F72" s="38">
+        <v>0</v>
+      </c>
+      <c r="G72" s="38">
         <v>0</v>
       </c>
       <c r="H72" s="2"/>
@@ -2490,13 +2477,13 @@
       <c r="B73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E73" s="42">
-        <v>0</v>
-      </c>
-      <c r="F73" s="42">
-        <v>0</v>
-      </c>
-      <c r="G73" s="42">
+      <c r="E73" s="39">
+        <v>0</v>
+      </c>
+      <c r="F73" s="39">
+        <v>0</v>
+      </c>
+      <c r="G73" s="39">
         <v>0</v>
       </c>
     </row>
@@ -2508,21 +2495,21 @@
       <c r="B75" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D75" s="25">
+      <c r="D75" s="24">
         <f>SUM(E75:G75)/3</f>
-        <v>0.59471428571428575</v>
-      </c>
-      <c r="E75" s="44">
+        <v>0.60666666666666658</v>
+      </c>
+      <c r="E75" s="41">
         <f>(SUM(E4:E73) - E54)/70</f>
-        <v>0.6</v>
-      </c>
-      <c r="F75" s="45">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="F75" s="42">
         <f>(SUM(F4:F73) - F54)/70</f>
-        <v>0.6</v>
-      </c>
-      <c r="G75" s="46">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="G75" s="43">
         <f>(SUM(G4:G73) - G54)/70</f>
-        <v>0.58414285714285719</v>
+        <v>0.60571428571428565</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Build Release Candidate 2] [Update] Derniers bugs, à tester
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -359,14 +359,46 @@
     </r>
   </si>
   <si>
-    <t>Corriger le problème des banners qui ne s'affichent pas, Les hands ne se comptent pas correctement, cubeBase qui va trop vite/trop lentement (n'attend pas la caméra)</t>
+    <r>
+      <t xml:space="preserve">Corriger le problème des banners qui ne s'affichent pas, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Les hands ne se comptent pas correctement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cubeBase qui va trop vite/trop lentement (n'attend pas la caméra)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +448,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -999,7 +1038,7 @@
   <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[Build 1001] [Update] Correction de quelques bugs légers
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>Stepchart</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Mode aventure</t>
   </si>
   <si>
-    <t>Pack Cublast Originals</t>
-  </si>
-  <si>
     <t>Mode 8t</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>Entrée dans le jeu et trans</t>
   </si>
   <si>
-    <t>Améliorable l'effet</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
   </si>
   <si>
     <t>Trouver un doubleur</t>
-  </si>
-  <si>
-    <t>Particle  de fond améliorable</t>
   </si>
   <si>
     <t>WheelSong / Stepchart</t>
@@ -357,6 +348,9 @@
       </rPr>
       <t/>
     </r>
+  </si>
+  <si>
+    <t>Troisième phase de test</t>
   </si>
 </sst>
 </file>
@@ -995,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,19 +1024,19 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1051,7 +1045,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="30">
         <v>1</v>
@@ -1149,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>23</v>
@@ -1170,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="31">
@@ -1192,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="31">
         <v>1</v>
@@ -1203,9 +1197,7 @@
       <c r="G11" s="26">
         <v>1</v>
       </c>
-      <c r="H11" s="22" t="s">
-        <v>87</v>
-      </c>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
@@ -1311,7 +1303,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="31">
         <v>1</v>
@@ -1323,7 +1315,7 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1353,7 +1345,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="31">
@@ -1373,10 +1365,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="32">
         <v>1</v>
@@ -1394,7 +1386,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="31">
@@ -1417,7 +1409,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="31">
@@ -1429,9 +1421,7 @@
       <c r="G22" s="31">
         <v>1</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="H22" s="2"/>
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1528,7 +1518,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1552,7 +1542,7 @@
         <v>29</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E28" s="31">
         <v>1</v>
@@ -1596,7 +1586,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E30" s="33">
         <v>0</v>
@@ -1608,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1619,7 +1609,7 @@
         <v>29</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E31" s="31">
         <v>1</v>
@@ -1661,7 +1651,7 @@
         <v>29</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E33" s="31">
         <v>1</v>
@@ -1703,7 +1693,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35" s="31">
         <v>1</v>
@@ -1715,18 +1705,18 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E36" s="31">
         <v>1</v>
@@ -1743,14 +1733,14 @@
         <v>41</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
       <c r="G37" s="26"/>
       <c r="H37" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1761,7 +1751,7 @@
         <v>23</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E38" s="31">
         <v>1</v>
@@ -1776,13 +1766,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E39" s="31">
         <v>1</v>
@@ -1847,7 +1837,7 @@
       </c>
       <c r="C42" s="46"/>
       <c r="D42" s="46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E42" s="38">
         <v>0</v>
@@ -1867,7 +1857,7 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E43" s="34">
         <v>0</v>
@@ -1886,10 +1876,10 @@
         <v>19</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E44" s="34">
         <v>0</v>
@@ -1930,7 +1920,7 @@
         <v>19</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="31">
@@ -1950,7 +1940,7 @@
         <v>900</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1964,19 +1954,19 @@
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="33">
@@ -1989,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I48" s="8"/>
     </row>
@@ -1998,10 +1988,10 @@
         <v>0</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E49" s="31">
         <v>1</v>
@@ -2023,10 +2013,10 @@
         <v>0</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E50" s="31">
         <v>1</v>
@@ -2045,11 +2035,11 @@
         <v>0</v>
       </c>
       <c r="C51" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D51" s="21" t="s">
-        <v>94</v>
-      </c>
       <c r="E51" s="33">
         <v>1</v>
       </c>
@@ -2060,7 +2050,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I51" s="8"/>
     </row>
@@ -2072,7 +2062,7 @@
         <v>41</v>
       </c>
       <c r="D52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E52" s="35">
         <v>1</v>
@@ -2100,10 +2090,10 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="24">
@@ -2130,13 +2120,13 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2262,7 +2252,7 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E62" s="38">
         <v>0</v>
@@ -2278,7 +2268,7 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -2333,9 +2323,6 @@
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>5000</v>
-      </c>
       <c r="B66" s="1" t="s">
         <v>1</v>
       </c>
@@ -2354,9 +2341,6 @@
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>6000</v>
-      </c>
       <c r="B67" s="1" t="s">
         <v>1</v>
       </c>
@@ -2394,7 +2378,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>3</v>
@@ -2412,6 +2396,9 @@
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>6000</v>
+      </c>
       <c r="B70" s="1" t="s">
         <v>51</v>
       </c>
@@ -2428,13 +2415,14 @@
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C71" s="1"/>
+      <c r="A71" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C71" s="12"/>
+      <c r="D71" s="10"/>
       <c r="E71" s="38">
         <v>0</v>
       </c>
@@ -2448,10 +2436,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C72" s="1"/>
       <c r="E72" s="38">
@@ -2467,10 +2455,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>62</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E73" s="39">
         <v>0</v>
@@ -2485,10 +2473,10 @@
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D75" s="24">
         <f>SUM(E75:G75)/3</f>

</xml_diff>

<commit_message>
[Build 1011] [Update] Optimisation de la stepchart à tester
Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="112">
   <si>
     <t>Stepchart</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Build</t>
-  </si>
-  <si>
-    <t>Mode LAN</t>
   </si>
   <si>
     <t>LAN</t>
@@ -351,6 +348,21 @@
   </si>
   <si>
     <t>Troisième phase de test</t>
+  </si>
+  <si>
+    <t>Optimisation du code Stepchart</t>
+  </si>
+  <si>
+    <t>Creation Scene</t>
+  </si>
+  <si>
+    <t>Creation Network</t>
+  </si>
+  <si>
+    <t>Avant 2013</t>
+  </si>
+  <si>
+    <t>Création du système</t>
   </si>
 </sst>
 </file>
@@ -444,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -555,11 +567,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -626,6 +647,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,13 +673,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -987,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,19 +1051,19 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>94</v>
-      </c>
-      <c r="G3" t="s">
-        <v>95</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1045,7 +1072,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="30">
         <v>1</v>
@@ -1143,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>23</v>
@@ -1164,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="31">
@@ -1186,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="31">
         <v>1</v>
@@ -1303,7 +1330,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="31">
         <v>1</v>
@@ -1315,7 +1342,7 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1345,7 +1372,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="31">
@@ -1365,10 +1392,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="32">
         <v>1</v>
@@ -1386,7 +1413,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="31">
@@ -1409,7 +1436,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="31">
@@ -1518,7 +1545,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1542,7 +1569,7 @@
         <v>29</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28" s="31">
         <v>1</v>
@@ -1586,7 +1613,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E30" s="33">
         <v>0</v>
@@ -1598,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,7 +1636,7 @@
         <v>29</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="31">
         <v>1</v>
@@ -1651,7 +1678,7 @@
         <v>29</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="31">
         <v>1</v>
@@ -1693,7 +1720,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E35" s="31">
         <v>1</v>
@@ -1705,18 +1732,18 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" s="31">
         <v>1</v>
@@ -1733,14 +1760,14 @@
         <v>41</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
       <c r="G37" s="26"/>
       <c r="H37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1751,7 +1778,7 @@
         <v>23</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E38" s="31">
         <v>1</v>
@@ -1766,13 +1793,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E39" s="31">
         <v>1</v>
@@ -1837,7 +1864,7 @@
       </c>
       <c r="C42" s="46"/>
       <c r="D42" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E42" s="38">
         <v>0</v>
@@ -1857,7 +1884,7 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E43" s="34">
         <v>0</v>
@@ -1876,10 +1903,10 @@
         <v>19</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E44" s="34">
         <v>0</v>
@@ -1920,7 +1947,7 @@
         <v>19</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="31">
@@ -1940,7 +1967,7 @@
         <v>900</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1954,19 +1981,19 @@
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="33">
@@ -1979,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I48" s="8"/>
     </row>
@@ -1988,10 +2015,10 @@
         <v>0</v>
       </c>
       <c r="C49" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="E49" s="31">
         <v>1</v>
@@ -2013,10 +2040,10 @@
         <v>0</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E50" s="31">
         <v>1</v>
@@ -2035,10 +2062,10 @@
         <v>0</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E51" s="33">
         <v>1</v>
@@ -2050,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I51" s="8"/>
     </row>
@@ -2062,7 +2089,7 @@
         <v>41</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E52" s="35">
         <v>1</v>
@@ -2079,7 +2106,7 @@
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -2090,10 +2117,10 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="23" t="s">
         <v>96</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>97</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="24">
@@ -2120,13 +2147,13 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="F55" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="G55" s="29" t="s">
         <v>94</v>
-      </c>
-      <c r="G55" s="29" t="s">
-        <v>95</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2135,103 +2162,120 @@
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
       <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
+      <c r="A57" s="9">
+        <v>1100</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="40">
+        <v>0</v>
+      </c>
+      <c r="F57" s="40">
+        <v>0</v>
+      </c>
+      <c r="G57" s="40">
+        <v>0</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1200</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E58" s="38">
+        <v>0</v>
+      </c>
+      <c r="F58" s="38">
+        <v>0</v>
+      </c>
+      <c r="G58" s="38">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1300</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="38">
+        <v>0</v>
+      </c>
+      <c r="F59" s="38">
+        <v>0</v>
+      </c>
+      <c r="G59" s="38">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1400</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="38">
-        <v>0</v>
-      </c>
-      <c r="F57" s="38">
-        <v>0</v>
-      </c>
-      <c r="G57" s="38">
-        <v>0</v>
-      </c>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E58" s="38">
-        <v>0</v>
-      </c>
-      <c r="F58" s="38">
-        <v>0</v>
-      </c>
-      <c r="G58" s="38">
-        <v>0</v>
-      </c>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
+      <c r="E60" s="38">
+        <v>0</v>
+      </c>
+      <c r="F60" s="38">
+        <v>0</v>
+      </c>
+      <c r="G60" s="38">
+        <v>0</v>
+      </c>
+      <c r="H60" s="50">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1500</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="38">
-        <v>0</v>
-      </c>
-      <c r="F59" s="38">
-        <v>0</v>
-      </c>
-      <c r="G59" s="38">
-        <v>0</v>
-      </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60" s="38">
-        <v>0</v>
-      </c>
-      <c r="F60" s="38">
-        <v>0</v>
-      </c>
-      <c r="G60" s="38">
-        <v>0</v>
-      </c>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D61" s="1"/>
+      <c r="C61" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="51" t="s">
+        <v>29</v>
+      </c>
       <c r="E61" s="38">
         <v>0</v>
       </c>
@@ -2241,18 +2285,22 @@
       <c r="G61" s="38">
         <v>0</v>
       </c>
-      <c r="H61" s="2"/>
+      <c r="H61" s="50">
+        <v>41306</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2000</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1" t="s">
-        <v>70</v>
+        <v>1600</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E62" s="38">
         <v>0</v>
@@ -2263,15 +2311,20 @@
       <c r="G62" s="38">
         <v>0</v>
       </c>
-      <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-      <c r="B63" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
+      <c r="A63">
+        <v>1700</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E63" s="38">
         <v>0</v>
       </c>
@@ -2281,89 +2334,78 @@
       <c r="G63" s="38">
         <v>0</v>
       </c>
-      <c r="H63" s="11"/>
+      <c r="H63" s="50">
+        <v>41334</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
+        <v>2000</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E64" s="38">
+        <v>0</v>
+      </c>
+      <c r="F64" s="38">
+        <v>0</v>
+      </c>
+      <c r="G64" s="38">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="38">
+        <v>0</v>
+      </c>
+      <c r="F65" s="38">
+        <v>0</v>
+      </c>
+      <c r="G65" s="38">
+        <v>0</v>
+      </c>
+      <c r="H65" s="11"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="20"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="9"/>
+      <c r="B67" s="46"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="49"/>
+      <c r="F67" s="49"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="20"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>3000</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E64" s="38">
-        <v>0</v>
-      </c>
-      <c r="F64" s="38">
-        <v>0</v>
-      </c>
-      <c r="G64" s="38">
-        <v>0</v>
-      </c>
-      <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>4000</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E65" s="38">
-        <v>0</v>
-      </c>
-      <c r="F65" s="38">
-        <v>0</v>
-      </c>
-      <c r="G65" s="38">
-        <v>0</v>
-      </c>
-      <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E66" s="38">
-        <v>0</v>
-      </c>
-      <c r="F66" s="38">
-        <v>0</v>
-      </c>
-      <c r="G66" s="38">
-        <v>0</v>
-      </c>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E67" s="38">
-        <v>0</v>
-      </c>
-      <c r="F67" s="38">
-        <v>0</v>
-      </c>
-      <c r="G67" s="38">
-        <v>0</v>
-      </c>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E68" s="38">
         <v>0</v>
@@ -2378,156 +2420,219 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
+        <v>4000</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E69" s="38">
+        <v>0</v>
+      </c>
+      <c r="F69" s="38">
+        <v>0</v>
+      </c>
+      <c r="G69" s="38">
+        <v>0</v>
+      </c>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="38">
+        <v>0</v>
+      </c>
+      <c r="F70" s="38">
+        <v>0</v>
+      </c>
+      <c r="G70" s="38">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E71" s="38">
+        <v>0</v>
+      </c>
+      <c r="F71" s="38">
+        <v>0</v>
+      </c>
+      <c r="G71" s="38">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" s="38">
+        <v>0</v>
+      </c>
+      <c r="F72" s="38">
+        <v>0</v>
+      </c>
+      <c r="G72" s="38">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>5000</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="E69" s="38">
-        <v>0</v>
-      </c>
-      <c r="F69" s="38">
-        <v>0</v>
-      </c>
-      <c r="G69" s="38">
-        <v>0</v>
-      </c>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="C73" s="1"/>
+      <c r="E73" s="38">
+        <v>0</v>
+      </c>
+      <c r="F73" s="38">
+        <v>0</v>
+      </c>
+      <c r="G73" s="38">
+        <v>0</v>
+      </c>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>6000</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="E74" s="38">
+        <v>0</v>
+      </c>
+      <c r="F74" s="38">
+        <v>0</v>
+      </c>
+      <c r="G74" s="38">
+        <v>0</v>
+      </c>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="38">
+        <v>0</v>
+      </c>
+      <c r="F75" s="38">
+        <v>0</v>
+      </c>
+      <c r="G75" s="38">
+        <v>0</v>
+      </c>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C70" s="1"/>
-      <c r="E70" s="38">
-        <v>0</v>
-      </c>
-      <c r="F70" s="38">
-        <v>0</v>
-      </c>
-      <c r="G70" s="38">
-        <v>0</v>
-      </c>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="38">
-        <v>0</v>
-      </c>
-      <c r="F71" s="38">
-        <v>0</v>
-      </c>
-      <c r="G71" s="38">
-        <v>0</v>
-      </c>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="E72" s="38">
-        <v>0</v>
-      </c>
-      <c r="F72" s="38">
-        <v>0</v>
-      </c>
-      <c r="G72" s="38">
-        <v>0</v>
-      </c>
-      <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="C76" s="1"/>
+      <c r="E76" s="38">
+        <v>0</v>
+      </c>
+      <c r="F76" s="38">
+        <v>0</v>
+      </c>
+      <c r="G76" s="38">
+        <v>0</v>
+      </c>
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E73" s="39">
-        <v>0</v>
-      </c>
-      <c r="F73" s="39">
-        <v>0</v>
-      </c>
-      <c r="G73" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>96</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D75" s="24">
-        <f>SUM(E75:G75)/3</f>
+      <c r="E77" s="39">
+        <v>0</v>
+      </c>
+      <c r="F77" s="39">
+        <v>0</v>
+      </c>
+      <c r="G77" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D79" s="24">
+        <f>SUM(E79:G79)/3</f>
         <v>0.61380952380952392</v>
       </c>
-      <c r="E75" s="41">
-        <f>(SUM(E4:E73) - E54)/70</f>
+      <c r="E79" s="41">
+        <f>(SUM(E4:E77) - E54)/70</f>
         <v>0.61428571428571432</v>
       </c>
-      <c r="F75" s="42">
-        <f>(SUM(F4:F73) - F54)/70</f>
+      <c r="F79" s="42">
+        <f>(SUM(F4:F77) - F54)/70</f>
         <v>0.61428571428571432</v>
       </c>
-      <c r="G75" s="43">
-        <f>(SUM(G4:G73) - G54)/70</f>
+      <c r="G79" s="43">
+        <f>(SUM(G4:G77) - G54)/70</f>
         <v>0.61285714285714288</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="15"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="15"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="17"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="2"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="17"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="2"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="16"/>
-    </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-      <c r="D83" s="18"/>
+      <c r="B83" s="15"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="15"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="17"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="15"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="17"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="15"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="16"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="15"/>
+      <c r="B87" s="2"/>
+      <c r="D87" s="18"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="15"/>
@@ -2633,6 +2738,18 @@
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="15"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="15"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="15"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="15"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E54:G54">
@@ -2711,7 +2828,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75:G75">
+  <conditionalFormatting sqref="E79:G79">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2773,7 +2890,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
+  <conditionalFormatting sqref="D79">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2932,7 +3049,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E75:G75</xm:sqref>
+          <xm:sqref>E79:G79</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0902D927-E259-4C22-AC26-A2682B1E694E}">
@@ -2947,7 +3064,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D75</xm:sqref>
+          <xm:sqref>D79</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
[Build 1431] [Update] [Non compilé]
Network en jeu fait, reste l'affichage

Signed-off-by: BenouKat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="270" windowWidth="12915" windowHeight="6150"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -604,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -690,6 +690,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,22 +2461,22 @@
       <c r="H68" s="44"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="22" t="s">
+      <c r="B69" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="46" t="s">
+      <c r="D69" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="E69" s="33">
-        <v>0</v>
-      </c>
-      <c r="F69" s="33">
-        <v>0</v>
-      </c>
-      <c r="G69" s="33">
+      <c r="E69" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="F69" s="59">
+        <v>0</v>
+      </c>
+      <c r="G69" s="59">
         <v>0</v>
       </c>
       <c r="H69" s="44"/>
@@ -2751,11 +2760,11 @@
       <c r="C82" s="9"/>
       <c r="D82" s="24">
         <f>SUM(E82:G82)/3</f>
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="E82" s="38">
         <f>SUM(E54:E80)/24</f>
-        <v>0.75</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F82" s="38">
         <f t="shared" ref="F82:G82" si="0">SUM(F54:F80)/24</f>

</xml_diff>